<commit_message>
Updated - Defect Log
</commit_message>
<xml_diff>
--- a/Testing/Revised Plan.xlsx
+++ b/Testing/Revised Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Revised Plan and Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="8_{783EC7BA-7F55-4B35-8C25-054FADF87783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF0A1A3E-969B-4CCB-8456-830795E63E07}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="8_{783EC7BA-7F55-4B35-8C25-054FADF87783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF4E83F1-5E53-4DBD-A44D-C5C0697DF6D6}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="7" xr2:uid="{FF53E854-575C-4B97-B6D0-9B270F57EAA4}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="798">
   <si>
     <t>WEEK 0</t>
   </si>
@@ -2813,21 +2813,12 @@
     <t>Create Invite</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeated characters is accepted in Employee Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeated Characters is accepted </t>
-  </si>
-  <si>
     <t>ACE number is limited to 4 characters. Should be increased</t>
   </si>
   <si>
     <t>Role is not filtered based on department</t>
   </si>
   <si>
-    <t xml:space="preserve">Error message in Email is not proper &amp; specific. </t>
-  </si>
-  <si>
     <t>FIlterdropdown</t>
   </si>
   <si>
@@ -2840,16 +2831,67 @@
     <t>Snack bar message is not correct(spelling mistakes &amp; punctuation)</t>
   </si>
   <si>
-    <t>Snack bar</t>
-  </si>
-  <si>
-    <t>Login button's hover colour is light</t>
-  </si>
-  <si>
     <t>Validation message should be changed. (Wait untill you receive a mail)</t>
   </si>
   <si>
     <t>Login Page is not responsive (Bg image and Title text alignment)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeated character is accepted in Employee Name </t>
+  </si>
+  <si>
+    <t>Login button's hover effect is light in colour</t>
+  </si>
+  <si>
+    <t>Repeated Character is accepted in Drive Name</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Error message in Email is not proper &amp; specific</t>
+  </si>
+  <si>
+    <t>Spelling mistake</t>
+  </si>
+  <si>
+    <t>Create account (Snack bar)</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>Add Project</t>
+  </si>
+  <si>
+    <t>Add Role</t>
+  </si>
+  <si>
+    <t>Card is misaligned</t>
+  </si>
+  <si>
+    <t>Repeated character is accepted as Department name (Ex: Javaaaaaa)</t>
+  </si>
+  <si>
+    <t>Repeated character is accepted as Location name (Ex: Kashmirrrrrrr)</t>
+  </si>
+  <si>
+    <t>Repeated character is accepted as Project name (Ex: rrrrrrrrrr)</t>
+  </si>
+  <si>
+    <t>Repeated character is accepted as Role name (Ex: rrrrrrrrrr)</t>
+  </si>
+  <si>
+    <t>Newly added role is not displayed at the top of the role list</t>
+  </si>
+  <si>
+    <t>Newly added project is not displayed at the top of the project list</t>
+  </si>
+  <si>
+    <t>Newly added location is not displayed at the top of the location list</t>
+  </si>
+  <si>
+    <t>Newly added department is not displayed at the top of the department list</t>
   </si>
 </sst>
 </file>
@@ -4174,7 +4216,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="351">
+  <cellXfs count="352">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4679,14 +4721,155 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4717,162 +4900,21 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4930,6 +4972,54 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4963,54 +5053,6 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5055,6 +5097,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6048,7 +6093,7 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="225" t="s">
+      <c r="D2" s="226" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -6063,7 +6108,7 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="226"/>
+      <c r="D3" s="225"/>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
@@ -6076,7 +6121,7 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="225" t="s">
+      <c r="D4" s="226" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -6091,7 +6136,7 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6106,7 +6151,7 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="225" t="s">
+      <c r="D6" s="226" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -6121,7 +6166,7 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="225"/>
+      <c r="D7" s="226"/>
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
@@ -6134,7 +6179,7 @@
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="225" t="s">
+      <c r="D8" s="226" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -6149,7 +6194,7 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="225"/>
+      <c r="D9" s="226"/>
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
@@ -6194,7 +6239,7 @@
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="226" t="s">
+      <c r="D12" s="225" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -6209,7 +6254,7 @@
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="226"/>
+      <c r="D13" s="225"/>
       <c r="E13" s="4" t="s">
         <v>3</v>
       </c>
@@ -6222,7 +6267,7 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="226"/>
+      <c r="D14" s="225"/>
       <c r="E14" s="4" t="s">
         <v>3</v>
       </c>
@@ -6235,7 +6280,7 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="226"/>
+      <c r="D15" s="225"/>
       <c r="E15" s="4" t="s">
         <v>3</v>
       </c>
@@ -6248,7 +6293,7 @@
       <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="226"/>
+      <c r="D16" s="225"/>
       <c r="E16" s="4" t="s">
         <v>3</v>
       </c>
@@ -6278,7 +6323,7 @@
       <c r="C18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="226" t="s">
+      <c r="D18" s="225" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -6293,7 +6338,7 @@
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="226"/>
+      <c r="D19" s="225"/>
       <c r="E19" s="4" t="s">
         <v>3</v>
       </c>
@@ -6306,7 +6351,7 @@
       <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="226"/>
+      <c r="D20" s="225"/>
       <c r="E20" s="4" t="s">
         <v>3</v>
       </c>
@@ -6321,7 +6366,7 @@
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="226" t="s">
+      <c r="D21" s="225" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -6336,7 +6381,7 @@
       <c r="C22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="226"/>
+      <c r="D22" s="225"/>
       <c r="E22" s="4" t="s">
         <v>3</v>
       </c>
@@ -6349,7 +6394,7 @@
       <c r="C23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="226" t="s">
+      <c r="D23" s="225" t="s">
         <v>37</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -6364,7 +6409,7 @@
       <c r="C24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="226"/>
+      <c r="D24" s="225"/>
       <c r="E24" s="4" t="s">
         <v>3</v>
       </c>
@@ -6379,7 +6424,7 @@
       <c r="C25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="225" t="s">
+      <c r="D25" s="226" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -6394,7 +6439,7 @@
       <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="225"/>
+      <c r="D26" s="226"/>
       <c r="E26" s="4" t="s">
         <v>3</v>
       </c>
@@ -6407,7 +6452,7 @@
       <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="225"/>
+      <c r="D27" s="226"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -6418,7 +6463,7 @@
       <c r="C28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="226" t="s">
+      <c r="D28" s="225" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="4"/>
@@ -6431,7 +6476,7 @@
       <c r="C29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="226"/>
+      <c r="D29" s="225"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -6442,7 +6487,7 @@
       <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="226"/>
+      <c r="D30" s="225"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -6455,7 +6500,7 @@
       <c r="C31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="226" t="s">
+      <c r="D31" s="225" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="4"/>
@@ -6468,7 +6513,7 @@
       <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="226"/>
+      <c r="D32" s="225"/>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -6494,7 +6539,7 @@
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="226" t="s">
+      <c r="D34" s="225" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="4"/>
@@ -6507,7 +6552,7 @@
       <c r="C35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="226"/>
+      <c r="D35" s="225"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -6518,7 +6563,7 @@
       <c r="C36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="226"/>
+      <c r="D36" s="225"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -6529,7 +6574,7 @@
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="226"/>
+      <c r="D37" s="225"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -6540,7 +6585,7 @@
       <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="225" t="s">
+      <c r="D38" s="226" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="4"/>
@@ -6553,7 +6598,7 @@
       <c r="C39" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="225"/>
+      <c r="D39" s="226"/>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -6566,7 +6611,7 @@
       <c r="C40" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="226" t="s">
+      <c r="D40" s="225" t="s">
         <v>58</v>
       </c>
       <c r="E40" s="4"/>
@@ -6579,7 +6624,7 @@
       <c r="C41" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="226"/>
+      <c r="D41" s="225"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -6590,7 +6635,7 @@
       <c r="C42" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="226"/>
+      <c r="D42" s="225"/>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -6601,7 +6646,7 @@
       <c r="C43" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="226" t="s">
+      <c r="D43" s="225" t="s">
         <v>65</v>
       </c>
       <c r="E43" s="4"/>
@@ -6614,7 +6659,7 @@
       <c r="C44" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="226"/>
+      <c r="D44" s="225"/>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -6625,11 +6670,24 @@
       <c r="C45" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="226"/>
+      <c r="D45" s="225"/>
       <c r="E45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="D43:D45"/>
@@ -6641,19 +6699,6 @@
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="D38:D39"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7659,16 +7704,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="D63:E63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D41:E41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7970,20 +8015,20 @@
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="271" t="s">
+      <c r="B4" s="237" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="272"/>
-      <c r="D4" s="272"/>
-      <c r="E4" s="272"/>
-      <c r="F4" s="272"/>
-      <c r="G4" s="272"/>
-      <c r="H4" s="272"/>
-      <c r="I4" s="272"/>
-      <c r="J4" s="272"/>
-      <c r="K4" s="272"/>
-      <c r="L4" s="272"/>
-      <c r="M4" s="273"/>
+      <c r="C4" s="238"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="238"/>
+      <c r="F4" s="238"/>
+      <c r="G4" s="238"/>
+      <c r="H4" s="238"/>
+      <c r="I4" s="238"/>
+      <c r="J4" s="238"/>
+      <c r="K4" s="238"/>
+      <c r="L4" s="238"/>
+      <c r="M4" s="239"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
@@ -8003,239 +8048,239 @@
       <c r="B6" s="250" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="252"/>
-      <c r="D6" s="278" t="s">
+      <c r="C6" s="251"/>
+      <c r="D6" s="256" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="268" t="s">
+      <c r="E6" s="267" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="269"/>
-      <c r="G6" s="269"/>
-      <c r="H6" s="269"/>
-      <c r="I6" s="269"/>
-      <c r="J6" s="269"/>
-      <c r="K6" s="269"/>
-      <c r="L6" s="269"/>
-      <c r="M6" s="270"/>
+      <c r="F6" s="268"/>
+      <c r="G6" s="268"/>
+      <c r="H6" s="268"/>
+      <c r="I6" s="268"/>
+      <c r="J6" s="268"/>
+      <c r="K6" s="268"/>
+      <c r="L6" s="268"/>
+      <c r="M6" s="269"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="253"/>
-      <c r="C7" s="255"/>
-      <c r="D7" s="279"/>
-      <c r="E7" s="241"/>
-      <c r="F7" s="242"/>
-      <c r="G7" s="242"/>
-      <c r="H7" s="242"/>
-      <c r="I7" s="242"/>
-      <c r="J7" s="242"/>
-      <c r="K7" s="242"/>
-      <c r="L7" s="242"/>
-      <c r="M7" s="243"/>
+      <c r="B7" s="252"/>
+      <c r="C7" s="253"/>
+      <c r="D7" s="257"/>
+      <c r="E7" s="244"/>
+      <c r="F7" s="245"/>
+      <c r="G7" s="245"/>
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="245"/>
+      <c r="M7" s="246"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="253"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="238" t="s">
+      <c r="B8" s="252"/>
+      <c r="C8" s="253"/>
+      <c r="D8" s="258" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="244" t="s">
+      <c r="E8" s="263" t="s">
         <v>143</v>
       </c>
-      <c r="F8" s="242"/>
-      <c r="G8" s="242"/>
-      <c r="H8" s="242"/>
-      <c r="I8" s="242"/>
-      <c r="J8" s="242"/>
-      <c r="K8" s="242"/>
-      <c r="L8" s="242"/>
-      <c r="M8" s="243"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245"/>
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="245"/>
+      <c r="K8" s="245"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="246"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="256"/>
-      <c r="C9" s="258"/>
-      <c r="D9" s="238"/>
-      <c r="E9" s="241"/>
-      <c r="F9" s="242"/>
-      <c r="G9" s="242"/>
-      <c r="H9" s="242"/>
-      <c r="I9" s="242"/>
-      <c r="J9" s="242"/>
-      <c r="K9" s="242"/>
-      <c r="L9" s="242"/>
-      <c r="M9" s="243"/>
+      <c r="B9" s="254"/>
+      <c r="C9" s="255"/>
+      <c r="D9" s="258"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="245"/>
+      <c r="G9" s="245"/>
+      <c r="H9" s="245"/>
+      <c r="I9" s="245"/>
+      <c r="J9" s="245"/>
+      <c r="K9" s="245"/>
+      <c r="L9" s="245"/>
+      <c r="M9" s="246"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="250" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="251"/>
-      <c r="D10" s="252"/>
-      <c r="E10" s="275" t="s">
+      <c r="C10" s="264"/>
+      <c r="D10" s="251"/>
+      <c r="E10" s="247" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="276"/>
-      <c r="G10" s="276"/>
-      <c r="H10" s="276"/>
-      <c r="I10" s="276"/>
-      <c r="J10" s="276"/>
-      <c r="K10" s="276"/>
-      <c r="L10" s="276"/>
-      <c r="M10" s="277"/>
+      <c r="F10" s="248"/>
+      <c r="G10" s="248"/>
+      <c r="H10" s="248"/>
+      <c r="I10" s="248"/>
+      <c r="J10" s="248"/>
+      <c r="K10" s="248"/>
+      <c r="L10" s="248"/>
+      <c r="M10" s="249"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="253"/>
-      <c r="C11" s="254"/>
-      <c r="D11" s="255"/>
-      <c r="E11" s="241"/>
-      <c r="F11" s="242"/>
-      <c r="G11" s="242"/>
-      <c r="H11" s="242"/>
-      <c r="I11" s="242"/>
-      <c r="J11" s="242"/>
-      <c r="K11" s="242"/>
-      <c r="L11" s="242"/>
-      <c r="M11" s="243"/>
+      <c r="B11" s="252"/>
+      <c r="C11" s="265"/>
+      <c r="D11" s="253"/>
+      <c r="E11" s="244"/>
+      <c r="F11" s="245"/>
+      <c r="G11" s="245"/>
+      <c r="H11" s="245"/>
+      <c r="I11" s="245"/>
+      <c r="J11" s="245"/>
+      <c r="K11" s="245"/>
+      <c r="L11" s="245"/>
+      <c r="M11" s="246"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="253"/>
-      <c r="C12" s="254"/>
-      <c r="D12" s="255"/>
-      <c r="E12" s="241"/>
-      <c r="F12" s="242"/>
-      <c r="G12" s="242"/>
-      <c r="H12" s="242"/>
-      <c r="I12" s="242"/>
-      <c r="J12" s="242"/>
-      <c r="K12" s="242"/>
-      <c r="L12" s="242"/>
-      <c r="M12" s="243"/>
+      <c r="B12" s="252"/>
+      <c r="C12" s="265"/>
+      <c r="D12" s="253"/>
+      <c r="E12" s="244"/>
+      <c r="F12" s="245"/>
+      <c r="G12" s="245"/>
+      <c r="H12" s="245"/>
+      <c r="I12" s="245"/>
+      <c r="J12" s="245"/>
+      <c r="K12" s="245"/>
+      <c r="L12" s="245"/>
+      <c r="M12" s="246"/>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="256"/>
-      <c r="C13" s="257"/>
-      <c r="D13" s="258"/>
-      <c r="E13" s="241"/>
-      <c r="F13" s="242"/>
-      <c r="G13" s="242"/>
-      <c r="H13" s="242"/>
-      <c r="I13" s="242"/>
-      <c r="J13" s="242"/>
-      <c r="K13" s="242"/>
-      <c r="L13" s="242"/>
-      <c r="M13" s="243"/>
+      <c r="B13" s="254"/>
+      <c r="C13" s="266"/>
+      <c r="D13" s="255"/>
+      <c r="E13" s="244"/>
+      <c r="F13" s="245"/>
+      <c r="G13" s="245"/>
+      <c r="H13" s="245"/>
+      <c r="I13" s="245"/>
+      <c r="J13" s="245"/>
+      <c r="K13" s="245"/>
+      <c r="L13" s="245"/>
+      <c r="M13" s="246"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="250" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="251"/>
-      <c r="D14" s="252"/>
-      <c r="E14" s="244" t="s">
+      <c r="C14" s="264"/>
+      <c r="D14" s="251"/>
+      <c r="E14" s="263" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="242"/>
-      <c r="G14" s="242"/>
-      <c r="H14" s="242"/>
-      <c r="I14" s="242"/>
-      <c r="J14" s="242"/>
-      <c r="K14" s="242"/>
-      <c r="L14" s="242"/>
-      <c r="M14" s="243"/>
+      <c r="F14" s="245"/>
+      <c r="G14" s="245"/>
+      <c r="H14" s="245"/>
+      <c r="I14" s="245"/>
+      <c r="J14" s="245"/>
+      <c r="K14" s="245"/>
+      <c r="L14" s="245"/>
+      <c r="M14" s="246"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="253"/>
-      <c r="C15" s="254"/>
-      <c r="D15" s="255"/>
-      <c r="E15" s="241"/>
-      <c r="F15" s="242"/>
-      <c r="G15" s="242"/>
-      <c r="H15" s="242"/>
-      <c r="I15" s="242"/>
-      <c r="J15" s="242"/>
-      <c r="K15" s="242"/>
-      <c r="L15" s="242"/>
-      <c r="M15" s="243"/>
+      <c r="B15" s="252"/>
+      <c r="C15" s="265"/>
+      <c r="D15" s="253"/>
+      <c r="E15" s="244"/>
+      <c r="F15" s="245"/>
+      <c r="G15" s="245"/>
+      <c r="H15" s="245"/>
+      <c r="I15" s="245"/>
+      <c r="J15" s="245"/>
+      <c r="K15" s="245"/>
+      <c r="L15" s="245"/>
+      <c r="M15" s="246"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="253"/>
-      <c r="C16" s="254"/>
-      <c r="D16" s="255"/>
-      <c r="E16" s="241"/>
-      <c r="F16" s="242"/>
-      <c r="G16" s="242"/>
-      <c r="H16" s="242"/>
-      <c r="I16" s="242"/>
-      <c r="J16" s="242"/>
-      <c r="K16" s="242"/>
-      <c r="L16" s="242"/>
-      <c r="M16" s="243"/>
+      <c r="B16" s="252"/>
+      <c r="C16" s="265"/>
+      <c r="D16" s="253"/>
+      <c r="E16" s="244"/>
+      <c r="F16" s="245"/>
+      <c r="G16" s="245"/>
+      <c r="H16" s="245"/>
+      <c r="I16" s="245"/>
+      <c r="J16" s="245"/>
+      <c r="K16" s="245"/>
+      <c r="L16" s="245"/>
+      <c r="M16" s="246"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="256"/>
-      <c r="C17" s="257"/>
-      <c r="D17" s="258"/>
-      <c r="E17" s="241"/>
-      <c r="F17" s="242"/>
-      <c r="G17" s="242"/>
-      <c r="H17" s="242"/>
-      <c r="I17" s="242"/>
-      <c r="J17" s="242"/>
-      <c r="K17" s="242"/>
-      <c r="L17" s="242"/>
-      <c r="M17" s="243"/>
+      <c r="B17" s="254"/>
+      <c r="C17" s="266"/>
+      <c r="D17" s="255"/>
+      <c r="E17" s="244"/>
+      <c r="F17" s="245"/>
+      <c r="G17" s="245"/>
+      <c r="H17" s="245"/>
+      <c r="I17" s="245"/>
+      <c r="J17" s="245"/>
+      <c r="K17" s="245"/>
+      <c r="L17" s="245"/>
+      <c r="M17" s="246"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="235" t="s">
+      <c r="B18" s="282" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="236"/>
+      <c r="C18" s="283"/>
       <c r="D18" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="244" t="s">
+      <c r="E18" s="263" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="242"/>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
-      <c r="I18" s="242"/>
-      <c r="J18" s="242"/>
-      <c r="K18" s="242"/>
-      <c r="L18" s="242"/>
-      <c r="M18" s="243"/>
+      <c r="F18" s="245"/>
+      <c r="G18" s="245"/>
+      <c r="H18" s="245"/>
+      <c r="I18" s="245"/>
+      <c r="J18" s="245"/>
+      <c r="K18" s="245"/>
+      <c r="L18" s="245"/>
+      <c r="M18" s="246"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="237"/>
-      <c r="C19" s="238"/>
+      <c r="B19" s="284"/>
+      <c r="C19" s="258"/>
       <c r="D19" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="244"/>
-      <c r="F19" s="242"/>
-      <c r="G19" s="242"/>
-      <c r="H19" s="242"/>
-      <c r="I19" s="242"/>
-      <c r="J19" s="242"/>
-      <c r="K19" s="242"/>
-      <c r="L19" s="242"/>
-      <c r="M19" s="243"/>
+      <c r="E19" s="263"/>
+      <c r="F19" s="245"/>
+      <c r="G19" s="245"/>
+      <c r="H19" s="245"/>
+      <c r="I19" s="245"/>
+      <c r="J19" s="245"/>
+      <c r="K19" s="245"/>
+      <c r="L19" s="245"/>
+      <c r="M19" s="246"/>
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="239"/>
-      <c r="C20" s="240"/>
+      <c r="B20" s="285"/>
+      <c r="C20" s="286"/>
       <c r="D20" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="241"/>
-      <c r="F20" s="242"/>
-      <c r="G20" s="242"/>
-      <c r="H20" s="242"/>
-      <c r="I20" s="242"/>
-      <c r="J20" s="242"/>
-      <c r="K20" s="242"/>
-      <c r="L20" s="242"/>
-      <c r="M20" s="243"/>
+      <c r="E20" s="244"/>
+      <c r="F20" s="245"/>
+      <c r="G20" s="245"/>
+      <c r="H20" s="245"/>
+      <c r="I20" s="245"/>
+      <c r="J20" s="245"/>
+      <c r="K20" s="245"/>
+      <c r="L20" s="245"/>
+      <c r="M20" s="246"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
@@ -8266,126 +8311,126 @@
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="229" t="s">
+      <c r="B23" s="276" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="230"/>
-      <c r="D23" s="230"/>
-      <c r="E23" s="230"/>
-      <c r="F23" s="230"/>
-      <c r="G23" s="230"/>
-      <c r="H23" s="230"/>
-      <c r="I23" s="230"/>
-      <c r="J23" s="230"/>
-      <c r="K23" s="230"/>
-      <c r="L23" s="230"/>
-      <c r="M23" s="231"/>
+      <c r="C23" s="277"/>
+      <c r="D23" s="277"/>
+      <c r="E23" s="277"/>
+      <c r="F23" s="277"/>
+      <c r="G23" s="277"/>
+      <c r="H23" s="277"/>
+      <c r="I23" s="277"/>
+      <c r="J23" s="277"/>
+      <c r="K23" s="277"/>
+      <c r="L23" s="277"/>
+      <c r="M23" s="278"/>
     </row>
     <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="232" t="s">
+      <c r="C24" s="279" t="s">
         <v>155</v>
       </c>
-      <c r="D24" s="234"/>
-      <c r="E24" s="232" t="s">
+      <c r="D24" s="281"/>
+      <c r="E24" s="279" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="233"/>
-      <c r="G24" s="233"/>
-      <c r="H24" s="233"/>
-      <c r="I24" s="233"/>
-      <c r="J24" s="233"/>
-      <c r="K24" s="234"/>
-      <c r="L24" s="280" t="s">
+      <c r="F24" s="280"/>
+      <c r="G24" s="280"/>
+      <c r="H24" s="280"/>
+      <c r="I24" s="280"/>
+      <c r="J24" s="280"/>
+      <c r="K24" s="281"/>
+      <c r="L24" s="259" t="s">
         <v>157</v>
       </c>
-      <c r="M24" s="281"/>
+      <c r="M24" s="260"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="13"/>
-      <c r="C25" s="245"/>
-      <c r="D25" s="247"/>
-      <c r="E25" s="245"/>
-      <c r="F25" s="246"/>
-      <c r="G25" s="246"/>
-      <c r="H25" s="246"/>
-      <c r="I25" s="246"/>
-      <c r="J25" s="246"/>
-      <c r="K25" s="247"/>
-      <c r="L25" s="245"/>
-      <c r="M25" s="274"/>
+      <c r="C25" s="240"/>
+      <c r="D25" s="288"/>
+      <c r="E25" s="240"/>
+      <c r="F25" s="287"/>
+      <c r="G25" s="287"/>
+      <c r="H25" s="287"/>
+      <c r="I25" s="287"/>
+      <c r="J25" s="287"/>
+      <c r="K25" s="288"/>
+      <c r="L25" s="240"/>
+      <c r="M25" s="241"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="248"/>
-      <c r="D26" s="249"/>
-      <c r="E26" s="248"/>
-      <c r="F26" s="265"/>
-      <c r="G26" s="265"/>
-      <c r="H26" s="265"/>
-      <c r="I26" s="265"/>
-      <c r="J26" s="265"/>
-      <c r="K26" s="249"/>
-      <c r="L26" s="248"/>
-      <c r="M26" s="267"/>
+      <c r="C26" s="242"/>
+      <c r="D26" s="262"/>
+      <c r="E26" s="242"/>
+      <c r="F26" s="261"/>
+      <c r="G26" s="261"/>
+      <c r="H26" s="261"/>
+      <c r="I26" s="261"/>
+      <c r="J26" s="261"/>
+      <c r="K26" s="262"/>
+      <c r="L26" s="242"/>
+      <c r="M26" s="243"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
-      <c r="C27" s="248"/>
-      <c r="D27" s="249"/>
-      <c r="E27" s="248"/>
-      <c r="F27" s="265"/>
-      <c r="G27" s="265"/>
-      <c r="H27" s="265"/>
-      <c r="I27" s="265"/>
-      <c r="J27" s="265"/>
-      <c r="K27" s="249"/>
-      <c r="L27" s="248"/>
-      <c r="M27" s="267"/>
+      <c r="C27" s="242"/>
+      <c r="D27" s="262"/>
+      <c r="E27" s="242"/>
+      <c r="F27" s="261"/>
+      <c r="G27" s="261"/>
+      <c r="H27" s="261"/>
+      <c r="I27" s="261"/>
+      <c r="J27" s="261"/>
+      <c r="K27" s="262"/>
+      <c r="L27" s="242"/>
+      <c r="M27" s="243"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="13"/>
-      <c r="C28" s="248"/>
-      <c r="D28" s="249"/>
-      <c r="E28" s="248"/>
-      <c r="F28" s="265"/>
-      <c r="G28" s="265"/>
-      <c r="H28" s="265"/>
-      <c r="I28" s="265"/>
-      <c r="J28" s="265"/>
-      <c r="K28" s="249"/>
-      <c r="L28" s="248"/>
-      <c r="M28" s="267"/>
+      <c r="C28" s="242"/>
+      <c r="D28" s="262"/>
+      <c r="E28" s="242"/>
+      <c r="F28" s="261"/>
+      <c r="G28" s="261"/>
+      <c r="H28" s="261"/>
+      <c r="I28" s="261"/>
+      <c r="J28" s="261"/>
+      <c r="K28" s="262"/>
+      <c r="L28" s="242"/>
+      <c r="M28" s="243"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="13"/>
-      <c r="C29" s="248"/>
-      <c r="D29" s="249"/>
-      <c r="E29" s="248"/>
-      <c r="F29" s="265"/>
-      <c r="G29" s="265"/>
-      <c r="H29" s="265"/>
-      <c r="I29" s="265"/>
-      <c r="J29" s="265"/>
-      <c r="K29" s="249"/>
-      <c r="L29" s="248"/>
-      <c r="M29" s="267"/>
+      <c r="C29" s="242"/>
+      <c r="D29" s="262"/>
+      <c r="E29" s="242"/>
+      <c r="F29" s="261"/>
+      <c r="G29" s="261"/>
+      <c r="H29" s="261"/>
+      <c r="I29" s="261"/>
+      <c r="J29" s="261"/>
+      <c r="K29" s="262"/>
+      <c r="L29" s="242"/>
+      <c r="M29" s="243"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
-      <c r="C30" s="262"/>
-      <c r="D30" s="264"/>
-      <c r="E30" s="262"/>
-      <c r="F30" s="266"/>
-      <c r="G30" s="266"/>
-      <c r="H30" s="266"/>
-      <c r="I30" s="266"/>
-      <c r="J30" s="266"/>
-      <c r="K30" s="264"/>
-      <c r="L30" s="262"/>
-      <c r="M30" s="263"/>
+      <c r="C30" s="271"/>
+      <c r="D30" s="273"/>
+      <c r="E30" s="271"/>
+      <c r="F30" s="274"/>
+      <c r="G30" s="274"/>
+      <c r="H30" s="274"/>
+      <c r="I30" s="274"/>
+      <c r="J30" s="274"/>
+      <c r="K30" s="273"/>
+      <c r="L30" s="271"/>
+      <c r="M30" s="272"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
@@ -8402,20 +8447,20 @@
       <c r="M31" s="12"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="229" t="s">
+      <c r="B32" s="276" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="230"/>
-      <c r="D32" s="230"/>
-      <c r="E32" s="230"/>
-      <c r="F32" s="230"/>
-      <c r="G32" s="230"/>
-      <c r="H32" s="230"/>
-      <c r="I32" s="230"/>
-      <c r="J32" s="230"/>
-      <c r="K32" s="230"/>
-      <c r="L32" s="230"/>
-      <c r="M32" s="231"/>
+      <c r="C32" s="277"/>
+      <c r="D32" s="277"/>
+      <c r="E32" s="277"/>
+      <c r="F32" s="277"/>
+      <c r="G32" s="277"/>
+      <c r="H32" s="277"/>
+      <c r="I32" s="277"/>
+      <c r="J32" s="277"/>
+      <c r="K32" s="277"/>
+      <c r="L32" s="277"/>
+      <c r="M32" s="278"/>
     </row>
     <row r="33" spans="2:13" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="26" t="s">
@@ -8424,10 +8469,10 @@
       <c r="C33" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="D33" s="232" t="s">
+      <c r="D33" s="279" t="s">
         <v>161</v>
       </c>
-      <c r="E33" s="234"/>
+      <c r="E33" s="281"/>
       <c r="F33" s="27" t="s">
         <v>162</v>
       </c>
@@ -8458,8 +8503,8 @@
         <v>1</v>
       </c>
       <c r="C34" s="22"/>
-      <c r="D34" s="259"/>
-      <c r="E34" s="259"/>
+      <c r="D34" s="289"/>
+      <c r="E34" s="289"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
@@ -8474,8 +8519,8 @@
         <v>2</v>
       </c>
       <c r="C35" s="17"/>
-      <c r="D35" s="260"/>
-      <c r="E35" s="260"/>
+      <c r="D35" s="236"/>
+      <c r="E35" s="236"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -8490,8 +8535,8 @@
         <v>3</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="260"/>
-      <c r="E36" s="260"/>
+      <c r="D36" s="236"/>
+      <c r="E36" s="236"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
@@ -8506,8 +8551,8 @@
         <v>4</v>
       </c>
       <c r="C37" s="29"/>
-      <c r="D37" s="261"/>
-      <c r="E37" s="261"/>
+      <c r="D37" s="270"/>
+      <c r="E37" s="270"/>
       <c r="F37" s="30"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
@@ -8520,8 +8565,8 @@
     <row r="38" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="33"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="228"/>
-      <c r="E38" s="228"/>
+      <c r="D38" s="275"/>
+      <c r="E38" s="275"/>
       <c r="F38" s="34"/>
       <c r="G38" s="34" t="s">
         <v>169</v>
@@ -8542,16 +8587,16 @@
       <c r="M38" s="36"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="286" t="s">
+      <c r="B41" s="232" t="s">
         <v>170</v>
       </c>
-      <c r="C41" s="286"/>
-      <c r="D41" s="286"/>
-      <c r="E41" s="286"/>
-      <c r="F41" s="286"/>
-      <c r="G41" s="286"/>
-      <c r="H41" s="286"/>
-      <c r="I41" s="286"/>
+      <c r="C41" s="232"/>
+      <c r="D41" s="232"/>
+      <c r="E41" s="232"/>
+      <c r="F41" s="232"/>
+      <c r="G41" s="232"/>
+      <c r="H41" s="232"/>
+      <c r="I41" s="232"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
@@ -8564,16 +8609,16 @@
       <c r="C42" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="285" t="s">
+      <c r="D42" s="231" t="s">
         <v>172</v>
       </c>
-      <c r="E42" s="285"/>
-      <c r="F42" s="285" t="s">
+      <c r="E42" s="231"/>
+      <c r="F42" s="231" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="285"/>
-      <c r="H42" s="285"/>
-      <c r="I42" s="285"/>
+      <c r="G42" s="231"/>
+      <c r="H42" s="231"/>
+      <c r="I42" s="231"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
@@ -8584,8 +8629,8 @@
         <v>1</v>
       </c>
       <c r="C43" s="17"/>
-      <c r="D43" s="260"/>
-      <c r="E43" s="260"/>
+      <c r="D43" s="236"/>
+      <c r="E43" s="236"/>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
@@ -8600,8 +8645,8 @@
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="260"/>
-      <c r="E44" s="260"/>
+      <c r="D44" s="236"/>
+      <c r="E44" s="236"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -8616,8 +8661,8 @@
         <v>3</v>
       </c>
       <c r="C45" s="17"/>
-      <c r="D45" s="260"/>
-      <c r="E45" s="260"/>
+      <c r="D45" s="236"/>
+      <c r="E45" s="236"/>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
@@ -8628,16 +8673,16 @@
       <c r="M45" s="12"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="286" t="s">
+      <c r="B47" s="232" t="s">
         <v>174</v>
       </c>
-      <c r="C47" s="286"/>
-      <c r="D47" s="286"/>
-      <c r="E47" s="286"/>
-      <c r="F47" s="286"/>
-      <c r="G47" s="286"/>
-      <c r="H47" s="286"/>
-      <c r="I47" s="286"/>
+      <c r="C47" s="232"/>
+      <c r="D47" s="232"/>
+      <c r="E47" s="232"/>
+      <c r="F47" s="232"/>
+      <c r="G47" s="232"/>
+      <c r="H47" s="232"/>
+      <c r="I47" s="232"/>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
@@ -8650,14 +8695,14 @@
       <c r="C48" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="D48" s="287" t="s">
+      <c r="D48" s="233" t="s">
         <v>176</v>
       </c>
-      <c r="E48" s="288"/>
-      <c r="F48" s="288"/>
-      <c r="G48" s="288"/>
-      <c r="H48" s="288"/>
-      <c r="I48" s="289"/>
+      <c r="E48" s="234"/>
+      <c r="F48" s="234"/>
+      <c r="G48" s="234"/>
+      <c r="H48" s="234"/>
+      <c r="I48" s="235"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
@@ -8670,12 +8715,12 @@
       <c r="C49" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D49" s="282"/>
-      <c r="E49" s="283"/>
-      <c r="F49" s="283"/>
-      <c r="G49" s="283"/>
-      <c r="H49" s="283"/>
-      <c r="I49" s="284"/>
+      <c r="D49" s="228"/>
+      <c r="E49" s="229"/>
+      <c r="F49" s="229"/>
+      <c r="G49" s="229"/>
+      <c r="H49" s="229"/>
+      <c r="I49" s="230"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="17">
@@ -8684,12 +8729,12 @@
       <c r="C50" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D50" s="282"/>
-      <c r="E50" s="283"/>
-      <c r="F50" s="283"/>
-      <c r="G50" s="283"/>
-      <c r="H50" s="283"/>
-      <c r="I50" s="284"/>
+      <c r="D50" s="228"/>
+      <c r="E50" s="229"/>
+      <c r="F50" s="229"/>
+      <c r="G50" s="229"/>
+      <c r="H50" s="229"/>
+      <c r="I50" s="230"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="17">
@@ -8698,77 +8743,128 @@
       <c r="C51" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D51" s="282"/>
-      <c r="E51" s="283"/>
-      <c r="F51" s="283"/>
-      <c r="G51" s="283"/>
-      <c r="H51" s="283"/>
-      <c r="I51" s="284"/>
+      <c r="D51" s="228"/>
+      <c r="E51" s="229"/>
+      <c r="F51" s="229"/>
+      <c r="G51" s="229"/>
+      <c r="H51" s="229"/>
+      <c r="I51" s="230"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="286" t="s">
+      <c r="B54" s="232" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="286"/>
-      <c r="D54" s="286"/>
-      <c r="E54" s="286"/>
-      <c r="F54" s="286"/>
-      <c r="G54" s="286"/>
-      <c r="H54" s="286"/>
-      <c r="I54" s="286"/>
+      <c r="C54" s="232"/>
+      <c r="D54" s="232"/>
+      <c r="E54" s="232"/>
+      <c r="F54" s="232"/>
+      <c r="G54" s="232"/>
+      <c r="H54" s="232"/>
+      <c r="I54" s="232"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="C55" s="287" t="s">
+      <c r="C55" s="233" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="288"/>
-      <c r="E55" s="288"/>
-      <c r="F55" s="288"/>
-      <c r="G55" s="288"/>
-      <c r="H55" s="288"/>
-      <c r="I55" s="289"/>
+      <c r="D55" s="234"/>
+      <c r="E55" s="234"/>
+      <c r="F55" s="234"/>
+      <c r="G55" s="234"/>
+      <c r="H55" s="234"/>
+      <c r="I55" s="235"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="17">
         <v>1</v>
       </c>
-      <c r="C56" s="282"/>
-      <c r="D56" s="283"/>
-      <c r="E56" s="283"/>
-      <c r="F56" s="283"/>
-      <c r="G56" s="283"/>
-      <c r="H56" s="283"/>
-      <c r="I56" s="284"/>
+      <c r="C56" s="228"/>
+      <c r="D56" s="229"/>
+      <c r="E56" s="229"/>
+      <c r="F56" s="229"/>
+      <c r="G56" s="229"/>
+      <c r="H56" s="229"/>
+      <c r="I56" s="230"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="17">
         <v>2</v>
       </c>
-      <c r="C57" s="282"/>
-      <c r="D57" s="283"/>
-      <c r="E57" s="283"/>
-      <c r="F57" s="283"/>
-      <c r="G57" s="283"/>
-      <c r="H57" s="283"/>
-      <c r="I57" s="284"/>
+      <c r="C57" s="228"/>
+      <c r="D57" s="229"/>
+      <c r="E57" s="229"/>
+      <c r="F57" s="229"/>
+      <c r="G57" s="229"/>
+      <c r="H57" s="229"/>
+      <c r="I57" s="230"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="17">
         <v>3</v>
       </c>
-      <c r="C58" s="282"/>
-      <c r="D58" s="283"/>
-      <c r="E58" s="283"/>
-      <c r="F58" s="283"/>
-      <c r="G58" s="283"/>
-      <c r="H58" s="283"/>
-      <c r="I58" s="284"/>
+      <c r="C58" s="228"/>
+      <c r="D58" s="229"/>
+      <c r="E58" s="229"/>
+      <c r="F58" s="229"/>
+      <c r="G58" s="229"/>
+      <c r="H58" s="229"/>
+      <c r="I58" s="230"/>
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="E24:K24"/>
+    <mergeCell ref="B18:C20"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B14:D17"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E27:K27"/>
+    <mergeCell ref="E28:K28"/>
+    <mergeCell ref="E29:K29"/>
+    <mergeCell ref="E30:K30"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="B10:D13"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="E7:M7"/>
+    <mergeCell ref="E8:M8"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="B6:C9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="E13:M13"/>
+    <mergeCell ref="E14:M14"/>
     <mergeCell ref="C57:I57"/>
     <mergeCell ref="C58:I58"/>
     <mergeCell ref="F42:I42"/>
@@ -8785,57 +8881,6 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="C56:I56"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E10:M10"/>
-    <mergeCell ref="B6:C9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="E11:M11"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="E13:M13"/>
-    <mergeCell ref="E14:M14"/>
-    <mergeCell ref="E15:M15"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="B10:D13"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="E7:M7"/>
-    <mergeCell ref="E8:M8"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E27:K27"/>
-    <mergeCell ref="E28:K28"/>
-    <mergeCell ref="E29:K29"/>
-    <mergeCell ref="E30:K30"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="E24:K24"/>
-    <mergeCell ref="B18:C20"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="E18:M18"/>
-    <mergeCell ref="E19:M19"/>
-    <mergeCell ref="E20:M20"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B14:D17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10627,34 +10672,34 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="323" t="s">
+      <c r="B2" s="312" t="s">
         <v>387</v>
       </c>
-      <c r="C2" s="324"/>
-      <c r="D2" s="324"/>
-      <c r="E2" s="324"/>
-      <c r="F2" s="324"/>
-      <c r="G2" s="324"/>
-      <c r="H2" s="324"/>
-      <c r="I2" s="324"/>
-      <c r="J2" s="324"/>
-      <c r="K2" s="325"/>
-      <c r="L2" s="326"/>
+      <c r="C2" s="313"/>
+      <c r="D2" s="313"/>
+      <c r="E2" s="313"/>
+      <c r="F2" s="313"/>
+      <c r="G2" s="313"/>
+      <c r="H2" s="313"/>
+      <c r="I2" s="313"/>
+      <c r="J2" s="313"/>
+      <c r="K2" s="314"/>
+      <c r="L2" s="315"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="327" t="s">
+      <c r="B3" s="316" t="s">
         <v>388</v>
       </c>
-      <c r="C3" s="328"/>
-      <c r="D3" s="328"/>
-      <c r="E3" s="328"/>
-      <c r="F3" s="328"/>
-      <c r="G3" s="328"/>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="328"/>
-      <c r="K3" s="329"/>
-      <c r="L3" s="330"/>
+      <c r="C3" s="317"/>
+      <c r="D3" s="317"/>
+      <c r="E3" s="317"/>
+      <c r="F3" s="317"/>
+      <c r="G3" s="317"/>
+      <c r="H3" s="317"/>
+      <c r="I3" s="317"/>
+      <c r="J3" s="317"/>
+      <c r="K3" s="318"/>
+      <c r="L3" s="319"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="303" t="s">
@@ -10668,7 +10713,7 @@
       <c r="H4" s="304"/>
       <c r="I4" s="304"/>
       <c r="J4" s="304"/>
-      <c r="K4" s="331"/>
+      <c r="K4" s="320"/>
       <c r="L4" s="305"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -10683,53 +10728,53 @@
       <c r="H5" s="293"/>
       <c r="I5" s="293"/>
       <c r="J5" s="293"/>
-      <c r="K5" s="332"/>
+      <c r="K5" s="321"/>
       <c r="L5" s="294"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="333" t="s">
+      <c r="B6" s="322" t="s">
         <v>389</v>
       </c>
-      <c r="C6" s="334"/>
-      <c r="D6" s="334"/>
-      <c r="E6" s="334"/>
-      <c r="F6" s="334"/>
-      <c r="G6" s="334"/>
-      <c r="H6" s="334"/>
-      <c r="I6" s="334"/>
-      <c r="J6" s="334"/>
-      <c r="K6" s="334"/>
-      <c r="L6" s="335"/>
+      <c r="C6" s="323"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="323"/>
+      <c r="G6" s="323"/>
+      <c r="H6" s="323"/>
+      <c r="I6" s="323"/>
+      <c r="J6" s="323"/>
+      <c r="K6" s="323"/>
+      <c r="L6" s="324"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="320" t="s">
+      <c r="B7" s="309" t="s">
         <v>390</v>
       </c>
-      <c r="C7" s="321"/>
-      <c r="D7" s="321"/>
-      <c r="E7" s="321"/>
-      <c r="F7" s="321"/>
-      <c r="G7" s="321"/>
-      <c r="H7" s="321"/>
-      <c r="I7" s="321"/>
-      <c r="J7" s="321"/>
-      <c r="K7" s="321"/>
-      <c r="L7" s="322"/>
+      <c r="C7" s="310"/>
+      <c r="D7" s="310"/>
+      <c r="E7" s="310"/>
+      <c r="F7" s="310"/>
+      <c r="G7" s="310"/>
+      <c r="H7" s="310"/>
+      <c r="I7" s="310"/>
+      <c r="J7" s="310"/>
+      <c r="K7" s="310"/>
+      <c r="L7" s="311"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="313" t="s">
+      <c r="B8" s="329" t="s">
         <v>391</v>
       </c>
-      <c r="C8" s="314"/>
-      <c r="D8" s="314"/>
-      <c r="E8" s="314"/>
-      <c r="F8" s="314"/>
-      <c r="G8" s="314"/>
-      <c r="H8" s="314"/>
-      <c r="I8" s="314"/>
-      <c r="J8" s="314"/>
-      <c r="K8" s="314"/>
-      <c r="L8" s="315"/>
+      <c r="C8" s="330"/>
+      <c r="D8" s="330"/>
+      <c r="E8" s="330"/>
+      <c r="F8" s="330"/>
+      <c r="G8" s="330"/>
+      <c r="H8" s="330"/>
+      <c r="I8" s="330"/>
+      <c r="J8" s="330"/>
+      <c r="K8" s="330"/>
+      <c r="L8" s="331"/>
     </row>
     <row r="9" spans="2:12" ht="33" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
@@ -12065,19 +12110,19 @@
       <c r="L65" s="51"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B66" s="316" t="s">
+      <c r="B66" s="332" t="s">
         <v>382</v>
       </c>
-      <c r="C66" s="317"/>
-      <c r="D66" s="317"/>
-      <c r="E66" s="317"/>
-      <c r="F66" s="317"/>
-      <c r="G66" s="317"/>
-      <c r="H66" s="317"/>
-      <c r="I66" s="317"/>
-      <c r="J66" s="317"/>
-      <c r="K66" s="318"/>
-      <c r="L66" s="319"/>
+      <c r="C66" s="333"/>
+      <c r="D66" s="333"/>
+      <c r="E66" s="333"/>
+      <c r="F66" s="333"/>
+      <c r="G66" s="333"/>
+      <c r="H66" s="333"/>
+      <c r="I66" s="333"/>
+      <c r="J66" s="333"/>
+      <c r="K66" s="334"/>
+      <c r="L66" s="335"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="298" t="s">
@@ -12086,15 +12131,15 @@
       <c r="C67" s="299"/>
       <c r="D67" s="299"/>
       <c r="E67" s="52"/>
-      <c r="F67" s="309" t="s">
+      <c r="F67" s="325" t="s">
         <v>191</v>
       </c>
-      <c r="G67" s="309"/>
-      <c r="H67" s="309"/>
-      <c r="I67" s="309"/>
-      <c r="J67" s="309"/>
-      <c r="K67" s="309"/>
-      <c r="L67" s="310"/>
+      <c r="G67" s="325"/>
+      <c r="H67" s="325"/>
+      <c r="I67" s="325"/>
+      <c r="J67" s="325"/>
+      <c r="K67" s="325"/>
+      <c r="L67" s="326"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="298" t="s">
@@ -12103,13 +12148,13 @@
       <c r="C68" s="299"/>
       <c r="D68" s="299"/>
       <c r="E68" s="52"/>
-      <c r="F68" s="309"/>
-      <c r="G68" s="309"/>
-      <c r="H68" s="309"/>
-      <c r="I68" s="309"/>
-      <c r="J68" s="309"/>
-      <c r="K68" s="309"/>
-      <c r="L68" s="310"/>
+      <c r="F68" s="325"/>
+      <c r="G68" s="325"/>
+      <c r="H68" s="325"/>
+      <c r="I68" s="325"/>
+      <c r="J68" s="325"/>
+      <c r="K68" s="325"/>
+      <c r="L68" s="326"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="298" t="s">
@@ -12118,15 +12163,15 @@
       <c r="C69" s="299"/>
       <c r="D69" s="299"/>
       <c r="E69" s="52"/>
-      <c r="F69" s="309" t="s">
+      <c r="F69" s="325" t="s">
         <v>191</v>
       </c>
-      <c r="G69" s="309"/>
-      <c r="H69" s="309"/>
-      <c r="I69" s="309"/>
-      <c r="J69" s="309"/>
-      <c r="K69" s="309"/>
-      <c r="L69" s="310"/>
+      <c r="G69" s="325"/>
+      <c r="H69" s="325"/>
+      <c r="I69" s="325"/>
+      <c r="J69" s="325"/>
+      <c r="K69" s="325"/>
+      <c r="L69" s="326"/>
     </row>
     <row r="70" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B70" s="290" t="s">
@@ -12135,22 +12180,16 @@
       <c r="C70" s="291"/>
       <c r="D70" s="291"/>
       <c r="E70" s="53"/>
-      <c r="F70" s="311"/>
-      <c r="G70" s="311"/>
-      <c r="H70" s="311"/>
-      <c r="I70" s="311"/>
-      <c r="J70" s="311"/>
-      <c r="K70" s="311"/>
-      <c r="L70" s="312"/>
+      <c r="F70" s="327"/>
+      <c r="G70" s="327"/>
+      <c r="H70" s="327"/>
+      <c r="I70" s="327"/>
+      <c r="J70" s="327"/>
+      <c r="K70" s="327"/>
+      <c r="L70" s="328"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:L5"/>
-    <mergeCell ref="B6:L6"/>
     <mergeCell ref="B69:D69"/>
     <mergeCell ref="F69:L69"/>
     <mergeCell ref="B70:D70"/>
@@ -12161,6 +12200,12 @@
     <mergeCell ref="F67:L67"/>
     <mergeCell ref="B68:D68"/>
     <mergeCell ref="F68:L68"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="B6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12170,8 +12215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F031F4EE-3EC7-47DE-91AF-34380ED2D64A}">
   <dimension ref="B1:AX159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14372,7 +14417,7 @@
         <v>705</v>
       </c>
       <c r="E7" s="191" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="F7" s="191" t="s">
         <v>626</v>
@@ -14387,7 +14432,9 @@
       <c r="J7" s="56" t="s">
         <v>612</v>
       </c>
-      <c r="K7" s="104"/>
+      <c r="K7" s="104" t="s">
+        <v>624</v>
+      </c>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
       <c r="N7" s="213">
@@ -14427,7 +14474,9 @@
       <c r="J8" s="200" t="s">
         <v>612</v>
       </c>
-      <c r="K8" s="201"/>
+      <c r="K8" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L8" s="200"/>
       <c r="M8" s="195"/>
       <c r="N8" s="202">
@@ -14469,7 +14518,9 @@
       <c r="J9" s="200" t="s">
         <v>613</v>
       </c>
-      <c r="K9" s="201"/>
+      <c r="K9" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L9" s="200"/>
       <c r="M9" s="195"/>
       <c r="N9" s="202">
@@ -14511,7 +14562,9 @@
       <c r="J10" s="200" t="s">
         <v>614</v>
       </c>
-      <c r="K10" s="201"/>
+      <c r="K10" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L10" s="200"/>
       <c r="M10" s="195"/>
       <c r="N10" s="202">
@@ -14551,7 +14604,9 @@
       <c r="J11" s="200" t="s">
         <v>615</v>
       </c>
-      <c r="K11" s="201"/>
+      <c r="K11" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L11" s="200"/>
       <c r="M11" s="195"/>
       <c r="N11" s="202">
@@ -14591,7 +14646,9 @@
       <c r="J12" s="200" t="s">
         <v>616</v>
       </c>
-      <c r="K12" s="201"/>
+      <c r="K12" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L12" s="200"/>
       <c r="M12" s="195"/>
       <c r="N12" s="202">
@@ -14629,7 +14686,9 @@
       </c>
       <c r="I13" s="195"/>
       <c r="J13" s="200"/>
-      <c r="K13" s="201"/>
+      <c r="K13" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L13" s="200"/>
       <c r="M13" s="195"/>
       <c r="N13" s="202">
@@ -14667,7 +14726,9 @@
       </c>
       <c r="I14" s="195"/>
       <c r="J14" s="200"/>
-      <c r="K14" s="201"/>
+      <c r="K14" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L14" s="200"/>
       <c r="M14" s="195"/>
       <c r="N14" s="202">
@@ -14705,7 +14766,9 @@
       </c>
       <c r="I15" s="195"/>
       <c r="J15" s="200"/>
-      <c r="K15" s="201"/>
+      <c r="K15" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L15" s="200"/>
       <c r="M15" s="195"/>
       <c r="N15" s="202">
@@ -14743,7 +14806,9 @@
       </c>
       <c r="I16" s="195"/>
       <c r="J16" s="200"/>
-      <c r="K16" s="201"/>
+      <c r="K16" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L16" s="200"/>
       <c r="M16" s="195"/>
       <c r="N16" s="202">
@@ -14781,7 +14846,9 @@
       </c>
       <c r="I17" s="195"/>
       <c r="J17" s="200"/>
-      <c r="K17" s="201"/>
+      <c r="K17" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L17" s="200"/>
       <c r="M17" s="195"/>
       <c r="N17" s="202">
@@ -14819,7 +14886,9 @@
       </c>
       <c r="I18" s="195"/>
       <c r="J18" s="200"/>
-      <c r="K18" s="201"/>
+      <c r="K18" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L18" s="200"/>
       <c r="M18" s="195"/>
       <c r="N18" s="202">
@@ -14857,7 +14926,9 @@
       </c>
       <c r="I19" s="195"/>
       <c r="J19" s="200"/>
-      <c r="K19" s="201"/>
+      <c r="K19" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L19" s="200"/>
       <c r="M19" s="195"/>
       <c r="N19" s="202">
@@ -14895,7 +14966,9 @@
       </c>
       <c r="I20" s="195"/>
       <c r="J20" s="200"/>
-      <c r="K20" s="201"/>
+      <c r="K20" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L20" s="200"/>
       <c r="M20" s="195"/>
       <c r="N20" s="202">
@@ -14933,7 +15006,9 @@
       </c>
       <c r="I21" s="195"/>
       <c r="J21" s="200"/>
-      <c r="K21" s="201"/>
+      <c r="K21" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L21" s="200"/>
       <c r="M21" s="195"/>
       <c r="N21" s="202">
@@ -14971,7 +15046,9 @@
       </c>
       <c r="I22" s="195"/>
       <c r="J22" s="200"/>
-      <c r="K22" s="201"/>
+      <c r="K22" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L22" s="200"/>
       <c r="M22" s="195"/>
       <c r="N22" s="202">
@@ -15009,7 +15086,9 @@
       </c>
       <c r="I23" s="195"/>
       <c r="J23" s="200"/>
-      <c r="K23" s="201"/>
+      <c r="K23" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L23" s="200"/>
       <c r="M23" s="195"/>
       <c r="N23" s="202">
@@ -15047,7 +15126,9 @@
       </c>
       <c r="I24" s="195"/>
       <c r="J24" s="200"/>
-      <c r="K24" s="201"/>
+      <c r="K24" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L24" s="200"/>
       <c r="M24" s="195"/>
       <c r="N24" s="202">
@@ -15085,7 +15166,9 @@
       </c>
       <c r="I25" s="195"/>
       <c r="J25" s="200"/>
-      <c r="K25" s="201"/>
+      <c r="K25" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L25" s="200"/>
       <c r="M25" s="195"/>
       <c r="N25" s="202">
@@ -15136,7 +15219,9 @@
       </c>
       <c r="I26" s="195"/>
       <c r="J26" s="200"/>
-      <c r="K26" s="201"/>
+      <c r="K26" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L26" s="200"/>
       <c r="M26" s="195"/>
       <c r="N26" s="202">
@@ -15187,7 +15272,9 @@
       </c>
       <c r="I27" s="195"/>
       <c r="J27" s="200"/>
-      <c r="K27" s="201"/>
+      <c r="K27" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L27" s="200"/>
       <c r="M27" s="195"/>
       <c r="N27" s="202">
@@ -15238,7 +15325,9 @@
       </c>
       <c r="I28" s="195"/>
       <c r="J28" s="200"/>
-      <c r="K28" s="201"/>
+      <c r="K28" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L28" s="200"/>
       <c r="M28" s="195"/>
       <c r="N28" s="202">
@@ -15293,7 +15382,9 @@
       </c>
       <c r="I29" s="195"/>
       <c r="J29" s="200"/>
-      <c r="K29" s="201"/>
+      <c r="K29" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L29" s="200"/>
       <c r="M29" s="195"/>
       <c r="N29" s="202">
@@ -15354,7 +15445,9 @@
       </c>
       <c r="I30" s="195"/>
       <c r="J30" s="200"/>
-      <c r="K30" s="201"/>
+      <c r="K30" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L30" s="200"/>
       <c r="M30" s="195"/>
       <c r="N30" s="202">
@@ -15415,7 +15508,9 @@
       </c>
       <c r="I31" s="195"/>
       <c r="J31" s="200"/>
-      <c r="K31" s="201"/>
+      <c r="K31" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L31" s="200"/>
       <c r="M31" s="195"/>
       <c r="N31" s="202">
@@ -15476,7 +15571,9 @@
       </c>
       <c r="I32" s="195"/>
       <c r="J32" s="200"/>
-      <c r="K32" s="201"/>
+      <c r="K32" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L32" s="200"/>
       <c r="M32" s="195"/>
       <c r="N32" s="202">
@@ -15537,7 +15634,9 @@
       </c>
       <c r="I33" s="195"/>
       <c r="J33" s="200"/>
-      <c r="K33" s="201"/>
+      <c r="K33" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L33" s="200"/>
       <c r="M33" s="195"/>
       <c r="N33" s="202">
@@ -15598,7 +15697,9 @@
       </c>
       <c r="I34" s="195"/>
       <c r="J34" s="200"/>
-      <c r="K34" s="201"/>
+      <c r="K34" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L34" s="200"/>
       <c r="M34" s="195"/>
       <c r="N34" s="202">
@@ -15655,7 +15756,9 @@
       </c>
       <c r="I35" s="195"/>
       <c r="J35" s="200"/>
-      <c r="K35" s="201"/>
+      <c r="K35" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L35" s="200"/>
       <c r="M35" s="195"/>
       <c r="N35" s="202">
@@ -15714,7 +15817,9 @@
       </c>
       <c r="I36" s="194"/>
       <c r="J36" s="200"/>
-      <c r="K36" s="201"/>
+      <c r="K36" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L36" s="200"/>
       <c r="M36" s="194"/>
       <c r="N36" s="202">
@@ -15771,7 +15876,9 @@
       </c>
       <c r="I37" s="194"/>
       <c r="J37" s="200"/>
-      <c r="K37" s="201"/>
+      <c r="K37" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L37" s="200"/>
       <c r="M37" s="194"/>
       <c r="N37" s="202">
@@ -15817,8 +15924,8 @@
       <c r="E38" s="194" t="s">
         <v>735</v>
       </c>
-      <c r="F38" s="194" t="s">
-        <v>626</v>
+      <c r="F38" s="216" t="s">
+        <v>640</v>
       </c>
       <c r="G38" s="195" t="s">
         <v>627</v>
@@ -15828,7 +15935,9 @@
       </c>
       <c r="I38" s="194"/>
       <c r="J38" s="200"/>
-      <c r="K38" s="201"/>
+      <c r="K38" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L38" s="200"/>
       <c r="M38" s="194"/>
       <c r="N38" s="202">
@@ -15881,7 +15990,9 @@
       </c>
       <c r="I39" s="194"/>
       <c r="J39" s="200"/>
-      <c r="K39" s="201"/>
+      <c r="K39" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L39" s="200"/>
       <c r="M39" s="194"/>
       <c r="N39" s="202">
@@ -15934,7 +16045,9 @@
       </c>
       <c r="I40" s="194"/>
       <c r="J40" s="200"/>
-      <c r="K40" s="201"/>
+      <c r="K40" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L40" s="200"/>
       <c r="M40" s="194"/>
       <c r="N40" s="202">
@@ -15987,7 +16100,9 @@
       </c>
       <c r="I41" s="194"/>
       <c r="J41" s="200"/>
-      <c r="K41" s="201"/>
+      <c r="K41" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L41" s="200"/>
       <c r="M41" s="194"/>
       <c r="N41" s="202">
@@ -16040,7 +16155,9 @@
       </c>
       <c r="I42" s="194"/>
       <c r="J42" s="200"/>
-      <c r="K42" s="201"/>
+      <c r="K42" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L42" s="200"/>
       <c r="M42" s="194"/>
       <c r="N42" s="202">
@@ -16093,7 +16210,9 @@
       </c>
       <c r="I43" s="194"/>
       <c r="J43" s="200"/>
-      <c r="K43" s="201"/>
+      <c r="K43" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L43" s="200"/>
       <c r="M43" s="194"/>
       <c r="N43" s="202">
@@ -16146,7 +16265,9 @@
       </c>
       <c r="I44" s="194"/>
       <c r="J44" s="200"/>
-      <c r="K44" s="201"/>
+      <c r="K44" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L44" s="200"/>
       <c r="M44" s="194"/>
       <c r="N44" s="202">
@@ -16211,7 +16332,9 @@
       </c>
       <c r="I45" s="194"/>
       <c r="J45" s="200"/>
-      <c r="K45" s="201"/>
+      <c r="K45" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L45" s="200"/>
       <c r="M45" s="194"/>
       <c r="N45" s="202">
@@ -16272,7 +16395,9 @@
       </c>
       <c r="I46" s="194"/>
       <c r="J46" s="200"/>
-      <c r="K46" s="201"/>
+      <c r="K46" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L46" s="200"/>
       <c r="M46" s="194"/>
       <c r="N46" s="202">
@@ -16333,7 +16458,9 @@
       </c>
       <c r="I47" s="194"/>
       <c r="J47" s="200"/>
-      <c r="K47" s="201"/>
+      <c r="K47" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L47" s="200"/>
       <c r="M47" s="194"/>
       <c r="N47" s="202">
@@ -16394,7 +16521,9 @@
       </c>
       <c r="I48" s="194"/>
       <c r="J48" s="200"/>
-      <c r="K48" s="201"/>
+      <c r="K48" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L48" s="200"/>
       <c r="M48" s="194"/>
       <c r="N48" s="202">
@@ -16455,7 +16584,9 @@
       </c>
       <c r="I49" s="194"/>
       <c r="J49" s="200"/>
-      <c r="K49" s="201"/>
+      <c r="K49" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L49" s="200"/>
       <c r="M49" s="194"/>
       <c r="N49" s="202">
@@ -16512,7 +16643,9 @@
       </c>
       <c r="I50" s="194"/>
       <c r="J50" s="200"/>
-      <c r="K50" s="201"/>
+      <c r="K50" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L50" s="200"/>
       <c r="M50" s="194"/>
       <c r="N50" s="202">
@@ -16567,7 +16700,9 @@
       </c>
       <c r="I51" s="194"/>
       <c r="J51" s="200"/>
-      <c r="K51" s="201"/>
+      <c r="K51" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L51" s="200"/>
       <c r="M51" s="194"/>
       <c r="N51" s="202">
@@ -16622,7 +16757,9 @@
       </c>
       <c r="I52" s="54"/>
       <c r="J52" s="56"/>
-      <c r="K52" s="57"/>
+      <c r="K52" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L52" s="56"/>
       <c r="M52" s="54"/>
       <c r="N52" s="212">
@@ -16677,7 +16814,9 @@
       </c>
       <c r="I53" s="54"/>
       <c r="J53" s="56"/>
-      <c r="K53" s="57"/>
+      <c r="K53" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L53" s="56"/>
       <c r="M53" s="54"/>
       <c r="N53" s="212">
@@ -16732,7 +16871,9 @@
       </c>
       <c r="I54" s="54"/>
       <c r="J54" s="56"/>
-      <c r="K54" s="57"/>
+      <c r="K54" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L54" s="56"/>
       <c r="M54" s="54"/>
       <c r="N54" s="212">
@@ -16787,7 +16928,9 @@
       </c>
       <c r="I55" s="54"/>
       <c r="J55" s="56"/>
-      <c r="K55" s="57"/>
+      <c r="K55" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L55" s="56"/>
       <c r="M55" s="54"/>
       <c r="N55" s="212">
@@ -16842,7 +16985,9 @@
       </c>
       <c r="I56" s="54"/>
       <c r="J56" s="56"/>
-      <c r="K56" s="57"/>
+      <c r="K56" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L56" s="56"/>
       <c r="M56" s="54"/>
       <c r="N56" s="212">
@@ -16877,30 +17022,34 @@
       <c r="B57" s="197">
         <v>51</v>
       </c>
-      <c r="C57" s="54" t="s">
+      <c r="C57" s="194" t="s">
         <v>767</v>
       </c>
-      <c r="D57" s="54" t="s">
+      <c r="D57" s="194" t="s">
         <v>765</v>
       </c>
-      <c r="E57" s="54" t="s">
+      <c r="E57" s="194" t="s">
         <v>766</v>
       </c>
-      <c r="F57" s="54" t="s">
+      <c r="F57" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G57" s="58" t="s">
+      <c r="G57" s="195" t="s">
         <v>627</v>
       </c>
-      <c r="H57" s="54" t="s">
+      <c r="H57" s="194" t="s">
         <v>623</v>
       </c>
-      <c r="I57" s="54"/>
-      <c r="J57" s="56"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="56"/>
-      <c r="M57" s="54"/>
-      <c r="N57" s="54"/>
+      <c r="I57" s="194"/>
+      <c r="J57" s="200"/>
+      <c r="K57" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L57" s="200"/>
+      <c r="M57" s="194"/>
+      <c r="N57" s="212">
+        <v>44755</v>
+      </c>
       <c r="O57" s="54"/>
       <c r="P57" s="56"/>
       <c r="Q57" s="54"/>
@@ -16928,30 +17077,34 @@
       <c r="B58" s="197">
         <v>52</v>
       </c>
-      <c r="C58" s="54" t="s">
+      <c r="C58" s="194" t="s">
         <v>769</v>
       </c>
-      <c r="D58" s="54" t="s">
+      <c r="D58" s="194" t="s">
         <v>765</v>
       </c>
-      <c r="E58" s="54" t="s">
+      <c r="E58" s="194" t="s">
         <v>768</v>
       </c>
-      <c r="F58" s="54" t="s">
+      <c r="F58" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G58" s="58" t="s">
+      <c r="G58" s="195" t="s">
         <v>627</v>
       </c>
-      <c r="H58" s="54" t="s">
+      <c r="H58" s="194" t="s">
         <v>623</v>
       </c>
-      <c r="I58" s="54"/>
-      <c r="J58" s="56"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="54"/>
-      <c r="N58" s="54"/>
+      <c r="I58" s="194"/>
+      <c r="J58" s="200"/>
+      <c r="K58" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L58" s="200"/>
+      <c r="M58" s="194"/>
+      <c r="N58" s="212">
+        <v>44755</v>
+      </c>
       <c r="O58" s="54"/>
       <c r="P58" s="56"/>
       <c r="Q58" s="54"/>
@@ -16979,26 +17132,34 @@
       <c r="B59" s="197">
         <v>53</v>
       </c>
-      <c r="C59" s="54"/>
-      <c r="D59" s="54" t="s">
+      <c r="C59" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D59" s="194" t="s">
         <v>770</v>
       </c>
-      <c r="E59" s="54" t="s">
-        <v>772</v>
-      </c>
-      <c r="F59" s="54" t="s">
+      <c r="E59" s="194" t="s">
+        <v>781</v>
+      </c>
+      <c r="F59" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G59" s="58" t="s">
+      <c r="G59" s="195" t="s">
         <v>627</v>
       </c>
-      <c r="H59" s="54"/>
-      <c r="I59" s="54"/>
-      <c r="J59" s="56"/>
-      <c r="K59" s="57"/>
-      <c r="L59" s="56"/>
-      <c r="M59" s="54"/>
-      <c r="N59" s="54"/>
+      <c r="H59" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I59" s="194"/>
+      <c r="J59" s="200"/>
+      <c r="K59" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L59" s="200"/>
+      <c r="M59" s="194"/>
+      <c r="N59" s="212">
+        <v>44755</v>
+      </c>
       <c r="O59" s="54"/>
       <c r="P59" s="56"/>
       <c r="Q59" s="54"/>
@@ -17026,24 +17187,34 @@
       <c r="B60" s="197">
         <v>54</v>
       </c>
-      <c r="C60" s="54"/>
-      <c r="D60" s="54" t="s">
+      <c r="C60" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D60" s="194" t="s">
         <v>765</v>
       </c>
-      <c r="E60" s="54" t="s">
-        <v>771</v>
-      </c>
-      <c r="F60" s="54" t="s">
+      <c r="E60" s="194" t="s">
+        <v>779</v>
+      </c>
+      <c r="F60" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="54"/>
-      <c r="I60" s="54"/>
-      <c r="J60" s="56"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="54"/>
-      <c r="N60" s="54"/>
+      <c r="G60" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H60" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I60" s="194"/>
+      <c r="J60" s="200"/>
+      <c r="K60" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L60" s="200"/>
+      <c r="M60" s="194"/>
+      <c r="N60" s="212">
+        <v>44755</v>
+      </c>
       <c r="O60" s="54"/>
       <c r="P60" s="56"/>
       <c r="Q60" s="54"/>
@@ -17071,24 +17242,34 @@
       <c r="B61" s="197">
         <v>55</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="54" t="s">
+      <c r="C61" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D61" s="194" t="s">
         <v>765</v>
       </c>
-      <c r="E61" s="54" t="s">
-        <v>773</v>
-      </c>
-      <c r="F61" s="54" t="s">
+      <c r="E61" s="194" t="s">
+        <v>771</v>
+      </c>
+      <c r="F61" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="56"/>
-      <c r="K61" s="57"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="54"/>
-      <c r="N61" s="54"/>
+      <c r="G61" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H61" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I61" s="194"/>
+      <c r="J61" s="200"/>
+      <c r="K61" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L61" s="200"/>
+      <c r="M61" s="194"/>
+      <c r="N61" s="212">
+        <v>44755</v>
+      </c>
       <c r="O61" s="54"/>
       <c r="P61" s="56"/>
       <c r="Q61" s="54"/>
@@ -17116,24 +17297,34 @@
       <c r="B62" s="197">
         <v>56</v>
       </c>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54" t="s">
-        <v>776</v>
-      </c>
-      <c r="E62" s="54" t="s">
-        <v>774</v>
-      </c>
-      <c r="F62" s="54" t="s">
+      <c r="C62" s="194" t="s">
+        <v>782</v>
+      </c>
+      <c r="D62" s="194" t="s">
+        <v>773</v>
+      </c>
+      <c r="E62" s="194" t="s">
+        <v>772</v>
+      </c>
+      <c r="F62" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G62" s="58"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="56"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="56"/>
-      <c r="M62" s="54"/>
-      <c r="N62" s="54"/>
+      <c r="G62" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H62" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I62" s="194"/>
+      <c r="J62" s="200"/>
+      <c r="K62" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L62" s="200"/>
+      <c r="M62" s="194"/>
+      <c r="N62" s="212">
+        <v>44755</v>
+      </c>
       <c r="O62" s="54"/>
       <c r="P62" s="56"/>
       <c r="Q62" s="54"/>
@@ -17161,24 +17352,34 @@
       <c r="B63" s="197">
         <v>57</v>
       </c>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54" t="s">
-        <v>777</v>
-      </c>
-      <c r="E63" s="54" t="s">
-        <v>775</v>
-      </c>
-      <c r="F63" s="54" t="s">
+      <c r="C63" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D63" s="194" t="s">
+        <v>774</v>
+      </c>
+      <c r="E63" s="194" t="s">
+        <v>783</v>
+      </c>
+      <c r="F63" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G63" s="58"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="54"/>
-      <c r="J63" s="56"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="56"/>
-      <c r="M63" s="54"/>
-      <c r="N63" s="54"/>
+      <c r="G63" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H63" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I63" s="194"/>
+      <c r="J63" s="200"/>
+      <c r="K63" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L63" s="200"/>
+      <c r="M63" s="194"/>
+      <c r="N63" s="212">
+        <v>44755</v>
+      </c>
       <c r="O63" s="54"/>
       <c r="P63" s="56"/>
       <c r="Q63" s="54"/>
@@ -17206,24 +17407,34 @@
       <c r="B64" s="197">
         <v>58</v>
       </c>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54" t="s">
+      <c r="C64" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D64" s="194" t="s">
         <v>767</v>
       </c>
-      <c r="E64" s="54" t="s">
-        <v>778</v>
-      </c>
-      <c r="F64" s="54" t="s">
+      <c r="E64" s="194" t="s">
+        <v>775</v>
+      </c>
+      <c r="F64" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G64" s="58"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="54"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="57"/>
-      <c r="L64" s="56"/>
-      <c r="M64" s="54"/>
-      <c r="N64" s="54"/>
+      <c r="G64" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H64" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I64" s="194"/>
+      <c r="J64" s="200"/>
+      <c r="K64" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L64" s="200"/>
+      <c r="M64" s="194"/>
+      <c r="N64" s="212">
+        <v>44755</v>
+      </c>
       <c r="O64" s="54"/>
       <c r="P64" s="56"/>
       <c r="Q64" s="54"/>
@@ -17249,24 +17460,34 @@
       <c r="B65" s="197">
         <v>59</v>
       </c>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54" t="s">
-        <v>780</v>
-      </c>
-      <c r="E65" s="54" t="s">
-        <v>779</v>
-      </c>
-      <c r="F65" s="54" t="s">
+      <c r="C65" s="194" t="s">
+        <v>784</v>
+      </c>
+      <c r="D65" s="194" t="s">
+        <v>785</v>
+      </c>
+      <c r="E65" s="194" t="s">
+        <v>776</v>
+      </c>
+      <c r="F65" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G65" s="58"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="57"/>
-      <c r="L65" s="56"/>
-      <c r="M65" s="54"/>
-      <c r="N65" s="54"/>
+      <c r="G65" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H65" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I65" s="194"/>
+      <c r="J65" s="200"/>
+      <c r="K65" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L65" s="200"/>
+      <c r="M65" s="194"/>
+      <c r="N65" s="212">
+        <v>44755</v>
+      </c>
       <c r="O65" s="54"/>
       <c r="P65" s="56"/>
       <c r="Q65" s="54"/>
@@ -17292,24 +17513,34 @@
       <c r="B66" s="197">
         <v>60</v>
       </c>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54" t="s">
+      <c r="C66" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D66" s="194" t="s">
         <v>698</v>
       </c>
-      <c r="E66" s="54" t="s">
-        <v>781</v>
-      </c>
-      <c r="F66" s="54" t="s">
+      <c r="E66" s="194" t="s">
+        <v>780</v>
+      </c>
+      <c r="F66" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G66" s="58"/>
-      <c r="H66" s="54"/>
-      <c r="I66" s="54"/>
-      <c r="J66" s="56"/>
-      <c r="K66" s="57"/>
-      <c r="L66" s="56"/>
-      <c r="M66" s="54"/>
-      <c r="N66" s="54"/>
+      <c r="G66" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H66" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I66" s="194"/>
+      <c r="J66" s="200"/>
+      <c r="K66" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L66" s="200"/>
+      <c r="M66" s="194"/>
+      <c r="N66" s="212">
+        <v>44755</v>
+      </c>
       <c r="O66" s="54"/>
       <c r="P66" s="56"/>
       <c r="Q66" s="54"/>
@@ -17335,24 +17566,34 @@
       <c r="B67" s="197">
         <v>61</v>
       </c>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54" t="s">
+      <c r="C67" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D67" s="194" t="s">
         <v>698</v>
       </c>
-      <c r="E67" s="54" t="s">
-        <v>782</v>
-      </c>
-      <c r="F67" s="54" t="s">
+      <c r="E67" s="194" t="s">
+        <v>777</v>
+      </c>
+      <c r="F67" s="194" t="s">
         <v>626</v>
       </c>
-      <c r="G67" s="58"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="54"/>
-      <c r="J67" s="56"/>
-      <c r="K67" s="57"/>
-      <c r="L67" s="56"/>
-      <c r="M67" s="54"/>
-      <c r="N67" s="54"/>
+      <c r="G67" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H67" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I67" s="194"/>
+      <c r="J67" s="200"/>
+      <c r="K67" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L67" s="200"/>
+      <c r="M67" s="194"/>
+      <c r="N67" s="212">
+        <v>44755</v>
+      </c>
       <c r="O67" s="54"/>
       <c r="P67" s="56"/>
       <c r="Q67" s="54"/>
@@ -17366,18 +17607,34 @@
       <c r="B68" s="197">
         <v>62</v>
       </c>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="54"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="54"/>
-      <c r="I68" s="54"/>
-      <c r="J68" s="56"/>
-      <c r="K68" s="57"/>
-      <c r="L68" s="56"/>
-      <c r="M68" s="54"/>
-      <c r="N68" s="54"/>
+      <c r="C68" s="194" t="s">
+        <v>786</v>
+      </c>
+      <c r="D68" s="194" t="s">
+        <v>706</v>
+      </c>
+      <c r="E68" s="194" t="s">
+        <v>789</v>
+      </c>
+      <c r="F68" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G68" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H68" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I68" s="194"/>
+      <c r="J68" s="200"/>
+      <c r="K68" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L68" s="200"/>
+      <c r="M68" s="194"/>
+      <c r="N68" s="212">
+        <v>44755</v>
+      </c>
       <c r="O68" s="54"/>
       <c r="P68" s="56"/>
       <c r="Q68" s="54"/>
@@ -17391,18 +17648,34 @@
       <c r="B69" s="197">
         <v>63</v>
       </c>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="54"/>
+      <c r="C69" s="194" t="s">
+        <v>786</v>
+      </c>
+      <c r="D69" s="54" t="s">
+        <v>707</v>
+      </c>
+      <c r="E69" s="54" t="s">
+        <v>789</v>
+      </c>
+      <c r="F69" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G69" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H69" s="194" t="s">
+        <v>623</v>
+      </c>
       <c r="I69" s="54"/>
       <c r="J69" s="56"/>
-      <c r="K69" s="57"/>
+      <c r="K69" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L69" s="56"/>
       <c r="M69" s="54"/>
-      <c r="N69" s="54"/>
+      <c r="N69" s="351">
+        <v>44755</v>
+      </c>
       <c r="O69" s="54"/>
       <c r="P69" s="56"/>
       <c r="Q69" s="54"/>
@@ -17416,18 +17689,34 @@
       <c r="B70" s="197">
         <v>64</v>
       </c>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="54"/>
+      <c r="C70" s="194" t="s">
+        <v>786</v>
+      </c>
+      <c r="D70" s="54" t="s">
+        <v>787</v>
+      </c>
+      <c r="E70" s="54" t="s">
+        <v>789</v>
+      </c>
+      <c r="F70" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G70" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H70" s="194" t="s">
+        <v>623</v>
+      </c>
       <c r="I70" s="54"/>
       <c r="J70" s="56"/>
-      <c r="K70" s="57"/>
+      <c r="K70" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L70" s="56"/>
       <c r="M70" s="54"/>
-      <c r="N70" s="54"/>
+      <c r="N70" s="351">
+        <v>44755</v>
+      </c>
       <c r="O70" s="54"/>
       <c r="P70" s="56"/>
       <c r="Q70" s="54"/>
@@ -17441,18 +17730,34 @@
       <c r="B71" s="197">
         <v>65</v>
       </c>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="54"/>
+      <c r="C71" s="194" t="s">
+        <v>786</v>
+      </c>
+      <c r="D71" s="54" t="s">
+        <v>788</v>
+      </c>
+      <c r="E71" s="54" t="s">
+        <v>789</v>
+      </c>
+      <c r="F71" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G71" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H71" s="194" t="s">
+        <v>623</v>
+      </c>
       <c r="I71" s="54"/>
       <c r="J71" s="56"/>
-      <c r="K71" s="57"/>
+      <c r="K71" s="201" t="s">
+        <v>624</v>
+      </c>
       <c r="L71" s="56"/>
       <c r="M71" s="54"/>
-      <c r="N71" s="54"/>
+      <c r="N71" s="351">
+        <v>44755</v>
+      </c>
       <c r="O71" s="54"/>
       <c r="P71" s="56"/>
       <c r="Q71" s="54"/>
@@ -17466,19 +17771,35 @@
       <c r="B72" s="197">
         <v>66</v>
       </c>
-      <c r="C72" s="54"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="56"/>
-      <c r="K72" s="57"/>
-      <c r="L72" s="56"/>
-      <c r="M72" s="54"/>
-      <c r="N72" s="54"/>
-      <c r="O72" s="54"/>
+      <c r="C72" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D72" s="194" t="s">
+        <v>706</v>
+      </c>
+      <c r="E72" s="194" t="s">
+        <v>790</v>
+      </c>
+      <c r="F72" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G72" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H72" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I72" s="194"/>
+      <c r="J72" s="200"/>
+      <c r="K72" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L72" s="200"/>
+      <c r="M72" s="194"/>
+      <c r="N72" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O72" s="194"/>
       <c r="P72" s="56"/>
       <c r="Q72" s="54"/>
       <c r="R72" s="54"/>
@@ -17491,19 +17812,35 @@
       <c r="B73" s="197">
         <v>67</v>
       </c>
-      <c r="C73" s="54"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="56"/>
-      <c r="K73" s="57"/>
-      <c r="L73" s="56"/>
-      <c r="M73" s="54"/>
-      <c r="N73" s="54"/>
-      <c r="O73" s="54"/>
+      <c r="C73" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D73" s="194" t="s">
+        <v>707</v>
+      </c>
+      <c r="E73" s="194" t="s">
+        <v>791</v>
+      </c>
+      <c r="F73" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G73" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H73" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I73" s="194"/>
+      <c r="J73" s="200"/>
+      <c r="K73" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L73" s="200"/>
+      <c r="M73" s="194"/>
+      <c r="N73" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O73" s="194"/>
       <c r="P73" s="56"/>
       <c r="Q73" s="54"/>
       <c r="R73" s="54"/>
@@ -17516,19 +17853,35 @@
       <c r="B74" s="197">
         <v>68</v>
       </c>
-      <c r="C74" s="54"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="54"/>
-      <c r="F74" s="54"/>
-      <c r="G74" s="58"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="56"/>
-      <c r="K74" s="57"/>
-      <c r="L74" s="56"/>
-      <c r="M74" s="54"/>
-      <c r="N74" s="54"/>
-      <c r="O74" s="54"/>
+      <c r="C74" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D74" s="194" t="s">
+        <v>787</v>
+      </c>
+      <c r="E74" s="194" t="s">
+        <v>792</v>
+      </c>
+      <c r="F74" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G74" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H74" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I74" s="194"/>
+      <c r="J74" s="200"/>
+      <c r="K74" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L74" s="200"/>
+      <c r="M74" s="194"/>
+      <c r="N74" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O74" s="194"/>
       <c r="P74" s="56"/>
       <c r="Q74" s="54"/>
       <c r="R74" s="54"/>
@@ -17541,19 +17894,35 @@
       <c r="B75" s="197">
         <v>69</v>
       </c>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="54"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="54"/>
-      <c r="J75" s="56"/>
-      <c r="K75" s="57"/>
-      <c r="L75" s="56"/>
-      <c r="M75" s="54"/>
-      <c r="N75" s="54"/>
-      <c r="O75" s="54"/>
+      <c r="C75" s="194" t="s">
+        <v>699</v>
+      </c>
+      <c r="D75" s="194" t="s">
+        <v>788</v>
+      </c>
+      <c r="E75" s="194" t="s">
+        <v>793</v>
+      </c>
+      <c r="F75" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G75" s="195" t="s">
+        <v>627</v>
+      </c>
+      <c r="H75" s="194" t="s">
+        <v>623</v>
+      </c>
+      <c r="I75" s="194"/>
+      <c r="J75" s="200"/>
+      <c r="K75" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L75" s="200"/>
+      <c r="M75" s="194"/>
+      <c r="N75" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O75" s="194"/>
       <c r="P75" s="56"/>
       <c r="Q75" s="54"/>
       <c r="R75" s="54"/>
@@ -17566,19 +17935,35 @@
       <c r="B76" s="197">
         <v>70</v>
       </c>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="54"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="58"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="54"/>
-      <c r="J76" s="56"/>
-      <c r="K76" s="57"/>
-      <c r="L76" s="56"/>
-      <c r="M76" s="54"/>
-      <c r="N76" s="54"/>
-      <c r="O76" s="54"/>
+      <c r="C76" s="194" t="s">
+        <v>762</v>
+      </c>
+      <c r="D76" s="194" t="s">
+        <v>706</v>
+      </c>
+      <c r="E76" s="194" t="s">
+        <v>797</v>
+      </c>
+      <c r="F76" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G76" s="195" t="s">
+        <v>631</v>
+      </c>
+      <c r="H76" s="194" t="s">
+        <v>632</v>
+      </c>
+      <c r="I76" s="194"/>
+      <c r="J76" s="200"/>
+      <c r="K76" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L76" s="200"/>
+      <c r="M76" s="194"/>
+      <c r="N76" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O76" s="194"/>
       <c r="P76" s="56"/>
       <c r="Q76" s="54"/>
       <c r="R76" s="54"/>
@@ -17588,20 +17973,38 @@
       <c r="AO76" s="60"/>
     </row>
     <row r="77" spans="2:50" x14ac:dyDescent="0.2">
-      <c r="B77" s="59"/>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
-      <c r="E77" s="54"/>
-      <c r="F77" s="54"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="54"/>
-      <c r="I77" s="54"/>
-      <c r="J77" s="56"/>
-      <c r="K77" s="57"/>
-      <c r="L77" s="56"/>
-      <c r="M77" s="54"/>
-      <c r="N77" s="54"/>
-      <c r="O77" s="54"/>
+      <c r="B77" s="197">
+        <v>71</v>
+      </c>
+      <c r="C77" s="194" t="s">
+        <v>762</v>
+      </c>
+      <c r="D77" s="194" t="s">
+        <v>707</v>
+      </c>
+      <c r="E77" s="194" t="s">
+        <v>796</v>
+      </c>
+      <c r="F77" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G77" s="195" t="s">
+        <v>631</v>
+      </c>
+      <c r="H77" s="194" t="s">
+        <v>632</v>
+      </c>
+      <c r="I77" s="194"/>
+      <c r="J77" s="200"/>
+      <c r="K77" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L77" s="200"/>
+      <c r="M77" s="194"/>
+      <c r="N77" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O77" s="194"/>
       <c r="P77" s="56"/>
       <c r="Q77" s="54"/>
       <c r="R77" s="54"/>
@@ -17611,20 +18014,38 @@
       <c r="AO77" s="60"/>
     </row>
     <row r="78" spans="2:50" x14ac:dyDescent="0.2">
-      <c r="B78" s="59"/>
-      <c r="C78" s="54"/>
-      <c r="D78" s="54"/>
-      <c r="E78" s="54"/>
-      <c r="F78" s="54"/>
-      <c r="G78" s="58"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
-      <c r="J78" s="56"/>
-      <c r="K78" s="57"/>
-      <c r="L78" s="56"/>
-      <c r="M78" s="54"/>
-      <c r="N78" s="54"/>
-      <c r="O78" s="54"/>
+      <c r="B78" s="197">
+        <v>72</v>
+      </c>
+      <c r="C78" s="194" t="s">
+        <v>762</v>
+      </c>
+      <c r="D78" s="194" t="s">
+        <v>787</v>
+      </c>
+      <c r="E78" s="194" t="s">
+        <v>795</v>
+      </c>
+      <c r="F78" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G78" s="195" t="s">
+        <v>631</v>
+      </c>
+      <c r="H78" s="194" t="s">
+        <v>632</v>
+      </c>
+      <c r="I78" s="194"/>
+      <c r="J78" s="200"/>
+      <c r="K78" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L78" s="200"/>
+      <c r="M78" s="194"/>
+      <c r="N78" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O78" s="194"/>
       <c r="P78" s="56"/>
       <c r="Q78" s="54"/>
       <c r="R78" s="54"/>
@@ -17634,20 +18055,38 @@
       <c r="AO78" s="60"/>
     </row>
     <row r="79" spans="2:50" x14ac:dyDescent="0.2">
-      <c r="B79" s="59"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54"/>
-      <c r="F79" s="54"/>
-      <c r="G79" s="58"/>
-      <c r="H79" s="54"/>
-      <c r="I79" s="54"/>
-      <c r="J79" s="56"/>
-      <c r="K79" s="57"/>
-      <c r="L79" s="56"/>
-      <c r="M79" s="54"/>
-      <c r="N79" s="54"/>
-      <c r="O79" s="54"/>
+      <c r="B79" s="197">
+        <v>73</v>
+      </c>
+      <c r="C79" s="194" t="s">
+        <v>762</v>
+      </c>
+      <c r="D79" s="194" t="s">
+        <v>788</v>
+      </c>
+      <c r="E79" s="194" t="s">
+        <v>794</v>
+      </c>
+      <c r="F79" s="194" t="s">
+        <v>626</v>
+      </c>
+      <c r="G79" s="195" t="s">
+        <v>631</v>
+      </c>
+      <c r="H79" s="194" t="s">
+        <v>632</v>
+      </c>
+      <c r="I79" s="194"/>
+      <c r="J79" s="200"/>
+      <c r="K79" s="201" t="s">
+        <v>624</v>
+      </c>
+      <c r="L79" s="200"/>
+      <c r="M79" s="194"/>
+      <c r="N79" s="212">
+        <v>44755</v>
+      </c>
+      <c r="O79" s="194"/>
       <c r="P79" s="56"/>
       <c r="Q79" s="54"/>
       <c r="R79" s="54"/>
@@ -17657,7 +18096,9 @@
       <c r="AO79" s="60"/>
     </row>
     <row r="80" spans="2:50" x14ac:dyDescent="0.2">
-      <c r="B80" s="59"/>
+      <c r="B80" s="197">
+        <v>74</v>
+      </c>
       <c r="C80" s="54"/>
       <c r="D80" s="54"/>
       <c r="E80" s="54"/>
@@ -17680,7 +18121,9 @@
       <c r="AO80" s="60"/>
     </row>
     <row r="81" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B81" s="59"/>
+      <c r="B81" s="197">
+        <v>75</v>
+      </c>
       <c r="C81" s="54"/>
       <c r="D81" s="54"/>
       <c r="E81" s="54"/>
@@ -17703,7 +18146,9 @@
       <c r="AO81" s="60"/>
     </row>
     <row r="82" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B82" s="59"/>
+      <c r="B82" s="197">
+        <v>76</v>
+      </c>
       <c r="C82" s="54"/>
       <c r="D82" s="54"/>
       <c r="E82" s="54"/>
@@ -17726,7 +18171,9 @@
       <c r="AO82" s="60"/>
     </row>
     <row r="83" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B83" s="59"/>
+      <c r="B83" s="197">
+        <v>77</v>
+      </c>
       <c r="C83" s="54"/>
       <c r="D83" s="54"/>
       <c r="E83" s="54"/>
@@ -17749,7 +18196,9 @@
       <c r="AO83" s="60"/>
     </row>
     <row r="84" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B84" s="59"/>
+      <c r="B84" s="197">
+        <v>78</v>
+      </c>
       <c r="C84" s="54"/>
       <c r="D84" s="54"/>
       <c r="E84" s="54"/>
@@ -17772,7 +18221,9 @@
       <c r="AO84" s="60"/>
     </row>
     <row r="85" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B85" s="59"/>
+      <c r="B85" s="197">
+        <v>79</v>
+      </c>
       <c r="C85" s="54"/>
       <c r="D85" s="54"/>
       <c r="E85" s="54"/>
@@ -17795,7 +18246,9 @@
       <c r="AO85" s="60"/>
     </row>
     <row r="86" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="B86" s="59"/>
+      <c r="B86" s="197">
+        <v>80</v>
+      </c>
       <c r="C86" s="54"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
@@ -19469,7 +19922,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:P159 WVX983047:WVX983199 WMB983047:WMB983199 WCF983047:WCF983199 VSJ983047:VSJ983199 VIN983047:VIN983199 UYR983047:UYR983199 UOV983047:UOV983199 UEZ983047:UEZ983199 TVD983047:TVD983199 TLH983047:TLH983199 TBL983047:TBL983199 SRP983047:SRP983199 SHT983047:SHT983199 RXX983047:RXX983199 ROB983047:ROB983199 REF983047:REF983199 QUJ983047:QUJ983199 QKN983047:QKN983199 QAR983047:QAR983199 PQV983047:PQV983199 PGZ983047:PGZ983199 OXD983047:OXD983199 ONH983047:ONH983199 ODL983047:ODL983199 NTP983047:NTP983199 NJT983047:NJT983199 MZX983047:MZX983199 MQB983047:MQB983199 MGF983047:MGF983199 LWJ983047:LWJ983199 LMN983047:LMN983199 LCR983047:LCR983199 KSV983047:KSV983199 KIZ983047:KIZ983199 JZD983047:JZD983199 JPH983047:JPH983199 JFL983047:JFL983199 IVP983047:IVP983199 ILT983047:ILT983199 IBX983047:IBX983199 HSB983047:HSB983199 HIF983047:HIF983199 GYJ983047:GYJ983199 GON983047:GON983199 GER983047:GER983199 FUV983047:FUV983199 FKZ983047:FKZ983199 FBD983047:FBD983199 ERH983047:ERH983199 EHL983047:EHL983199 DXP983047:DXP983199 DNT983047:DNT983199 DDX983047:DDX983199 CUB983047:CUB983199 CKF983047:CKF983199 CAJ983047:CAJ983199 BQN983047:BQN983199 BGR983047:BGR983199 AWV983047:AWV983199 AMZ983047:AMZ983199 ADD983047:ADD983199 TH983047:TH983199 JL983047:JL983199 P983047:P983199 WVX917511:WVX917663 WMB917511:WMB917663 WCF917511:WCF917663 VSJ917511:VSJ917663 VIN917511:VIN917663 UYR917511:UYR917663 UOV917511:UOV917663 UEZ917511:UEZ917663 TVD917511:TVD917663 TLH917511:TLH917663 TBL917511:TBL917663 SRP917511:SRP917663 SHT917511:SHT917663 RXX917511:RXX917663 ROB917511:ROB917663 REF917511:REF917663 QUJ917511:QUJ917663 QKN917511:QKN917663 QAR917511:QAR917663 PQV917511:PQV917663 PGZ917511:PGZ917663 OXD917511:OXD917663 ONH917511:ONH917663 ODL917511:ODL917663 NTP917511:NTP917663 NJT917511:NJT917663 MZX917511:MZX917663 MQB917511:MQB917663 MGF917511:MGF917663 LWJ917511:LWJ917663 LMN917511:LMN917663 LCR917511:LCR917663 KSV917511:KSV917663 KIZ917511:KIZ917663 JZD917511:JZD917663 JPH917511:JPH917663 JFL917511:JFL917663 IVP917511:IVP917663 ILT917511:ILT917663 IBX917511:IBX917663 HSB917511:HSB917663 HIF917511:HIF917663 GYJ917511:GYJ917663 GON917511:GON917663 GER917511:GER917663 FUV917511:FUV917663 FKZ917511:FKZ917663 FBD917511:FBD917663 ERH917511:ERH917663 EHL917511:EHL917663 DXP917511:DXP917663 DNT917511:DNT917663 DDX917511:DDX917663 CUB917511:CUB917663 CKF917511:CKF917663 CAJ917511:CAJ917663 BQN917511:BQN917663 BGR917511:BGR917663 AWV917511:AWV917663 AMZ917511:AMZ917663 ADD917511:ADD917663 TH917511:TH917663 JL917511:JL917663 P917511:P917663 WVX851975:WVX852127 WMB851975:WMB852127 WCF851975:WCF852127 VSJ851975:VSJ852127 VIN851975:VIN852127 UYR851975:UYR852127 UOV851975:UOV852127 UEZ851975:UEZ852127 TVD851975:TVD852127 TLH851975:TLH852127 TBL851975:TBL852127 SRP851975:SRP852127 SHT851975:SHT852127 RXX851975:RXX852127 ROB851975:ROB852127 REF851975:REF852127 QUJ851975:QUJ852127 QKN851975:QKN852127 QAR851975:QAR852127 PQV851975:PQV852127 PGZ851975:PGZ852127 OXD851975:OXD852127 ONH851975:ONH852127 ODL851975:ODL852127 NTP851975:NTP852127 NJT851975:NJT852127 MZX851975:MZX852127 MQB851975:MQB852127 MGF851975:MGF852127 LWJ851975:LWJ852127 LMN851975:LMN852127 LCR851975:LCR852127 KSV851975:KSV852127 KIZ851975:KIZ852127 JZD851975:JZD852127 JPH851975:JPH852127 JFL851975:JFL852127 IVP851975:IVP852127 ILT851975:ILT852127 IBX851975:IBX852127 HSB851975:HSB852127 HIF851975:HIF852127 GYJ851975:GYJ852127 GON851975:GON852127 GER851975:GER852127 FUV851975:FUV852127 FKZ851975:FKZ852127 FBD851975:FBD852127 ERH851975:ERH852127 EHL851975:EHL852127 DXP851975:DXP852127 DNT851975:DNT852127 DDX851975:DDX852127 CUB851975:CUB852127 CKF851975:CKF852127 CAJ851975:CAJ852127 BQN851975:BQN852127 BGR851975:BGR852127 AWV851975:AWV852127 AMZ851975:AMZ852127 ADD851975:ADD852127 TH851975:TH852127 JL851975:JL852127 P851975:P852127 WVX786439:WVX786591 WMB786439:WMB786591 WCF786439:WCF786591 VSJ786439:VSJ786591 VIN786439:VIN786591 UYR786439:UYR786591 UOV786439:UOV786591 UEZ786439:UEZ786591 TVD786439:TVD786591 TLH786439:TLH786591 TBL786439:TBL786591 SRP786439:SRP786591 SHT786439:SHT786591 RXX786439:RXX786591 ROB786439:ROB786591 REF786439:REF786591 QUJ786439:QUJ786591 QKN786439:QKN786591 QAR786439:QAR786591 PQV786439:PQV786591 PGZ786439:PGZ786591 OXD786439:OXD786591 ONH786439:ONH786591 ODL786439:ODL786591 NTP786439:NTP786591 NJT786439:NJT786591 MZX786439:MZX786591 MQB786439:MQB786591 MGF786439:MGF786591 LWJ786439:LWJ786591 LMN786439:LMN786591 LCR786439:LCR786591 KSV786439:KSV786591 KIZ786439:KIZ786591 JZD786439:JZD786591 JPH786439:JPH786591 JFL786439:JFL786591 IVP786439:IVP786591 ILT786439:ILT786591 IBX786439:IBX786591 HSB786439:HSB786591 HIF786439:HIF786591 GYJ786439:GYJ786591 GON786439:GON786591 GER786439:GER786591 FUV786439:FUV786591 FKZ786439:FKZ786591 FBD786439:FBD786591 ERH786439:ERH786591 EHL786439:EHL786591 DXP786439:DXP786591 DNT786439:DNT786591 DDX786439:DDX786591 CUB786439:CUB786591 CKF786439:CKF786591 CAJ786439:CAJ786591 BQN786439:BQN786591 BGR786439:BGR786591 AWV786439:AWV786591 AMZ786439:AMZ786591 ADD786439:ADD786591 TH786439:TH786591 JL786439:JL786591 P786439:P786591 WVX720903:WVX721055 WMB720903:WMB721055 WCF720903:WCF721055 VSJ720903:VSJ721055 VIN720903:VIN721055 UYR720903:UYR721055 UOV720903:UOV721055 UEZ720903:UEZ721055 TVD720903:TVD721055 TLH720903:TLH721055 TBL720903:TBL721055 SRP720903:SRP721055 SHT720903:SHT721055 RXX720903:RXX721055 ROB720903:ROB721055 REF720903:REF721055 QUJ720903:QUJ721055 QKN720903:QKN721055 QAR720903:QAR721055 PQV720903:PQV721055 PGZ720903:PGZ721055 OXD720903:OXD721055 ONH720903:ONH721055 ODL720903:ODL721055 NTP720903:NTP721055 NJT720903:NJT721055 MZX720903:MZX721055 MQB720903:MQB721055 MGF720903:MGF721055 LWJ720903:LWJ721055 LMN720903:LMN721055 LCR720903:LCR721055 KSV720903:KSV721055 KIZ720903:KIZ721055 JZD720903:JZD721055 JPH720903:JPH721055 JFL720903:JFL721055 IVP720903:IVP721055 ILT720903:ILT721055 IBX720903:IBX721055 HSB720903:HSB721055 HIF720903:HIF721055 GYJ720903:GYJ721055 GON720903:GON721055 GER720903:GER721055 FUV720903:FUV721055 FKZ720903:FKZ721055 FBD720903:FBD721055 ERH720903:ERH721055 EHL720903:EHL721055 DXP720903:DXP721055 DNT720903:DNT721055 DDX720903:DDX721055 CUB720903:CUB721055 CKF720903:CKF721055 CAJ720903:CAJ721055 BQN720903:BQN721055 BGR720903:BGR721055 AWV720903:AWV721055 AMZ720903:AMZ721055 ADD720903:ADD721055 TH720903:TH721055 JL720903:JL721055 P720903:P721055 WVX655367:WVX655519 WMB655367:WMB655519 WCF655367:WCF655519 VSJ655367:VSJ655519 VIN655367:VIN655519 UYR655367:UYR655519 UOV655367:UOV655519 UEZ655367:UEZ655519 TVD655367:TVD655519 TLH655367:TLH655519 TBL655367:TBL655519 SRP655367:SRP655519 SHT655367:SHT655519 RXX655367:RXX655519 ROB655367:ROB655519 REF655367:REF655519 QUJ655367:QUJ655519 QKN655367:QKN655519 QAR655367:QAR655519 PQV655367:PQV655519 PGZ655367:PGZ655519 OXD655367:OXD655519 ONH655367:ONH655519 ODL655367:ODL655519 NTP655367:NTP655519 NJT655367:NJT655519 MZX655367:MZX655519 MQB655367:MQB655519 MGF655367:MGF655519 LWJ655367:LWJ655519 LMN655367:LMN655519 LCR655367:LCR655519 KSV655367:KSV655519 KIZ655367:KIZ655519 JZD655367:JZD655519 JPH655367:JPH655519 JFL655367:JFL655519 IVP655367:IVP655519 ILT655367:ILT655519 IBX655367:IBX655519 HSB655367:HSB655519 HIF655367:HIF655519 GYJ655367:GYJ655519 GON655367:GON655519 GER655367:GER655519 FUV655367:FUV655519 FKZ655367:FKZ655519 FBD655367:FBD655519 ERH655367:ERH655519 EHL655367:EHL655519 DXP655367:DXP655519 DNT655367:DNT655519 DDX655367:DDX655519 CUB655367:CUB655519 CKF655367:CKF655519 CAJ655367:CAJ655519 BQN655367:BQN655519 BGR655367:BGR655519 AWV655367:AWV655519 AMZ655367:AMZ655519 ADD655367:ADD655519 TH655367:TH655519 JL655367:JL655519 P655367:P655519 WVX589831:WVX589983 WMB589831:WMB589983 WCF589831:WCF589983 VSJ589831:VSJ589983 VIN589831:VIN589983 UYR589831:UYR589983 UOV589831:UOV589983 UEZ589831:UEZ589983 TVD589831:TVD589983 TLH589831:TLH589983 TBL589831:TBL589983 SRP589831:SRP589983 SHT589831:SHT589983 RXX589831:RXX589983 ROB589831:ROB589983 REF589831:REF589983 QUJ589831:QUJ589983 QKN589831:QKN589983 QAR589831:QAR589983 PQV589831:PQV589983 PGZ589831:PGZ589983 OXD589831:OXD589983 ONH589831:ONH589983 ODL589831:ODL589983 NTP589831:NTP589983 NJT589831:NJT589983 MZX589831:MZX589983 MQB589831:MQB589983 MGF589831:MGF589983 LWJ589831:LWJ589983 LMN589831:LMN589983 LCR589831:LCR589983 KSV589831:KSV589983 KIZ589831:KIZ589983 JZD589831:JZD589983 JPH589831:JPH589983 JFL589831:JFL589983 IVP589831:IVP589983 ILT589831:ILT589983 IBX589831:IBX589983 HSB589831:HSB589983 HIF589831:HIF589983 GYJ589831:GYJ589983 GON589831:GON589983 GER589831:GER589983 FUV589831:FUV589983 FKZ589831:FKZ589983 FBD589831:FBD589983 ERH589831:ERH589983 EHL589831:EHL589983 DXP589831:DXP589983 DNT589831:DNT589983 DDX589831:DDX589983 CUB589831:CUB589983 CKF589831:CKF589983 CAJ589831:CAJ589983 BQN589831:BQN589983 BGR589831:BGR589983 AWV589831:AWV589983 AMZ589831:AMZ589983 ADD589831:ADD589983 TH589831:TH589983 JL589831:JL589983 P589831:P589983 WVX524295:WVX524447 WMB524295:WMB524447 WCF524295:WCF524447 VSJ524295:VSJ524447 VIN524295:VIN524447 UYR524295:UYR524447 UOV524295:UOV524447 UEZ524295:UEZ524447 TVD524295:TVD524447 TLH524295:TLH524447 TBL524295:TBL524447 SRP524295:SRP524447 SHT524295:SHT524447 RXX524295:RXX524447 ROB524295:ROB524447 REF524295:REF524447 QUJ524295:QUJ524447 QKN524295:QKN524447 QAR524295:QAR524447 PQV524295:PQV524447 PGZ524295:PGZ524447 OXD524295:OXD524447 ONH524295:ONH524447 ODL524295:ODL524447 NTP524295:NTP524447 NJT524295:NJT524447 MZX524295:MZX524447 MQB524295:MQB524447 MGF524295:MGF524447 LWJ524295:LWJ524447 LMN524295:LMN524447 LCR524295:LCR524447 KSV524295:KSV524447 KIZ524295:KIZ524447 JZD524295:JZD524447 JPH524295:JPH524447 JFL524295:JFL524447 IVP524295:IVP524447 ILT524295:ILT524447 IBX524295:IBX524447 HSB524295:HSB524447 HIF524295:HIF524447 GYJ524295:GYJ524447 GON524295:GON524447 GER524295:GER524447 FUV524295:FUV524447 FKZ524295:FKZ524447 FBD524295:FBD524447 ERH524295:ERH524447 EHL524295:EHL524447 DXP524295:DXP524447 DNT524295:DNT524447 DDX524295:DDX524447 CUB524295:CUB524447 CKF524295:CKF524447 CAJ524295:CAJ524447 BQN524295:BQN524447 BGR524295:BGR524447 AWV524295:AWV524447 AMZ524295:AMZ524447 ADD524295:ADD524447 TH524295:TH524447 JL524295:JL524447 P524295:P524447 WVX458759:WVX458911 WMB458759:WMB458911 WCF458759:WCF458911 VSJ458759:VSJ458911 VIN458759:VIN458911 UYR458759:UYR458911 UOV458759:UOV458911 UEZ458759:UEZ458911 TVD458759:TVD458911 TLH458759:TLH458911 TBL458759:TBL458911 SRP458759:SRP458911 SHT458759:SHT458911 RXX458759:RXX458911 ROB458759:ROB458911 REF458759:REF458911 QUJ458759:QUJ458911 QKN458759:QKN458911 QAR458759:QAR458911 PQV458759:PQV458911 PGZ458759:PGZ458911 OXD458759:OXD458911 ONH458759:ONH458911 ODL458759:ODL458911 NTP458759:NTP458911 NJT458759:NJT458911 MZX458759:MZX458911 MQB458759:MQB458911 MGF458759:MGF458911 LWJ458759:LWJ458911 LMN458759:LMN458911 LCR458759:LCR458911 KSV458759:KSV458911 KIZ458759:KIZ458911 JZD458759:JZD458911 JPH458759:JPH458911 JFL458759:JFL458911 IVP458759:IVP458911 ILT458759:ILT458911 IBX458759:IBX458911 HSB458759:HSB458911 HIF458759:HIF458911 GYJ458759:GYJ458911 GON458759:GON458911 GER458759:GER458911 FUV458759:FUV458911 FKZ458759:FKZ458911 FBD458759:FBD458911 ERH458759:ERH458911 EHL458759:EHL458911 DXP458759:DXP458911 DNT458759:DNT458911 DDX458759:DDX458911 CUB458759:CUB458911 CKF458759:CKF458911 CAJ458759:CAJ458911 BQN458759:BQN458911 BGR458759:BGR458911 AWV458759:AWV458911 AMZ458759:AMZ458911 ADD458759:ADD458911 TH458759:TH458911 JL458759:JL458911 P458759:P458911 WVX393223:WVX393375 WMB393223:WMB393375 WCF393223:WCF393375 VSJ393223:VSJ393375 VIN393223:VIN393375 UYR393223:UYR393375 UOV393223:UOV393375 UEZ393223:UEZ393375 TVD393223:TVD393375 TLH393223:TLH393375 TBL393223:TBL393375 SRP393223:SRP393375 SHT393223:SHT393375 RXX393223:RXX393375 ROB393223:ROB393375 REF393223:REF393375 QUJ393223:QUJ393375 QKN393223:QKN393375 QAR393223:QAR393375 PQV393223:PQV393375 PGZ393223:PGZ393375 OXD393223:OXD393375 ONH393223:ONH393375 ODL393223:ODL393375 NTP393223:NTP393375 NJT393223:NJT393375 MZX393223:MZX393375 MQB393223:MQB393375 MGF393223:MGF393375 LWJ393223:LWJ393375 LMN393223:LMN393375 LCR393223:LCR393375 KSV393223:KSV393375 KIZ393223:KIZ393375 JZD393223:JZD393375 JPH393223:JPH393375 JFL393223:JFL393375 IVP393223:IVP393375 ILT393223:ILT393375 IBX393223:IBX393375 HSB393223:HSB393375 HIF393223:HIF393375 GYJ393223:GYJ393375 GON393223:GON393375 GER393223:GER393375 FUV393223:FUV393375 FKZ393223:FKZ393375 FBD393223:FBD393375 ERH393223:ERH393375 EHL393223:EHL393375 DXP393223:DXP393375 DNT393223:DNT393375 DDX393223:DDX393375 CUB393223:CUB393375 CKF393223:CKF393375 CAJ393223:CAJ393375 BQN393223:BQN393375 BGR393223:BGR393375 AWV393223:AWV393375 AMZ393223:AMZ393375 ADD393223:ADD393375 TH393223:TH393375 JL393223:JL393375 P393223:P393375 WVX327687:WVX327839 WMB327687:WMB327839 WCF327687:WCF327839 VSJ327687:VSJ327839 VIN327687:VIN327839 UYR327687:UYR327839 UOV327687:UOV327839 UEZ327687:UEZ327839 TVD327687:TVD327839 TLH327687:TLH327839 TBL327687:TBL327839 SRP327687:SRP327839 SHT327687:SHT327839 RXX327687:RXX327839 ROB327687:ROB327839 REF327687:REF327839 QUJ327687:QUJ327839 QKN327687:QKN327839 QAR327687:QAR327839 PQV327687:PQV327839 PGZ327687:PGZ327839 OXD327687:OXD327839 ONH327687:ONH327839 ODL327687:ODL327839 NTP327687:NTP327839 NJT327687:NJT327839 MZX327687:MZX327839 MQB327687:MQB327839 MGF327687:MGF327839 LWJ327687:LWJ327839 LMN327687:LMN327839 LCR327687:LCR327839 KSV327687:KSV327839 KIZ327687:KIZ327839 JZD327687:JZD327839 JPH327687:JPH327839 JFL327687:JFL327839 IVP327687:IVP327839 ILT327687:ILT327839 IBX327687:IBX327839 HSB327687:HSB327839 HIF327687:HIF327839 GYJ327687:GYJ327839 GON327687:GON327839 GER327687:GER327839 FUV327687:FUV327839 FKZ327687:FKZ327839 FBD327687:FBD327839 ERH327687:ERH327839 EHL327687:EHL327839 DXP327687:DXP327839 DNT327687:DNT327839 DDX327687:DDX327839 CUB327687:CUB327839 CKF327687:CKF327839 CAJ327687:CAJ327839 BQN327687:BQN327839 BGR327687:BGR327839 AWV327687:AWV327839 AMZ327687:AMZ327839 ADD327687:ADD327839 TH327687:TH327839 JL327687:JL327839 P327687:P327839 WVX262151:WVX262303 WMB262151:WMB262303 WCF262151:WCF262303 VSJ262151:VSJ262303 VIN262151:VIN262303 UYR262151:UYR262303 UOV262151:UOV262303 UEZ262151:UEZ262303 TVD262151:TVD262303 TLH262151:TLH262303 TBL262151:TBL262303 SRP262151:SRP262303 SHT262151:SHT262303 RXX262151:RXX262303 ROB262151:ROB262303 REF262151:REF262303 QUJ262151:QUJ262303 QKN262151:QKN262303 QAR262151:QAR262303 PQV262151:PQV262303 PGZ262151:PGZ262303 OXD262151:OXD262303 ONH262151:ONH262303 ODL262151:ODL262303 NTP262151:NTP262303 NJT262151:NJT262303 MZX262151:MZX262303 MQB262151:MQB262303 MGF262151:MGF262303 LWJ262151:LWJ262303 LMN262151:LMN262303 LCR262151:LCR262303 KSV262151:KSV262303 KIZ262151:KIZ262303 JZD262151:JZD262303 JPH262151:JPH262303 JFL262151:JFL262303 IVP262151:IVP262303 ILT262151:ILT262303 IBX262151:IBX262303 HSB262151:HSB262303 HIF262151:HIF262303 GYJ262151:GYJ262303 GON262151:GON262303 GER262151:GER262303 FUV262151:FUV262303 FKZ262151:FKZ262303 FBD262151:FBD262303 ERH262151:ERH262303 EHL262151:EHL262303 DXP262151:DXP262303 DNT262151:DNT262303 DDX262151:DDX262303 CUB262151:CUB262303 CKF262151:CKF262303 CAJ262151:CAJ262303 BQN262151:BQN262303 BGR262151:BGR262303 AWV262151:AWV262303 AMZ262151:AMZ262303 ADD262151:ADD262303 TH262151:TH262303 JL262151:JL262303 P262151:P262303 WVX196615:WVX196767 WMB196615:WMB196767 WCF196615:WCF196767 VSJ196615:VSJ196767 VIN196615:VIN196767 UYR196615:UYR196767 UOV196615:UOV196767 UEZ196615:UEZ196767 TVD196615:TVD196767 TLH196615:TLH196767 TBL196615:TBL196767 SRP196615:SRP196767 SHT196615:SHT196767 RXX196615:RXX196767 ROB196615:ROB196767 REF196615:REF196767 QUJ196615:QUJ196767 QKN196615:QKN196767 QAR196615:QAR196767 PQV196615:PQV196767 PGZ196615:PGZ196767 OXD196615:OXD196767 ONH196615:ONH196767 ODL196615:ODL196767 NTP196615:NTP196767 NJT196615:NJT196767 MZX196615:MZX196767 MQB196615:MQB196767 MGF196615:MGF196767 LWJ196615:LWJ196767 LMN196615:LMN196767 LCR196615:LCR196767 KSV196615:KSV196767 KIZ196615:KIZ196767 JZD196615:JZD196767 JPH196615:JPH196767 JFL196615:JFL196767 IVP196615:IVP196767 ILT196615:ILT196767 IBX196615:IBX196767 HSB196615:HSB196767 HIF196615:HIF196767 GYJ196615:GYJ196767 GON196615:GON196767 GER196615:GER196767 FUV196615:FUV196767 FKZ196615:FKZ196767 FBD196615:FBD196767 ERH196615:ERH196767 EHL196615:EHL196767 DXP196615:DXP196767 DNT196615:DNT196767 DDX196615:DDX196767 CUB196615:CUB196767 CKF196615:CKF196767 CAJ196615:CAJ196767 BQN196615:BQN196767 BGR196615:BGR196767 AWV196615:AWV196767 AMZ196615:AMZ196767 ADD196615:ADD196767 TH196615:TH196767 JL196615:JL196767 P196615:P196767 WVX131079:WVX131231 WMB131079:WMB131231 WCF131079:WCF131231 VSJ131079:VSJ131231 VIN131079:VIN131231 UYR131079:UYR131231 UOV131079:UOV131231 UEZ131079:UEZ131231 TVD131079:TVD131231 TLH131079:TLH131231 TBL131079:TBL131231 SRP131079:SRP131231 SHT131079:SHT131231 RXX131079:RXX131231 ROB131079:ROB131231 REF131079:REF131231 QUJ131079:QUJ131231 QKN131079:QKN131231 QAR131079:QAR131231 PQV131079:PQV131231 PGZ131079:PGZ131231 OXD131079:OXD131231 ONH131079:ONH131231 ODL131079:ODL131231 NTP131079:NTP131231 NJT131079:NJT131231 MZX131079:MZX131231 MQB131079:MQB131231 MGF131079:MGF131231 LWJ131079:LWJ131231 LMN131079:LMN131231 LCR131079:LCR131231 KSV131079:KSV131231 KIZ131079:KIZ131231 JZD131079:JZD131231 JPH131079:JPH131231 JFL131079:JFL131231 IVP131079:IVP131231 ILT131079:ILT131231 IBX131079:IBX131231 HSB131079:HSB131231 HIF131079:HIF131231 GYJ131079:GYJ131231 GON131079:GON131231 GER131079:GER131231 FUV131079:FUV131231 FKZ131079:FKZ131231 FBD131079:FBD131231 ERH131079:ERH131231 EHL131079:EHL131231 DXP131079:DXP131231 DNT131079:DNT131231 DDX131079:DDX131231 CUB131079:CUB131231 CKF131079:CKF131231 CAJ131079:CAJ131231 BQN131079:BQN131231 BGR131079:BGR131231 AWV131079:AWV131231 AMZ131079:AMZ131231 ADD131079:ADD131231 TH131079:TH131231 JL131079:JL131231 P131079:P131231 WVX65543:WVX65695 WMB65543:WMB65695 WCF65543:WCF65695 VSJ65543:VSJ65695 VIN65543:VIN65695 UYR65543:UYR65695 UOV65543:UOV65695 UEZ65543:UEZ65695 TVD65543:TVD65695 TLH65543:TLH65695 TBL65543:TBL65695 SRP65543:SRP65695 SHT65543:SHT65695 RXX65543:RXX65695 ROB65543:ROB65695 REF65543:REF65695 QUJ65543:QUJ65695 QKN65543:QKN65695 QAR65543:QAR65695 PQV65543:PQV65695 PGZ65543:PGZ65695 OXD65543:OXD65695 ONH65543:ONH65695 ODL65543:ODL65695 NTP65543:NTP65695 NJT65543:NJT65695 MZX65543:MZX65695 MQB65543:MQB65695 MGF65543:MGF65695 LWJ65543:LWJ65695 LMN65543:LMN65695 LCR65543:LCR65695 KSV65543:KSV65695 KIZ65543:KIZ65695 JZD65543:JZD65695 JPH65543:JPH65695 JFL65543:JFL65695 IVP65543:IVP65695 ILT65543:ILT65695 IBX65543:IBX65695 HSB65543:HSB65695 HIF65543:HIF65695 GYJ65543:GYJ65695 GON65543:GON65695 GER65543:GER65695 FUV65543:FUV65695 FKZ65543:FKZ65695 FBD65543:FBD65695 ERH65543:ERH65695 EHL65543:EHL65695 DXP65543:DXP65695 DNT65543:DNT65695 DDX65543:DDX65695 CUB65543:CUB65695 CKF65543:CKF65695 CAJ65543:CAJ65695 BQN65543:BQN65695 BGR65543:BGR65695 AWV65543:AWV65695 AMZ65543:AMZ65695 ADD65543:ADD65695 TH65543:TH65695 JL65543:JL65695 P65543:P65695 WVX7:WVX159 WMB7:WMB159 WCF7:WCF159 VSJ7:VSJ159 VIN7:VIN159 UYR7:UYR159 UOV7:UOV159 UEZ7:UEZ159 TVD7:TVD159 TLH7:TLH159 TBL7:TBL159 SRP7:SRP159 SHT7:SHT159 RXX7:RXX159 ROB7:ROB159 REF7:REF159 QUJ7:QUJ159 QKN7:QKN159 QAR7:QAR159 PQV7:PQV159 PGZ7:PGZ159 OXD7:OXD159 ONH7:ONH159 ODL7:ODL159 NTP7:NTP159 NJT7:NJT159 MZX7:MZX159 MQB7:MQB159 MGF7:MGF159 LWJ7:LWJ159 LMN7:LMN159 LCR7:LCR159 KSV7:KSV159 KIZ7:KIZ159 JZD7:JZD159 JPH7:JPH159 JFL7:JFL159 IVP7:IVP159 ILT7:ILT159 IBX7:IBX159 HSB7:HSB159 HIF7:HIF159 GYJ7:GYJ159 GON7:GON159 GER7:GER159 FUV7:FUV159 FKZ7:FKZ159 FBD7:FBD159 ERH7:ERH159 EHL7:EHL159 DXP7:DXP159 DNT7:DNT159 DDX7:DDX159 CUB7:CUB159 CKF7:CKF159 CAJ7:CAJ159 BQN7:BQN159 BGR7:BGR159 AWV7:AWV159 AMZ7:AMZ159 ADD7:ADD159 TH7:TH159 JL7:JL159" xr:uid="{E7830AF5-61D6-458D-A73E-440033A2476A}">
       <formula1>$AT$44:$AT$56</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K159 WVS983047:WVS983199 WLW983047:WLW983199 WCA983047:WCA983199 VSE983047:VSE983199 VII983047:VII983199 UYM983047:UYM983199 UOQ983047:UOQ983199 UEU983047:UEU983199 TUY983047:TUY983199 TLC983047:TLC983199 TBG983047:TBG983199 SRK983047:SRK983199 SHO983047:SHO983199 RXS983047:RXS983199 RNW983047:RNW983199 REA983047:REA983199 QUE983047:QUE983199 QKI983047:QKI983199 QAM983047:QAM983199 PQQ983047:PQQ983199 PGU983047:PGU983199 OWY983047:OWY983199 ONC983047:ONC983199 ODG983047:ODG983199 NTK983047:NTK983199 NJO983047:NJO983199 MZS983047:MZS983199 MPW983047:MPW983199 MGA983047:MGA983199 LWE983047:LWE983199 LMI983047:LMI983199 LCM983047:LCM983199 KSQ983047:KSQ983199 KIU983047:KIU983199 JYY983047:JYY983199 JPC983047:JPC983199 JFG983047:JFG983199 IVK983047:IVK983199 ILO983047:ILO983199 IBS983047:IBS983199 HRW983047:HRW983199 HIA983047:HIA983199 GYE983047:GYE983199 GOI983047:GOI983199 GEM983047:GEM983199 FUQ983047:FUQ983199 FKU983047:FKU983199 FAY983047:FAY983199 ERC983047:ERC983199 EHG983047:EHG983199 DXK983047:DXK983199 DNO983047:DNO983199 DDS983047:DDS983199 CTW983047:CTW983199 CKA983047:CKA983199 CAE983047:CAE983199 BQI983047:BQI983199 BGM983047:BGM983199 AWQ983047:AWQ983199 AMU983047:AMU983199 ACY983047:ACY983199 TC983047:TC983199 JG983047:JG983199 K983047:K983199 WVS917511:WVS917663 WLW917511:WLW917663 WCA917511:WCA917663 VSE917511:VSE917663 VII917511:VII917663 UYM917511:UYM917663 UOQ917511:UOQ917663 UEU917511:UEU917663 TUY917511:TUY917663 TLC917511:TLC917663 TBG917511:TBG917663 SRK917511:SRK917663 SHO917511:SHO917663 RXS917511:RXS917663 RNW917511:RNW917663 REA917511:REA917663 QUE917511:QUE917663 QKI917511:QKI917663 QAM917511:QAM917663 PQQ917511:PQQ917663 PGU917511:PGU917663 OWY917511:OWY917663 ONC917511:ONC917663 ODG917511:ODG917663 NTK917511:NTK917663 NJO917511:NJO917663 MZS917511:MZS917663 MPW917511:MPW917663 MGA917511:MGA917663 LWE917511:LWE917663 LMI917511:LMI917663 LCM917511:LCM917663 KSQ917511:KSQ917663 KIU917511:KIU917663 JYY917511:JYY917663 JPC917511:JPC917663 JFG917511:JFG917663 IVK917511:IVK917663 ILO917511:ILO917663 IBS917511:IBS917663 HRW917511:HRW917663 HIA917511:HIA917663 GYE917511:GYE917663 GOI917511:GOI917663 GEM917511:GEM917663 FUQ917511:FUQ917663 FKU917511:FKU917663 FAY917511:FAY917663 ERC917511:ERC917663 EHG917511:EHG917663 DXK917511:DXK917663 DNO917511:DNO917663 DDS917511:DDS917663 CTW917511:CTW917663 CKA917511:CKA917663 CAE917511:CAE917663 BQI917511:BQI917663 BGM917511:BGM917663 AWQ917511:AWQ917663 AMU917511:AMU917663 ACY917511:ACY917663 TC917511:TC917663 JG917511:JG917663 K917511:K917663 WVS851975:WVS852127 WLW851975:WLW852127 WCA851975:WCA852127 VSE851975:VSE852127 VII851975:VII852127 UYM851975:UYM852127 UOQ851975:UOQ852127 UEU851975:UEU852127 TUY851975:TUY852127 TLC851975:TLC852127 TBG851975:TBG852127 SRK851975:SRK852127 SHO851975:SHO852127 RXS851975:RXS852127 RNW851975:RNW852127 REA851975:REA852127 QUE851975:QUE852127 QKI851975:QKI852127 QAM851975:QAM852127 PQQ851975:PQQ852127 PGU851975:PGU852127 OWY851975:OWY852127 ONC851975:ONC852127 ODG851975:ODG852127 NTK851975:NTK852127 NJO851975:NJO852127 MZS851975:MZS852127 MPW851975:MPW852127 MGA851975:MGA852127 LWE851975:LWE852127 LMI851975:LMI852127 LCM851975:LCM852127 KSQ851975:KSQ852127 KIU851975:KIU852127 JYY851975:JYY852127 JPC851975:JPC852127 JFG851975:JFG852127 IVK851975:IVK852127 ILO851975:ILO852127 IBS851975:IBS852127 HRW851975:HRW852127 HIA851975:HIA852127 GYE851975:GYE852127 GOI851975:GOI852127 GEM851975:GEM852127 FUQ851975:FUQ852127 FKU851975:FKU852127 FAY851975:FAY852127 ERC851975:ERC852127 EHG851975:EHG852127 DXK851975:DXK852127 DNO851975:DNO852127 DDS851975:DDS852127 CTW851975:CTW852127 CKA851975:CKA852127 CAE851975:CAE852127 BQI851975:BQI852127 BGM851975:BGM852127 AWQ851975:AWQ852127 AMU851975:AMU852127 ACY851975:ACY852127 TC851975:TC852127 JG851975:JG852127 K851975:K852127 WVS786439:WVS786591 WLW786439:WLW786591 WCA786439:WCA786591 VSE786439:VSE786591 VII786439:VII786591 UYM786439:UYM786591 UOQ786439:UOQ786591 UEU786439:UEU786591 TUY786439:TUY786591 TLC786439:TLC786591 TBG786439:TBG786591 SRK786439:SRK786591 SHO786439:SHO786591 RXS786439:RXS786591 RNW786439:RNW786591 REA786439:REA786591 QUE786439:QUE786591 QKI786439:QKI786591 QAM786439:QAM786591 PQQ786439:PQQ786591 PGU786439:PGU786591 OWY786439:OWY786591 ONC786439:ONC786591 ODG786439:ODG786591 NTK786439:NTK786591 NJO786439:NJO786591 MZS786439:MZS786591 MPW786439:MPW786591 MGA786439:MGA786591 LWE786439:LWE786591 LMI786439:LMI786591 LCM786439:LCM786591 KSQ786439:KSQ786591 KIU786439:KIU786591 JYY786439:JYY786591 JPC786439:JPC786591 JFG786439:JFG786591 IVK786439:IVK786591 ILO786439:ILO786591 IBS786439:IBS786591 HRW786439:HRW786591 HIA786439:HIA786591 GYE786439:GYE786591 GOI786439:GOI786591 GEM786439:GEM786591 FUQ786439:FUQ786591 FKU786439:FKU786591 FAY786439:FAY786591 ERC786439:ERC786591 EHG786439:EHG786591 DXK786439:DXK786591 DNO786439:DNO786591 DDS786439:DDS786591 CTW786439:CTW786591 CKA786439:CKA786591 CAE786439:CAE786591 BQI786439:BQI786591 BGM786439:BGM786591 AWQ786439:AWQ786591 AMU786439:AMU786591 ACY786439:ACY786591 TC786439:TC786591 JG786439:JG786591 K786439:K786591 WVS720903:WVS721055 WLW720903:WLW721055 WCA720903:WCA721055 VSE720903:VSE721055 VII720903:VII721055 UYM720903:UYM721055 UOQ720903:UOQ721055 UEU720903:UEU721055 TUY720903:TUY721055 TLC720903:TLC721055 TBG720903:TBG721055 SRK720903:SRK721055 SHO720903:SHO721055 RXS720903:RXS721055 RNW720903:RNW721055 REA720903:REA721055 QUE720903:QUE721055 QKI720903:QKI721055 QAM720903:QAM721055 PQQ720903:PQQ721055 PGU720903:PGU721055 OWY720903:OWY721055 ONC720903:ONC721055 ODG720903:ODG721055 NTK720903:NTK721055 NJO720903:NJO721055 MZS720903:MZS721055 MPW720903:MPW721055 MGA720903:MGA721055 LWE720903:LWE721055 LMI720903:LMI721055 LCM720903:LCM721055 KSQ720903:KSQ721055 KIU720903:KIU721055 JYY720903:JYY721055 JPC720903:JPC721055 JFG720903:JFG721055 IVK720903:IVK721055 ILO720903:ILO721055 IBS720903:IBS721055 HRW720903:HRW721055 HIA720903:HIA721055 GYE720903:GYE721055 GOI720903:GOI721055 GEM720903:GEM721055 FUQ720903:FUQ721055 FKU720903:FKU721055 FAY720903:FAY721055 ERC720903:ERC721055 EHG720903:EHG721055 DXK720903:DXK721055 DNO720903:DNO721055 DDS720903:DDS721055 CTW720903:CTW721055 CKA720903:CKA721055 CAE720903:CAE721055 BQI720903:BQI721055 BGM720903:BGM721055 AWQ720903:AWQ721055 AMU720903:AMU721055 ACY720903:ACY721055 TC720903:TC721055 JG720903:JG721055 K720903:K721055 WVS655367:WVS655519 WLW655367:WLW655519 WCA655367:WCA655519 VSE655367:VSE655519 VII655367:VII655519 UYM655367:UYM655519 UOQ655367:UOQ655519 UEU655367:UEU655519 TUY655367:TUY655519 TLC655367:TLC655519 TBG655367:TBG655519 SRK655367:SRK655519 SHO655367:SHO655519 RXS655367:RXS655519 RNW655367:RNW655519 REA655367:REA655519 QUE655367:QUE655519 QKI655367:QKI655519 QAM655367:QAM655519 PQQ655367:PQQ655519 PGU655367:PGU655519 OWY655367:OWY655519 ONC655367:ONC655519 ODG655367:ODG655519 NTK655367:NTK655519 NJO655367:NJO655519 MZS655367:MZS655519 MPW655367:MPW655519 MGA655367:MGA655519 LWE655367:LWE655519 LMI655367:LMI655519 LCM655367:LCM655519 KSQ655367:KSQ655519 KIU655367:KIU655519 JYY655367:JYY655519 JPC655367:JPC655519 JFG655367:JFG655519 IVK655367:IVK655519 ILO655367:ILO655519 IBS655367:IBS655519 HRW655367:HRW655519 HIA655367:HIA655519 GYE655367:GYE655519 GOI655367:GOI655519 GEM655367:GEM655519 FUQ655367:FUQ655519 FKU655367:FKU655519 FAY655367:FAY655519 ERC655367:ERC655519 EHG655367:EHG655519 DXK655367:DXK655519 DNO655367:DNO655519 DDS655367:DDS655519 CTW655367:CTW655519 CKA655367:CKA655519 CAE655367:CAE655519 BQI655367:BQI655519 BGM655367:BGM655519 AWQ655367:AWQ655519 AMU655367:AMU655519 ACY655367:ACY655519 TC655367:TC655519 JG655367:JG655519 K655367:K655519 WVS589831:WVS589983 WLW589831:WLW589983 WCA589831:WCA589983 VSE589831:VSE589983 VII589831:VII589983 UYM589831:UYM589983 UOQ589831:UOQ589983 UEU589831:UEU589983 TUY589831:TUY589983 TLC589831:TLC589983 TBG589831:TBG589983 SRK589831:SRK589983 SHO589831:SHO589983 RXS589831:RXS589983 RNW589831:RNW589983 REA589831:REA589983 QUE589831:QUE589983 QKI589831:QKI589983 QAM589831:QAM589983 PQQ589831:PQQ589983 PGU589831:PGU589983 OWY589831:OWY589983 ONC589831:ONC589983 ODG589831:ODG589983 NTK589831:NTK589983 NJO589831:NJO589983 MZS589831:MZS589983 MPW589831:MPW589983 MGA589831:MGA589983 LWE589831:LWE589983 LMI589831:LMI589983 LCM589831:LCM589983 KSQ589831:KSQ589983 KIU589831:KIU589983 JYY589831:JYY589983 JPC589831:JPC589983 JFG589831:JFG589983 IVK589831:IVK589983 ILO589831:ILO589983 IBS589831:IBS589983 HRW589831:HRW589983 HIA589831:HIA589983 GYE589831:GYE589983 GOI589831:GOI589983 GEM589831:GEM589983 FUQ589831:FUQ589983 FKU589831:FKU589983 FAY589831:FAY589983 ERC589831:ERC589983 EHG589831:EHG589983 DXK589831:DXK589983 DNO589831:DNO589983 DDS589831:DDS589983 CTW589831:CTW589983 CKA589831:CKA589983 CAE589831:CAE589983 BQI589831:BQI589983 BGM589831:BGM589983 AWQ589831:AWQ589983 AMU589831:AMU589983 ACY589831:ACY589983 TC589831:TC589983 JG589831:JG589983 K589831:K589983 WVS524295:WVS524447 WLW524295:WLW524447 WCA524295:WCA524447 VSE524295:VSE524447 VII524295:VII524447 UYM524295:UYM524447 UOQ524295:UOQ524447 UEU524295:UEU524447 TUY524295:TUY524447 TLC524295:TLC524447 TBG524295:TBG524447 SRK524295:SRK524447 SHO524295:SHO524447 RXS524295:RXS524447 RNW524295:RNW524447 REA524295:REA524447 QUE524295:QUE524447 QKI524295:QKI524447 QAM524295:QAM524447 PQQ524295:PQQ524447 PGU524295:PGU524447 OWY524295:OWY524447 ONC524295:ONC524447 ODG524295:ODG524447 NTK524295:NTK524447 NJO524295:NJO524447 MZS524295:MZS524447 MPW524295:MPW524447 MGA524295:MGA524447 LWE524295:LWE524447 LMI524295:LMI524447 LCM524295:LCM524447 KSQ524295:KSQ524447 KIU524295:KIU524447 JYY524295:JYY524447 JPC524295:JPC524447 JFG524295:JFG524447 IVK524295:IVK524447 ILO524295:ILO524447 IBS524295:IBS524447 HRW524295:HRW524447 HIA524295:HIA524447 GYE524295:GYE524447 GOI524295:GOI524447 GEM524295:GEM524447 FUQ524295:FUQ524447 FKU524295:FKU524447 FAY524295:FAY524447 ERC524295:ERC524447 EHG524295:EHG524447 DXK524295:DXK524447 DNO524295:DNO524447 DDS524295:DDS524447 CTW524295:CTW524447 CKA524295:CKA524447 CAE524295:CAE524447 BQI524295:BQI524447 BGM524295:BGM524447 AWQ524295:AWQ524447 AMU524295:AMU524447 ACY524295:ACY524447 TC524295:TC524447 JG524295:JG524447 K524295:K524447 WVS458759:WVS458911 WLW458759:WLW458911 WCA458759:WCA458911 VSE458759:VSE458911 VII458759:VII458911 UYM458759:UYM458911 UOQ458759:UOQ458911 UEU458759:UEU458911 TUY458759:TUY458911 TLC458759:TLC458911 TBG458759:TBG458911 SRK458759:SRK458911 SHO458759:SHO458911 RXS458759:RXS458911 RNW458759:RNW458911 REA458759:REA458911 QUE458759:QUE458911 QKI458759:QKI458911 QAM458759:QAM458911 PQQ458759:PQQ458911 PGU458759:PGU458911 OWY458759:OWY458911 ONC458759:ONC458911 ODG458759:ODG458911 NTK458759:NTK458911 NJO458759:NJO458911 MZS458759:MZS458911 MPW458759:MPW458911 MGA458759:MGA458911 LWE458759:LWE458911 LMI458759:LMI458911 LCM458759:LCM458911 KSQ458759:KSQ458911 KIU458759:KIU458911 JYY458759:JYY458911 JPC458759:JPC458911 JFG458759:JFG458911 IVK458759:IVK458911 ILO458759:ILO458911 IBS458759:IBS458911 HRW458759:HRW458911 HIA458759:HIA458911 GYE458759:GYE458911 GOI458759:GOI458911 GEM458759:GEM458911 FUQ458759:FUQ458911 FKU458759:FKU458911 FAY458759:FAY458911 ERC458759:ERC458911 EHG458759:EHG458911 DXK458759:DXK458911 DNO458759:DNO458911 DDS458759:DDS458911 CTW458759:CTW458911 CKA458759:CKA458911 CAE458759:CAE458911 BQI458759:BQI458911 BGM458759:BGM458911 AWQ458759:AWQ458911 AMU458759:AMU458911 ACY458759:ACY458911 TC458759:TC458911 JG458759:JG458911 K458759:K458911 WVS393223:WVS393375 WLW393223:WLW393375 WCA393223:WCA393375 VSE393223:VSE393375 VII393223:VII393375 UYM393223:UYM393375 UOQ393223:UOQ393375 UEU393223:UEU393375 TUY393223:TUY393375 TLC393223:TLC393375 TBG393223:TBG393375 SRK393223:SRK393375 SHO393223:SHO393375 RXS393223:RXS393375 RNW393223:RNW393375 REA393223:REA393375 QUE393223:QUE393375 QKI393223:QKI393375 QAM393223:QAM393375 PQQ393223:PQQ393375 PGU393223:PGU393375 OWY393223:OWY393375 ONC393223:ONC393375 ODG393223:ODG393375 NTK393223:NTK393375 NJO393223:NJO393375 MZS393223:MZS393375 MPW393223:MPW393375 MGA393223:MGA393375 LWE393223:LWE393375 LMI393223:LMI393375 LCM393223:LCM393375 KSQ393223:KSQ393375 KIU393223:KIU393375 JYY393223:JYY393375 JPC393223:JPC393375 JFG393223:JFG393375 IVK393223:IVK393375 ILO393223:ILO393375 IBS393223:IBS393375 HRW393223:HRW393375 HIA393223:HIA393375 GYE393223:GYE393375 GOI393223:GOI393375 GEM393223:GEM393375 FUQ393223:FUQ393375 FKU393223:FKU393375 FAY393223:FAY393375 ERC393223:ERC393375 EHG393223:EHG393375 DXK393223:DXK393375 DNO393223:DNO393375 DDS393223:DDS393375 CTW393223:CTW393375 CKA393223:CKA393375 CAE393223:CAE393375 BQI393223:BQI393375 BGM393223:BGM393375 AWQ393223:AWQ393375 AMU393223:AMU393375 ACY393223:ACY393375 TC393223:TC393375 JG393223:JG393375 K393223:K393375 WVS327687:WVS327839 WLW327687:WLW327839 WCA327687:WCA327839 VSE327687:VSE327839 VII327687:VII327839 UYM327687:UYM327839 UOQ327687:UOQ327839 UEU327687:UEU327839 TUY327687:TUY327839 TLC327687:TLC327839 TBG327687:TBG327839 SRK327687:SRK327839 SHO327687:SHO327839 RXS327687:RXS327839 RNW327687:RNW327839 REA327687:REA327839 QUE327687:QUE327839 QKI327687:QKI327839 QAM327687:QAM327839 PQQ327687:PQQ327839 PGU327687:PGU327839 OWY327687:OWY327839 ONC327687:ONC327839 ODG327687:ODG327839 NTK327687:NTK327839 NJO327687:NJO327839 MZS327687:MZS327839 MPW327687:MPW327839 MGA327687:MGA327839 LWE327687:LWE327839 LMI327687:LMI327839 LCM327687:LCM327839 KSQ327687:KSQ327839 KIU327687:KIU327839 JYY327687:JYY327839 JPC327687:JPC327839 JFG327687:JFG327839 IVK327687:IVK327839 ILO327687:ILO327839 IBS327687:IBS327839 HRW327687:HRW327839 HIA327687:HIA327839 GYE327687:GYE327839 GOI327687:GOI327839 GEM327687:GEM327839 FUQ327687:FUQ327839 FKU327687:FKU327839 FAY327687:FAY327839 ERC327687:ERC327839 EHG327687:EHG327839 DXK327687:DXK327839 DNO327687:DNO327839 DDS327687:DDS327839 CTW327687:CTW327839 CKA327687:CKA327839 CAE327687:CAE327839 BQI327687:BQI327839 BGM327687:BGM327839 AWQ327687:AWQ327839 AMU327687:AMU327839 ACY327687:ACY327839 TC327687:TC327839 JG327687:JG327839 K327687:K327839 WVS262151:WVS262303 WLW262151:WLW262303 WCA262151:WCA262303 VSE262151:VSE262303 VII262151:VII262303 UYM262151:UYM262303 UOQ262151:UOQ262303 UEU262151:UEU262303 TUY262151:TUY262303 TLC262151:TLC262303 TBG262151:TBG262303 SRK262151:SRK262303 SHO262151:SHO262303 RXS262151:RXS262303 RNW262151:RNW262303 REA262151:REA262303 QUE262151:QUE262303 QKI262151:QKI262303 QAM262151:QAM262303 PQQ262151:PQQ262303 PGU262151:PGU262303 OWY262151:OWY262303 ONC262151:ONC262303 ODG262151:ODG262303 NTK262151:NTK262303 NJO262151:NJO262303 MZS262151:MZS262303 MPW262151:MPW262303 MGA262151:MGA262303 LWE262151:LWE262303 LMI262151:LMI262303 LCM262151:LCM262303 KSQ262151:KSQ262303 KIU262151:KIU262303 JYY262151:JYY262303 JPC262151:JPC262303 JFG262151:JFG262303 IVK262151:IVK262303 ILO262151:ILO262303 IBS262151:IBS262303 HRW262151:HRW262303 HIA262151:HIA262303 GYE262151:GYE262303 GOI262151:GOI262303 GEM262151:GEM262303 FUQ262151:FUQ262303 FKU262151:FKU262303 FAY262151:FAY262303 ERC262151:ERC262303 EHG262151:EHG262303 DXK262151:DXK262303 DNO262151:DNO262303 DDS262151:DDS262303 CTW262151:CTW262303 CKA262151:CKA262303 CAE262151:CAE262303 BQI262151:BQI262303 BGM262151:BGM262303 AWQ262151:AWQ262303 AMU262151:AMU262303 ACY262151:ACY262303 TC262151:TC262303 JG262151:JG262303 K262151:K262303 WVS196615:WVS196767 WLW196615:WLW196767 WCA196615:WCA196767 VSE196615:VSE196767 VII196615:VII196767 UYM196615:UYM196767 UOQ196615:UOQ196767 UEU196615:UEU196767 TUY196615:TUY196767 TLC196615:TLC196767 TBG196615:TBG196767 SRK196615:SRK196767 SHO196615:SHO196767 RXS196615:RXS196767 RNW196615:RNW196767 REA196615:REA196767 QUE196615:QUE196767 QKI196615:QKI196767 QAM196615:QAM196767 PQQ196615:PQQ196767 PGU196615:PGU196767 OWY196615:OWY196767 ONC196615:ONC196767 ODG196615:ODG196767 NTK196615:NTK196767 NJO196615:NJO196767 MZS196615:MZS196767 MPW196615:MPW196767 MGA196615:MGA196767 LWE196615:LWE196767 LMI196615:LMI196767 LCM196615:LCM196767 KSQ196615:KSQ196767 KIU196615:KIU196767 JYY196615:JYY196767 JPC196615:JPC196767 JFG196615:JFG196767 IVK196615:IVK196767 ILO196615:ILO196767 IBS196615:IBS196767 HRW196615:HRW196767 HIA196615:HIA196767 GYE196615:GYE196767 GOI196615:GOI196767 GEM196615:GEM196767 FUQ196615:FUQ196767 FKU196615:FKU196767 FAY196615:FAY196767 ERC196615:ERC196767 EHG196615:EHG196767 DXK196615:DXK196767 DNO196615:DNO196767 DDS196615:DDS196767 CTW196615:CTW196767 CKA196615:CKA196767 CAE196615:CAE196767 BQI196615:BQI196767 BGM196615:BGM196767 AWQ196615:AWQ196767 AMU196615:AMU196767 ACY196615:ACY196767 TC196615:TC196767 JG196615:JG196767 K196615:K196767 WVS131079:WVS131231 WLW131079:WLW131231 WCA131079:WCA131231 VSE131079:VSE131231 VII131079:VII131231 UYM131079:UYM131231 UOQ131079:UOQ131231 UEU131079:UEU131231 TUY131079:TUY131231 TLC131079:TLC131231 TBG131079:TBG131231 SRK131079:SRK131231 SHO131079:SHO131231 RXS131079:RXS131231 RNW131079:RNW131231 REA131079:REA131231 QUE131079:QUE131231 QKI131079:QKI131231 QAM131079:QAM131231 PQQ131079:PQQ131231 PGU131079:PGU131231 OWY131079:OWY131231 ONC131079:ONC131231 ODG131079:ODG131231 NTK131079:NTK131231 NJO131079:NJO131231 MZS131079:MZS131231 MPW131079:MPW131231 MGA131079:MGA131231 LWE131079:LWE131231 LMI131079:LMI131231 LCM131079:LCM131231 KSQ131079:KSQ131231 KIU131079:KIU131231 JYY131079:JYY131231 JPC131079:JPC131231 JFG131079:JFG131231 IVK131079:IVK131231 ILO131079:ILO131231 IBS131079:IBS131231 HRW131079:HRW131231 HIA131079:HIA131231 GYE131079:GYE131231 GOI131079:GOI131231 GEM131079:GEM131231 FUQ131079:FUQ131231 FKU131079:FKU131231 FAY131079:FAY131231 ERC131079:ERC131231 EHG131079:EHG131231 DXK131079:DXK131231 DNO131079:DNO131231 DDS131079:DDS131231 CTW131079:CTW131231 CKA131079:CKA131231 CAE131079:CAE131231 BQI131079:BQI131231 BGM131079:BGM131231 AWQ131079:AWQ131231 AMU131079:AMU131231 ACY131079:ACY131231 TC131079:TC131231 JG131079:JG131231 K131079:K131231 WVS65543:WVS65695 WLW65543:WLW65695 WCA65543:WCA65695 VSE65543:VSE65695 VII65543:VII65695 UYM65543:UYM65695 UOQ65543:UOQ65695 UEU65543:UEU65695 TUY65543:TUY65695 TLC65543:TLC65695 TBG65543:TBG65695 SRK65543:SRK65695 SHO65543:SHO65695 RXS65543:RXS65695 RNW65543:RNW65695 REA65543:REA65695 QUE65543:QUE65695 QKI65543:QKI65695 QAM65543:QAM65695 PQQ65543:PQQ65695 PGU65543:PGU65695 OWY65543:OWY65695 ONC65543:ONC65695 ODG65543:ODG65695 NTK65543:NTK65695 NJO65543:NJO65695 MZS65543:MZS65695 MPW65543:MPW65695 MGA65543:MGA65695 LWE65543:LWE65695 LMI65543:LMI65695 LCM65543:LCM65695 KSQ65543:KSQ65695 KIU65543:KIU65695 JYY65543:JYY65695 JPC65543:JPC65695 JFG65543:JFG65695 IVK65543:IVK65695 ILO65543:ILO65695 IBS65543:IBS65695 HRW65543:HRW65695 HIA65543:HIA65695 GYE65543:GYE65695 GOI65543:GOI65695 GEM65543:GEM65695 FUQ65543:FUQ65695 FKU65543:FKU65695 FAY65543:FAY65695 ERC65543:ERC65695 EHG65543:EHG65695 DXK65543:DXK65695 DNO65543:DNO65695 DDS65543:DDS65695 CTW65543:CTW65695 CKA65543:CKA65695 CAE65543:CAE65695 BQI65543:BQI65695 BGM65543:BGM65695 AWQ65543:AWQ65695 AMU65543:AMU65695 ACY65543:ACY65695 TC65543:TC65695 JG65543:JG65695 K65543:K65695 WVS7:WVS159 WLW7:WLW159 WCA7:WCA159 VSE7:VSE159 VII7:VII159 UYM7:UYM159 UOQ7:UOQ159 UEU7:UEU159 TUY7:TUY159 TLC7:TLC159 TBG7:TBG159 SRK7:SRK159 SHO7:SHO159 RXS7:RXS159 RNW7:RNW159 REA7:REA159 QUE7:QUE159 QKI7:QKI159 QAM7:QAM159 PQQ7:PQQ159 PGU7:PGU159 OWY7:OWY159 ONC7:ONC159 ODG7:ODG159 NTK7:NTK159 NJO7:NJO159 MZS7:MZS159 MPW7:MPW159 MGA7:MGA159 LWE7:LWE159 LMI7:LMI159 LCM7:LCM159 KSQ7:KSQ159 KIU7:KIU159 JYY7:JYY159 JPC7:JPC159 JFG7:JFG159 IVK7:IVK159 ILO7:ILO159 IBS7:IBS159 HRW7:HRW159 HIA7:HIA159 GYE7:GYE159 GOI7:GOI159 GEM7:GEM159 FUQ7:FUQ159 FKU7:FKU159 FAY7:FAY159 ERC7:ERC159 EHG7:EHG159 DXK7:DXK159 DNO7:DNO159 DDS7:DDS159 CTW7:CTW159 CKA7:CKA159 CAE7:CAE159 BQI7:BQI159 BGM7:BGM159 AWQ7:AWQ159 AMU7:AMU159 ACY7:ACY159 TC7:TC159 JG7:JG159" xr:uid="{16400355-3C3D-43F8-B702-E29A5B9CC1B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JG7:JG159 WVS983047:WVS983199 WLW983047:WLW983199 WCA983047:WCA983199 VSE983047:VSE983199 VII983047:VII983199 UYM983047:UYM983199 UOQ983047:UOQ983199 UEU983047:UEU983199 TUY983047:TUY983199 TLC983047:TLC983199 TBG983047:TBG983199 SRK983047:SRK983199 SHO983047:SHO983199 RXS983047:RXS983199 RNW983047:RNW983199 REA983047:REA983199 QUE983047:QUE983199 QKI983047:QKI983199 QAM983047:QAM983199 PQQ983047:PQQ983199 PGU983047:PGU983199 OWY983047:OWY983199 ONC983047:ONC983199 ODG983047:ODG983199 NTK983047:NTK983199 NJO983047:NJO983199 MZS983047:MZS983199 MPW983047:MPW983199 MGA983047:MGA983199 LWE983047:LWE983199 LMI983047:LMI983199 LCM983047:LCM983199 KSQ983047:KSQ983199 KIU983047:KIU983199 JYY983047:JYY983199 JPC983047:JPC983199 JFG983047:JFG983199 IVK983047:IVK983199 ILO983047:ILO983199 IBS983047:IBS983199 HRW983047:HRW983199 HIA983047:HIA983199 GYE983047:GYE983199 GOI983047:GOI983199 GEM983047:GEM983199 FUQ983047:FUQ983199 FKU983047:FKU983199 FAY983047:FAY983199 ERC983047:ERC983199 EHG983047:EHG983199 DXK983047:DXK983199 DNO983047:DNO983199 DDS983047:DDS983199 CTW983047:CTW983199 CKA983047:CKA983199 CAE983047:CAE983199 BQI983047:BQI983199 BGM983047:BGM983199 AWQ983047:AWQ983199 AMU983047:AMU983199 ACY983047:ACY983199 TC983047:TC983199 JG983047:JG983199 K983047:K983199 WVS917511:WVS917663 WLW917511:WLW917663 WCA917511:WCA917663 VSE917511:VSE917663 VII917511:VII917663 UYM917511:UYM917663 UOQ917511:UOQ917663 UEU917511:UEU917663 TUY917511:TUY917663 TLC917511:TLC917663 TBG917511:TBG917663 SRK917511:SRK917663 SHO917511:SHO917663 RXS917511:RXS917663 RNW917511:RNW917663 REA917511:REA917663 QUE917511:QUE917663 QKI917511:QKI917663 QAM917511:QAM917663 PQQ917511:PQQ917663 PGU917511:PGU917663 OWY917511:OWY917663 ONC917511:ONC917663 ODG917511:ODG917663 NTK917511:NTK917663 NJO917511:NJO917663 MZS917511:MZS917663 MPW917511:MPW917663 MGA917511:MGA917663 LWE917511:LWE917663 LMI917511:LMI917663 LCM917511:LCM917663 KSQ917511:KSQ917663 KIU917511:KIU917663 JYY917511:JYY917663 JPC917511:JPC917663 JFG917511:JFG917663 IVK917511:IVK917663 ILO917511:ILO917663 IBS917511:IBS917663 HRW917511:HRW917663 HIA917511:HIA917663 GYE917511:GYE917663 GOI917511:GOI917663 GEM917511:GEM917663 FUQ917511:FUQ917663 FKU917511:FKU917663 FAY917511:FAY917663 ERC917511:ERC917663 EHG917511:EHG917663 DXK917511:DXK917663 DNO917511:DNO917663 DDS917511:DDS917663 CTW917511:CTW917663 CKA917511:CKA917663 CAE917511:CAE917663 BQI917511:BQI917663 BGM917511:BGM917663 AWQ917511:AWQ917663 AMU917511:AMU917663 ACY917511:ACY917663 TC917511:TC917663 JG917511:JG917663 K917511:K917663 WVS851975:WVS852127 WLW851975:WLW852127 WCA851975:WCA852127 VSE851975:VSE852127 VII851975:VII852127 UYM851975:UYM852127 UOQ851975:UOQ852127 UEU851975:UEU852127 TUY851975:TUY852127 TLC851975:TLC852127 TBG851975:TBG852127 SRK851975:SRK852127 SHO851975:SHO852127 RXS851975:RXS852127 RNW851975:RNW852127 REA851975:REA852127 QUE851975:QUE852127 QKI851975:QKI852127 QAM851975:QAM852127 PQQ851975:PQQ852127 PGU851975:PGU852127 OWY851975:OWY852127 ONC851975:ONC852127 ODG851975:ODG852127 NTK851975:NTK852127 NJO851975:NJO852127 MZS851975:MZS852127 MPW851975:MPW852127 MGA851975:MGA852127 LWE851975:LWE852127 LMI851975:LMI852127 LCM851975:LCM852127 KSQ851975:KSQ852127 KIU851975:KIU852127 JYY851975:JYY852127 JPC851975:JPC852127 JFG851975:JFG852127 IVK851975:IVK852127 ILO851975:ILO852127 IBS851975:IBS852127 HRW851975:HRW852127 HIA851975:HIA852127 GYE851975:GYE852127 GOI851975:GOI852127 GEM851975:GEM852127 FUQ851975:FUQ852127 FKU851975:FKU852127 FAY851975:FAY852127 ERC851975:ERC852127 EHG851975:EHG852127 DXK851975:DXK852127 DNO851975:DNO852127 DDS851975:DDS852127 CTW851975:CTW852127 CKA851975:CKA852127 CAE851975:CAE852127 BQI851975:BQI852127 BGM851975:BGM852127 AWQ851975:AWQ852127 AMU851975:AMU852127 ACY851975:ACY852127 TC851975:TC852127 JG851975:JG852127 K851975:K852127 WVS786439:WVS786591 WLW786439:WLW786591 WCA786439:WCA786591 VSE786439:VSE786591 VII786439:VII786591 UYM786439:UYM786591 UOQ786439:UOQ786591 UEU786439:UEU786591 TUY786439:TUY786591 TLC786439:TLC786591 TBG786439:TBG786591 SRK786439:SRK786591 SHO786439:SHO786591 RXS786439:RXS786591 RNW786439:RNW786591 REA786439:REA786591 QUE786439:QUE786591 QKI786439:QKI786591 QAM786439:QAM786591 PQQ786439:PQQ786591 PGU786439:PGU786591 OWY786439:OWY786591 ONC786439:ONC786591 ODG786439:ODG786591 NTK786439:NTK786591 NJO786439:NJO786591 MZS786439:MZS786591 MPW786439:MPW786591 MGA786439:MGA786591 LWE786439:LWE786591 LMI786439:LMI786591 LCM786439:LCM786591 KSQ786439:KSQ786591 KIU786439:KIU786591 JYY786439:JYY786591 JPC786439:JPC786591 JFG786439:JFG786591 IVK786439:IVK786591 ILO786439:ILO786591 IBS786439:IBS786591 HRW786439:HRW786591 HIA786439:HIA786591 GYE786439:GYE786591 GOI786439:GOI786591 GEM786439:GEM786591 FUQ786439:FUQ786591 FKU786439:FKU786591 FAY786439:FAY786591 ERC786439:ERC786591 EHG786439:EHG786591 DXK786439:DXK786591 DNO786439:DNO786591 DDS786439:DDS786591 CTW786439:CTW786591 CKA786439:CKA786591 CAE786439:CAE786591 BQI786439:BQI786591 BGM786439:BGM786591 AWQ786439:AWQ786591 AMU786439:AMU786591 ACY786439:ACY786591 TC786439:TC786591 JG786439:JG786591 K786439:K786591 WVS720903:WVS721055 WLW720903:WLW721055 WCA720903:WCA721055 VSE720903:VSE721055 VII720903:VII721055 UYM720903:UYM721055 UOQ720903:UOQ721055 UEU720903:UEU721055 TUY720903:TUY721055 TLC720903:TLC721055 TBG720903:TBG721055 SRK720903:SRK721055 SHO720903:SHO721055 RXS720903:RXS721055 RNW720903:RNW721055 REA720903:REA721055 QUE720903:QUE721055 QKI720903:QKI721055 QAM720903:QAM721055 PQQ720903:PQQ721055 PGU720903:PGU721055 OWY720903:OWY721055 ONC720903:ONC721055 ODG720903:ODG721055 NTK720903:NTK721055 NJO720903:NJO721055 MZS720903:MZS721055 MPW720903:MPW721055 MGA720903:MGA721055 LWE720903:LWE721055 LMI720903:LMI721055 LCM720903:LCM721055 KSQ720903:KSQ721055 KIU720903:KIU721055 JYY720903:JYY721055 JPC720903:JPC721055 JFG720903:JFG721055 IVK720903:IVK721055 ILO720903:ILO721055 IBS720903:IBS721055 HRW720903:HRW721055 HIA720903:HIA721055 GYE720903:GYE721055 GOI720903:GOI721055 GEM720903:GEM721055 FUQ720903:FUQ721055 FKU720903:FKU721055 FAY720903:FAY721055 ERC720903:ERC721055 EHG720903:EHG721055 DXK720903:DXK721055 DNO720903:DNO721055 DDS720903:DDS721055 CTW720903:CTW721055 CKA720903:CKA721055 CAE720903:CAE721055 BQI720903:BQI721055 BGM720903:BGM721055 AWQ720903:AWQ721055 AMU720903:AMU721055 ACY720903:ACY721055 TC720903:TC721055 JG720903:JG721055 K720903:K721055 WVS655367:WVS655519 WLW655367:WLW655519 WCA655367:WCA655519 VSE655367:VSE655519 VII655367:VII655519 UYM655367:UYM655519 UOQ655367:UOQ655519 UEU655367:UEU655519 TUY655367:TUY655519 TLC655367:TLC655519 TBG655367:TBG655519 SRK655367:SRK655519 SHO655367:SHO655519 RXS655367:RXS655519 RNW655367:RNW655519 REA655367:REA655519 QUE655367:QUE655519 QKI655367:QKI655519 QAM655367:QAM655519 PQQ655367:PQQ655519 PGU655367:PGU655519 OWY655367:OWY655519 ONC655367:ONC655519 ODG655367:ODG655519 NTK655367:NTK655519 NJO655367:NJO655519 MZS655367:MZS655519 MPW655367:MPW655519 MGA655367:MGA655519 LWE655367:LWE655519 LMI655367:LMI655519 LCM655367:LCM655519 KSQ655367:KSQ655519 KIU655367:KIU655519 JYY655367:JYY655519 JPC655367:JPC655519 JFG655367:JFG655519 IVK655367:IVK655519 ILO655367:ILO655519 IBS655367:IBS655519 HRW655367:HRW655519 HIA655367:HIA655519 GYE655367:GYE655519 GOI655367:GOI655519 GEM655367:GEM655519 FUQ655367:FUQ655519 FKU655367:FKU655519 FAY655367:FAY655519 ERC655367:ERC655519 EHG655367:EHG655519 DXK655367:DXK655519 DNO655367:DNO655519 DDS655367:DDS655519 CTW655367:CTW655519 CKA655367:CKA655519 CAE655367:CAE655519 BQI655367:BQI655519 BGM655367:BGM655519 AWQ655367:AWQ655519 AMU655367:AMU655519 ACY655367:ACY655519 TC655367:TC655519 JG655367:JG655519 K655367:K655519 WVS589831:WVS589983 WLW589831:WLW589983 WCA589831:WCA589983 VSE589831:VSE589983 VII589831:VII589983 UYM589831:UYM589983 UOQ589831:UOQ589983 UEU589831:UEU589983 TUY589831:TUY589983 TLC589831:TLC589983 TBG589831:TBG589983 SRK589831:SRK589983 SHO589831:SHO589983 RXS589831:RXS589983 RNW589831:RNW589983 REA589831:REA589983 QUE589831:QUE589983 QKI589831:QKI589983 QAM589831:QAM589983 PQQ589831:PQQ589983 PGU589831:PGU589983 OWY589831:OWY589983 ONC589831:ONC589983 ODG589831:ODG589983 NTK589831:NTK589983 NJO589831:NJO589983 MZS589831:MZS589983 MPW589831:MPW589983 MGA589831:MGA589983 LWE589831:LWE589983 LMI589831:LMI589983 LCM589831:LCM589983 KSQ589831:KSQ589983 KIU589831:KIU589983 JYY589831:JYY589983 JPC589831:JPC589983 JFG589831:JFG589983 IVK589831:IVK589983 ILO589831:ILO589983 IBS589831:IBS589983 HRW589831:HRW589983 HIA589831:HIA589983 GYE589831:GYE589983 GOI589831:GOI589983 GEM589831:GEM589983 FUQ589831:FUQ589983 FKU589831:FKU589983 FAY589831:FAY589983 ERC589831:ERC589983 EHG589831:EHG589983 DXK589831:DXK589983 DNO589831:DNO589983 DDS589831:DDS589983 CTW589831:CTW589983 CKA589831:CKA589983 CAE589831:CAE589983 BQI589831:BQI589983 BGM589831:BGM589983 AWQ589831:AWQ589983 AMU589831:AMU589983 ACY589831:ACY589983 TC589831:TC589983 JG589831:JG589983 K589831:K589983 WVS524295:WVS524447 WLW524295:WLW524447 WCA524295:WCA524447 VSE524295:VSE524447 VII524295:VII524447 UYM524295:UYM524447 UOQ524295:UOQ524447 UEU524295:UEU524447 TUY524295:TUY524447 TLC524295:TLC524447 TBG524295:TBG524447 SRK524295:SRK524447 SHO524295:SHO524447 RXS524295:RXS524447 RNW524295:RNW524447 REA524295:REA524447 QUE524295:QUE524447 QKI524295:QKI524447 QAM524295:QAM524447 PQQ524295:PQQ524447 PGU524295:PGU524447 OWY524295:OWY524447 ONC524295:ONC524447 ODG524295:ODG524447 NTK524295:NTK524447 NJO524295:NJO524447 MZS524295:MZS524447 MPW524295:MPW524447 MGA524295:MGA524447 LWE524295:LWE524447 LMI524295:LMI524447 LCM524295:LCM524447 KSQ524295:KSQ524447 KIU524295:KIU524447 JYY524295:JYY524447 JPC524295:JPC524447 JFG524295:JFG524447 IVK524295:IVK524447 ILO524295:ILO524447 IBS524295:IBS524447 HRW524295:HRW524447 HIA524295:HIA524447 GYE524295:GYE524447 GOI524295:GOI524447 GEM524295:GEM524447 FUQ524295:FUQ524447 FKU524295:FKU524447 FAY524295:FAY524447 ERC524295:ERC524447 EHG524295:EHG524447 DXK524295:DXK524447 DNO524295:DNO524447 DDS524295:DDS524447 CTW524295:CTW524447 CKA524295:CKA524447 CAE524295:CAE524447 BQI524295:BQI524447 BGM524295:BGM524447 AWQ524295:AWQ524447 AMU524295:AMU524447 ACY524295:ACY524447 TC524295:TC524447 JG524295:JG524447 K524295:K524447 WVS458759:WVS458911 WLW458759:WLW458911 WCA458759:WCA458911 VSE458759:VSE458911 VII458759:VII458911 UYM458759:UYM458911 UOQ458759:UOQ458911 UEU458759:UEU458911 TUY458759:TUY458911 TLC458759:TLC458911 TBG458759:TBG458911 SRK458759:SRK458911 SHO458759:SHO458911 RXS458759:RXS458911 RNW458759:RNW458911 REA458759:REA458911 QUE458759:QUE458911 QKI458759:QKI458911 QAM458759:QAM458911 PQQ458759:PQQ458911 PGU458759:PGU458911 OWY458759:OWY458911 ONC458759:ONC458911 ODG458759:ODG458911 NTK458759:NTK458911 NJO458759:NJO458911 MZS458759:MZS458911 MPW458759:MPW458911 MGA458759:MGA458911 LWE458759:LWE458911 LMI458759:LMI458911 LCM458759:LCM458911 KSQ458759:KSQ458911 KIU458759:KIU458911 JYY458759:JYY458911 JPC458759:JPC458911 JFG458759:JFG458911 IVK458759:IVK458911 ILO458759:ILO458911 IBS458759:IBS458911 HRW458759:HRW458911 HIA458759:HIA458911 GYE458759:GYE458911 GOI458759:GOI458911 GEM458759:GEM458911 FUQ458759:FUQ458911 FKU458759:FKU458911 FAY458759:FAY458911 ERC458759:ERC458911 EHG458759:EHG458911 DXK458759:DXK458911 DNO458759:DNO458911 DDS458759:DDS458911 CTW458759:CTW458911 CKA458759:CKA458911 CAE458759:CAE458911 BQI458759:BQI458911 BGM458759:BGM458911 AWQ458759:AWQ458911 AMU458759:AMU458911 ACY458759:ACY458911 TC458759:TC458911 JG458759:JG458911 K458759:K458911 WVS393223:WVS393375 WLW393223:WLW393375 WCA393223:WCA393375 VSE393223:VSE393375 VII393223:VII393375 UYM393223:UYM393375 UOQ393223:UOQ393375 UEU393223:UEU393375 TUY393223:TUY393375 TLC393223:TLC393375 TBG393223:TBG393375 SRK393223:SRK393375 SHO393223:SHO393375 RXS393223:RXS393375 RNW393223:RNW393375 REA393223:REA393375 QUE393223:QUE393375 QKI393223:QKI393375 QAM393223:QAM393375 PQQ393223:PQQ393375 PGU393223:PGU393375 OWY393223:OWY393375 ONC393223:ONC393375 ODG393223:ODG393375 NTK393223:NTK393375 NJO393223:NJO393375 MZS393223:MZS393375 MPW393223:MPW393375 MGA393223:MGA393375 LWE393223:LWE393375 LMI393223:LMI393375 LCM393223:LCM393375 KSQ393223:KSQ393375 KIU393223:KIU393375 JYY393223:JYY393375 JPC393223:JPC393375 JFG393223:JFG393375 IVK393223:IVK393375 ILO393223:ILO393375 IBS393223:IBS393375 HRW393223:HRW393375 HIA393223:HIA393375 GYE393223:GYE393375 GOI393223:GOI393375 GEM393223:GEM393375 FUQ393223:FUQ393375 FKU393223:FKU393375 FAY393223:FAY393375 ERC393223:ERC393375 EHG393223:EHG393375 DXK393223:DXK393375 DNO393223:DNO393375 DDS393223:DDS393375 CTW393223:CTW393375 CKA393223:CKA393375 CAE393223:CAE393375 BQI393223:BQI393375 BGM393223:BGM393375 AWQ393223:AWQ393375 AMU393223:AMU393375 ACY393223:ACY393375 TC393223:TC393375 JG393223:JG393375 K393223:K393375 WVS327687:WVS327839 WLW327687:WLW327839 WCA327687:WCA327839 VSE327687:VSE327839 VII327687:VII327839 UYM327687:UYM327839 UOQ327687:UOQ327839 UEU327687:UEU327839 TUY327687:TUY327839 TLC327687:TLC327839 TBG327687:TBG327839 SRK327687:SRK327839 SHO327687:SHO327839 RXS327687:RXS327839 RNW327687:RNW327839 REA327687:REA327839 QUE327687:QUE327839 QKI327687:QKI327839 QAM327687:QAM327839 PQQ327687:PQQ327839 PGU327687:PGU327839 OWY327687:OWY327839 ONC327687:ONC327839 ODG327687:ODG327839 NTK327687:NTK327839 NJO327687:NJO327839 MZS327687:MZS327839 MPW327687:MPW327839 MGA327687:MGA327839 LWE327687:LWE327839 LMI327687:LMI327839 LCM327687:LCM327839 KSQ327687:KSQ327839 KIU327687:KIU327839 JYY327687:JYY327839 JPC327687:JPC327839 JFG327687:JFG327839 IVK327687:IVK327839 ILO327687:ILO327839 IBS327687:IBS327839 HRW327687:HRW327839 HIA327687:HIA327839 GYE327687:GYE327839 GOI327687:GOI327839 GEM327687:GEM327839 FUQ327687:FUQ327839 FKU327687:FKU327839 FAY327687:FAY327839 ERC327687:ERC327839 EHG327687:EHG327839 DXK327687:DXK327839 DNO327687:DNO327839 DDS327687:DDS327839 CTW327687:CTW327839 CKA327687:CKA327839 CAE327687:CAE327839 BQI327687:BQI327839 BGM327687:BGM327839 AWQ327687:AWQ327839 AMU327687:AMU327839 ACY327687:ACY327839 TC327687:TC327839 JG327687:JG327839 K327687:K327839 WVS262151:WVS262303 WLW262151:WLW262303 WCA262151:WCA262303 VSE262151:VSE262303 VII262151:VII262303 UYM262151:UYM262303 UOQ262151:UOQ262303 UEU262151:UEU262303 TUY262151:TUY262303 TLC262151:TLC262303 TBG262151:TBG262303 SRK262151:SRK262303 SHO262151:SHO262303 RXS262151:RXS262303 RNW262151:RNW262303 REA262151:REA262303 QUE262151:QUE262303 QKI262151:QKI262303 QAM262151:QAM262303 PQQ262151:PQQ262303 PGU262151:PGU262303 OWY262151:OWY262303 ONC262151:ONC262303 ODG262151:ODG262303 NTK262151:NTK262303 NJO262151:NJO262303 MZS262151:MZS262303 MPW262151:MPW262303 MGA262151:MGA262303 LWE262151:LWE262303 LMI262151:LMI262303 LCM262151:LCM262303 KSQ262151:KSQ262303 KIU262151:KIU262303 JYY262151:JYY262303 JPC262151:JPC262303 JFG262151:JFG262303 IVK262151:IVK262303 ILO262151:ILO262303 IBS262151:IBS262303 HRW262151:HRW262303 HIA262151:HIA262303 GYE262151:GYE262303 GOI262151:GOI262303 GEM262151:GEM262303 FUQ262151:FUQ262303 FKU262151:FKU262303 FAY262151:FAY262303 ERC262151:ERC262303 EHG262151:EHG262303 DXK262151:DXK262303 DNO262151:DNO262303 DDS262151:DDS262303 CTW262151:CTW262303 CKA262151:CKA262303 CAE262151:CAE262303 BQI262151:BQI262303 BGM262151:BGM262303 AWQ262151:AWQ262303 AMU262151:AMU262303 ACY262151:ACY262303 TC262151:TC262303 JG262151:JG262303 K262151:K262303 WVS196615:WVS196767 WLW196615:WLW196767 WCA196615:WCA196767 VSE196615:VSE196767 VII196615:VII196767 UYM196615:UYM196767 UOQ196615:UOQ196767 UEU196615:UEU196767 TUY196615:TUY196767 TLC196615:TLC196767 TBG196615:TBG196767 SRK196615:SRK196767 SHO196615:SHO196767 RXS196615:RXS196767 RNW196615:RNW196767 REA196615:REA196767 QUE196615:QUE196767 QKI196615:QKI196767 QAM196615:QAM196767 PQQ196615:PQQ196767 PGU196615:PGU196767 OWY196615:OWY196767 ONC196615:ONC196767 ODG196615:ODG196767 NTK196615:NTK196767 NJO196615:NJO196767 MZS196615:MZS196767 MPW196615:MPW196767 MGA196615:MGA196767 LWE196615:LWE196767 LMI196615:LMI196767 LCM196615:LCM196767 KSQ196615:KSQ196767 KIU196615:KIU196767 JYY196615:JYY196767 JPC196615:JPC196767 JFG196615:JFG196767 IVK196615:IVK196767 ILO196615:ILO196767 IBS196615:IBS196767 HRW196615:HRW196767 HIA196615:HIA196767 GYE196615:GYE196767 GOI196615:GOI196767 GEM196615:GEM196767 FUQ196615:FUQ196767 FKU196615:FKU196767 FAY196615:FAY196767 ERC196615:ERC196767 EHG196615:EHG196767 DXK196615:DXK196767 DNO196615:DNO196767 DDS196615:DDS196767 CTW196615:CTW196767 CKA196615:CKA196767 CAE196615:CAE196767 BQI196615:BQI196767 BGM196615:BGM196767 AWQ196615:AWQ196767 AMU196615:AMU196767 ACY196615:ACY196767 TC196615:TC196767 JG196615:JG196767 K196615:K196767 WVS131079:WVS131231 WLW131079:WLW131231 WCA131079:WCA131231 VSE131079:VSE131231 VII131079:VII131231 UYM131079:UYM131231 UOQ131079:UOQ131231 UEU131079:UEU131231 TUY131079:TUY131231 TLC131079:TLC131231 TBG131079:TBG131231 SRK131079:SRK131231 SHO131079:SHO131231 RXS131079:RXS131231 RNW131079:RNW131231 REA131079:REA131231 QUE131079:QUE131231 QKI131079:QKI131231 QAM131079:QAM131231 PQQ131079:PQQ131231 PGU131079:PGU131231 OWY131079:OWY131231 ONC131079:ONC131231 ODG131079:ODG131231 NTK131079:NTK131231 NJO131079:NJO131231 MZS131079:MZS131231 MPW131079:MPW131231 MGA131079:MGA131231 LWE131079:LWE131231 LMI131079:LMI131231 LCM131079:LCM131231 KSQ131079:KSQ131231 KIU131079:KIU131231 JYY131079:JYY131231 JPC131079:JPC131231 JFG131079:JFG131231 IVK131079:IVK131231 ILO131079:ILO131231 IBS131079:IBS131231 HRW131079:HRW131231 HIA131079:HIA131231 GYE131079:GYE131231 GOI131079:GOI131231 GEM131079:GEM131231 FUQ131079:FUQ131231 FKU131079:FKU131231 FAY131079:FAY131231 ERC131079:ERC131231 EHG131079:EHG131231 DXK131079:DXK131231 DNO131079:DNO131231 DDS131079:DDS131231 CTW131079:CTW131231 CKA131079:CKA131231 CAE131079:CAE131231 BQI131079:BQI131231 BGM131079:BGM131231 AWQ131079:AWQ131231 AMU131079:AMU131231 ACY131079:ACY131231 TC131079:TC131231 JG131079:JG131231 K131079:K131231 WVS65543:WVS65695 WLW65543:WLW65695 WCA65543:WCA65695 VSE65543:VSE65695 VII65543:VII65695 UYM65543:UYM65695 UOQ65543:UOQ65695 UEU65543:UEU65695 TUY65543:TUY65695 TLC65543:TLC65695 TBG65543:TBG65695 SRK65543:SRK65695 SHO65543:SHO65695 RXS65543:RXS65695 RNW65543:RNW65695 REA65543:REA65695 QUE65543:QUE65695 QKI65543:QKI65695 QAM65543:QAM65695 PQQ65543:PQQ65695 PGU65543:PGU65695 OWY65543:OWY65695 ONC65543:ONC65695 ODG65543:ODG65695 NTK65543:NTK65695 NJO65543:NJO65695 MZS65543:MZS65695 MPW65543:MPW65695 MGA65543:MGA65695 LWE65543:LWE65695 LMI65543:LMI65695 LCM65543:LCM65695 KSQ65543:KSQ65695 KIU65543:KIU65695 JYY65543:JYY65695 JPC65543:JPC65695 JFG65543:JFG65695 IVK65543:IVK65695 ILO65543:ILO65695 IBS65543:IBS65695 HRW65543:HRW65695 HIA65543:HIA65695 GYE65543:GYE65695 GOI65543:GOI65695 GEM65543:GEM65695 FUQ65543:FUQ65695 FKU65543:FKU65695 FAY65543:FAY65695 ERC65543:ERC65695 EHG65543:EHG65695 DXK65543:DXK65695 DNO65543:DNO65695 DDS65543:DDS65695 CTW65543:CTW65695 CKA65543:CKA65695 CAE65543:CAE65695 BQI65543:BQI65695 BGM65543:BGM65695 AWQ65543:AWQ65695 AMU65543:AMU65695 ACY65543:ACY65695 TC65543:TC65695 JG65543:JG65695 K65543:K65695 WVS7:WVS159 WLW7:WLW159 WCA7:WCA159 VSE7:VSE159 VII7:VII159 UYM7:UYM159 UOQ7:UOQ159 UEU7:UEU159 TUY7:TUY159 TLC7:TLC159 TBG7:TBG159 SRK7:SRK159 SHO7:SHO159 RXS7:RXS159 RNW7:RNW159 REA7:REA159 QUE7:QUE159 QKI7:QKI159 QAM7:QAM159 PQQ7:PQQ159 PGU7:PGU159 OWY7:OWY159 ONC7:ONC159 ODG7:ODG159 NTK7:NTK159 NJO7:NJO159 MZS7:MZS159 MPW7:MPW159 MGA7:MGA159 LWE7:LWE159 LMI7:LMI159 LCM7:LCM159 KSQ7:KSQ159 KIU7:KIU159 JYY7:JYY159 JPC7:JPC159 JFG7:JFG159 IVK7:IVK159 ILO7:ILO159 IBS7:IBS159 HRW7:HRW159 HIA7:HIA159 GYE7:GYE159 GOI7:GOI159 GEM7:GEM159 FUQ7:FUQ159 FKU7:FKU159 FAY7:FAY159 ERC7:ERC159 EHG7:EHG159 DXK7:DXK159 DNO7:DNO159 DDS7:DDS159 CTW7:CTW159 CKA7:CKA159 CAE7:CAE159 BQI7:BQI159 BGM7:BGM159 AWQ7:AWQ159 AMU7:AMU159 ACY7:ACY159 TC7:TC159 K7:K159" xr:uid="{16400355-3C3D-43F8-B702-E29A5B9CC1B1}">
       <formula1>$AQ$45:$AQ$48</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Defect Log - Updated
</commit_message>
<xml_diff>
--- a/Testing/Revised Plan.xlsx
+++ b/Testing/Revised Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Revised Plan and Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="810" documentId="8_{783EC7BA-7F55-4B35-8C25-054FADF87783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA3416E5-B615-43E0-8407-9B7C3003AA4D}"/>
+  <xr:revisionPtr revIDLastSave="839" documentId="8_{783EC7BA-7F55-4B35-8C25-054FADF87783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{304D0766-4F27-4208-B20E-52E59A0DAB1E}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="7" xr2:uid="{FF53E854-575C-4B97-B6D0-9B270F57EAA4}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="846">
   <si>
     <t>WEEK 0</t>
   </si>
@@ -3021,6 +3021,18 @@
   </si>
   <si>
     <t>Kumaresh</t>
+  </si>
+  <si>
+    <t>Filter dropdown is not working</t>
+  </si>
+  <si>
+    <t>Pagination is not there</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Gokul,Kumaresh</t>
   </si>
 </sst>
 </file>
@@ -4344,7 +4356,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="354">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4864,14 +4876,155 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4902,162 +5055,21 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5115,6 +5127,54 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5148,54 +5208,6 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5234,6 +5246,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5967,7 +5982,7 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="230" t="s">
+      <c r="D2" s="231" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -5982,7 +5997,7 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="231"/>
+      <c r="D3" s="230"/>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
@@ -5995,7 +6010,7 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="230" t="s">
+      <c r="D4" s="231" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -6010,7 +6025,7 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="230"/>
+      <c r="D5" s="231"/>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6025,7 +6040,7 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="230" t="s">
+      <c r="D6" s="231" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -6040,7 +6055,7 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="230"/>
+      <c r="D7" s="231"/>
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
@@ -6053,7 +6068,7 @@
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="230" t="s">
+      <c r="D8" s="231" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -6068,7 +6083,7 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="230"/>
+      <c r="D9" s="231"/>
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
@@ -6113,7 +6128,7 @@
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="231" t="s">
+      <c r="D12" s="230" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -6128,7 +6143,7 @@
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="231"/>
+      <c r="D13" s="230"/>
       <c r="E13" s="4" t="s">
         <v>3</v>
       </c>
@@ -6141,7 +6156,7 @@
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="231"/>
+      <c r="D14" s="230"/>
       <c r="E14" s="4" t="s">
         <v>3</v>
       </c>
@@ -6154,7 +6169,7 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="231"/>
+      <c r="D15" s="230"/>
       <c r="E15" s="4" t="s">
         <v>3</v>
       </c>
@@ -6167,7 +6182,7 @@
       <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="231"/>
+      <c r="D16" s="230"/>
       <c r="E16" s="4" t="s">
         <v>3</v>
       </c>
@@ -6197,7 +6212,7 @@
       <c r="C18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="231" t="s">
+      <c r="D18" s="230" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -6212,7 +6227,7 @@
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="231"/>
+      <c r="D19" s="230"/>
       <c r="E19" s="4" t="s">
         <v>3</v>
       </c>
@@ -6225,7 +6240,7 @@
       <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="231"/>
+      <c r="D20" s="230"/>
       <c r="E20" s="4" t="s">
         <v>3</v>
       </c>
@@ -6240,7 +6255,7 @@
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="231" t="s">
+      <c r="D21" s="230" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -6255,7 +6270,7 @@
       <c r="C22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="231"/>
+      <c r="D22" s="230"/>
       <c r="E22" s="4" t="s">
         <v>3</v>
       </c>
@@ -6268,7 +6283,7 @@
       <c r="C23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="231" t="s">
+      <c r="D23" s="230" t="s">
         <v>37</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -6283,7 +6298,7 @@
       <c r="C24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="231"/>
+      <c r="D24" s="230"/>
       <c r="E24" s="4" t="s">
         <v>3</v>
       </c>
@@ -6298,7 +6313,7 @@
       <c r="C25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="230" t="s">
+      <c r="D25" s="231" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -6313,7 +6328,7 @@
       <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="230"/>
+      <c r="D26" s="231"/>
       <c r="E26" s="4" t="s">
         <v>3</v>
       </c>
@@ -6326,7 +6341,7 @@
       <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="230"/>
+      <c r="D27" s="231"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -6337,7 +6352,7 @@
       <c r="C28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="231" t="s">
+      <c r="D28" s="230" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="4"/>
@@ -6350,7 +6365,7 @@
       <c r="C29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="231"/>
+      <c r="D29" s="230"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -6361,7 +6376,7 @@
       <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="231"/>
+      <c r="D30" s="230"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -6374,7 +6389,7 @@
       <c r="C31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="231" t="s">
+      <c r="D31" s="230" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="4"/>
@@ -6387,7 +6402,7 @@
       <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="231"/>
+      <c r="D32" s="230"/>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -6413,7 +6428,7 @@
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="231" t="s">
+      <c r="D34" s="230" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="4"/>
@@ -6426,7 +6441,7 @@
       <c r="C35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="231"/>
+      <c r="D35" s="230"/>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -6437,7 +6452,7 @@
       <c r="C36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="231"/>
+      <c r="D36" s="230"/>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -6448,7 +6463,7 @@
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="231"/>
+      <c r="D37" s="230"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -6459,7 +6474,7 @@
       <c r="C38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="230" t="s">
+      <c r="D38" s="231" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="4"/>
@@ -6472,7 +6487,7 @@
       <c r="C39" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="230"/>
+      <c r="D39" s="231"/>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -6485,7 +6500,7 @@
       <c r="C40" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="231" t="s">
+      <c r="D40" s="230" t="s">
         <v>58</v>
       </c>
       <c r="E40" s="4"/>
@@ -6498,7 +6513,7 @@
       <c r="C41" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="231"/>
+      <c r="D41" s="230"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -6509,7 +6524,7 @@
       <c r="C42" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="231"/>
+      <c r="D42" s="230"/>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -6520,7 +6535,7 @@
       <c r="C43" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="231" t="s">
+      <c r="D43" s="230" t="s">
         <v>65</v>
       </c>
       <c r="E43" s="4"/>
@@ -6533,7 +6548,7 @@
       <c r="C44" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="231"/>
+      <c r="D44" s="230"/>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -6544,11 +6559,24 @@
       <c r="C45" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="231"/>
+      <c r="D45" s="230"/>
       <c r="E45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="D43:D45"/>
@@ -6560,19 +6588,6 @@
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="D38:D39"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7578,16 +7593,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="D63:E63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D41:E41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7889,20 +7904,20 @@
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="276" t="s">
+      <c r="B4" s="242" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="277"/>
-      <c r="D4" s="277"/>
-      <c r="E4" s="277"/>
-      <c r="F4" s="277"/>
-      <c r="G4" s="277"/>
-      <c r="H4" s="277"/>
-      <c r="I4" s="277"/>
-      <c r="J4" s="277"/>
-      <c r="K4" s="277"/>
-      <c r="L4" s="277"/>
-      <c r="M4" s="278"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="243"/>
+      <c r="E4" s="243"/>
+      <c r="F4" s="243"/>
+      <c r="G4" s="243"/>
+      <c r="H4" s="243"/>
+      <c r="I4" s="243"/>
+      <c r="J4" s="243"/>
+      <c r="K4" s="243"/>
+      <c r="L4" s="243"/>
+      <c r="M4" s="244"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
@@ -7922,239 +7937,239 @@
       <c r="B6" s="255" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="257"/>
-      <c r="D6" s="283" t="s">
+      <c r="C6" s="256"/>
+      <c r="D6" s="261" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="273" t="s">
+      <c r="E6" s="272" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="274"/>
-      <c r="G6" s="274"/>
-      <c r="H6" s="274"/>
-      <c r="I6" s="274"/>
-      <c r="J6" s="274"/>
-      <c r="K6" s="274"/>
-      <c r="L6" s="274"/>
-      <c r="M6" s="275"/>
+      <c r="F6" s="273"/>
+      <c r="G6" s="273"/>
+      <c r="H6" s="273"/>
+      <c r="I6" s="273"/>
+      <c r="J6" s="273"/>
+      <c r="K6" s="273"/>
+      <c r="L6" s="273"/>
+      <c r="M6" s="274"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="258"/>
-      <c r="C7" s="260"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="247"/>
-      <c r="G7" s="247"/>
-      <c r="H7" s="247"/>
-      <c r="I7" s="247"/>
-      <c r="J7" s="247"/>
-      <c r="K7" s="247"/>
-      <c r="L7" s="247"/>
-      <c r="M7" s="248"/>
+      <c r="B7" s="257"/>
+      <c r="C7" s="258"/>
+      <c r="D7" s="262"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="250"/>
+      <c r="G7" s="250"/>
+      <c r="H7" s="250"/>
+      <c r="I7" s="250"/>
+      <c r="J7" s="250"/>
+      <c r="K7" s="250"/>
+      <c r="L7" s="250"/>
+      <c r="M7" s="251"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="258"/>
-      <c r="C8" s="260"/>
-      <c r="D8" s="243" t="s">
+      <c r="B8" s="257"/>
+      <c r="C8" s="258"/>
+      <c r="D8" s="263" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="249" t="s">
+      <c r="E8" s="268" t="s">
         <v>143</v>
       </c>
-      <c r="F8" s="247"/>
-      <c r="G8" s="247"/>
-      <c r="H8" s="247"/>
-      <c r="I8" s="247"/>
-      <c r="J8" s="247"/>
-      <c r="K8" s="247"/>
-      <c r="L8" s="247"/>
-      <c r="M8" s="248"/>
+      <c r="F8" s="250"/>
+      <c r="G8" s="250"/>
+      <c r="H8" s="250"/>
+      <c r="I8" s="250"/>
+      <c r="J8" s="250"/>
+      <c r="K8" s="250"/>
+      <c r="L8" s="250"/>
+      <c r="M8" s="251"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="261"/>
-      <c r="C9" s="263"/>
-      <c r="D9" s="243"/>
-      <c r="E9" s="246"/>
-      <c r="F9" s="247"/>
-      <c r="G9" s="247"/>
-      <c r="H9" s="247"/>
-      <c r="I9" s="247"/>
-      <c r="J9" s="247"/>
-      <c r="K9" s="247"/>
-      <c r="L9" s="247"/>
-      <c r="M9" s="248"/>
+      <c r="B9" s="259"/>
+      <c r="C9" s="260"/>
+      <c r="D9" s="263"/>
+      <c r="E9" s="249"/>
+      <c r="F9" s="250"/>
+      <c r="G9" s="250"/>
+      <c r="H9" s="250"/>
+      <c r="I9" s="250"/>
+      <c r="J9" s="250"/>
+      <c r="K9" s="250"/>
+      <c r="L9" s="250"/>
+      <c r="M9" s="251"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="255" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="256"/>
-      <c r="D10" s="257"/>
-      <c r="E10" s="280" t="s">
+      <c r="C10" s="269"/>
+      <c r="D10" s="256"/>
+      <c r="E10" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="281"/>
-      <c r="G10" s="281"/>
-      <c r="H10" s="281"/>
-      <c r="I10" s="281"/>
-      <c r="J10" s="281"/>
-      <c r="K10" s="281"/>
-      <c r="L10" s="281"/>
-      <c r="M10" s="282"/>
+      <c r="F10" s="253"/>
+      <c r="G10" s="253"/>
+      <c r="H10" s="253"/>
+      <c r="I10" s="253"/>
+      <c r="J10" s="253"/>
+      <c r="K10" s="253"/>
+      <c r="L10" s="253"/>
+      <c r="M10" s="254"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="258"/>
-      <c r="C11" s="259"/>
-      <c r="D11" s="260"/>
-      <c r="E11" s="246"/>
-      <c r="F11" s="247"/>
-      <c r="G11" s="247"/>
-      <c r="H11" s="247"/>
-      <c r="I11" s="247"/>
-      <c r="J11" s="247"/>
-      <c r="K11" s="247"/>
-      <c r="L11" s="247"/>
-      <c r="M11" s="248"/>
+      <c r="B11" s="257"/>
+      <c r="C11" s="270"/>
+      <c r="D11" s="258"/>
+      <c r="E11" s="249"/>
+      <c r="F11" s="250"/>
+      <c r="G11" s="250"/>
+      <c r="H11" s="250"/>
+      <c r="I11" s="250"/>
+      <c r="J11" s="250"/>
+      <c r="K11" s="250"/>
+      <c r="L11" s="250"/>
+      <c r="M11" s="251"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="258"/>
-      <c r="C12" s="259"/>
-      <c r="D12" s="260"/>
-      <c r="E12" s="246"/>
-      <c r="F12" s="247"/>
-      <c r="G12" s="247"/>
-      <c r="H12" s="247"/>
-      <c r="I12" s="247"/>
-      <c r="J12" s="247"/>
-      <c r="K12" s="247"/>
-      <c r="L12" s="247"/>
-      <c r="M12" s="248"/>
+      <c r="B12" s="257"/>
+      <c r="C12" s="270"/>
+      <c r="D12" s="258"/>
+      <c r="E12" s="249"/>
+      <c r="F12" s="250"/>
+      <c r="G12" s="250"/>
+      <c r="H12" s="250"/>
+      <c r="I12" s="250"/>
+      <c r="J12" s="250"/>
+      <c r="K12" s="250"/>
+      <c r="L12" s="250"/>
+      <c r="M12" s="251"/>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="261"/>
-      <c r="C13" s="262"/>
-      <c r="D13" s="263"/>
-      <c r="E13" s="246"/>
-      <c r="F13" s="247"/>
-      <c r="G13" s="247"/>
-      <c r="H13" s="247"/>
-      <c r="I13" s="247"/>
-      <c r="J13" s="247"/>
-      <c r="K13" s="247"/>
-      <c r="L13" s="247"/>
-      <c r="M13" s="248"/>
+      <c r="B13" s="259"/>
+      <c r="C13" s="271"/>
+      <c r="D13" s="260"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="250"/>
+      <c r="G13" s="250"/>
+      <c r="H13" s="250"/>
+      <c r="I13" s="250"/>
+      <c r="J13" s="250"/>
+      <c r="K13" s="250"/>
+      <c r="L13" s="250"/>
+      <c r="M13" s="251"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="255" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="256"/>
-      <c r="D14" s="257"/>
-      <c r="E14" s="249" t="s">
+      <c r="C14" s="269"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="268" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="247"/>
-      <c r="G14" s="247"/>
-      <c r="H14" s="247"/>
-      <c r="I14" s="247"/>
-      <c r="J14" s="247"/>
-      <c r="K14" s="247"/>
-      <c r="L14" s="247"/>
-      <c r="M14" s="248"/>
+      <c r="F14" s="250"/>
+      <c r="G14" s="250"/>
+      <c r="H14" s="250"/>
+      <c r="I14" s="250"/>
+      <c r="J14" s="250"/>
+      <c r="K14" s="250"/>
+      <c r="L14" s="250"/>
+      <c r="M14" s="251"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="258"/>
-      <c r="C15" s="259"/>
-      <c r="D15" s="260"/>
-      <c r="E15" s="246"/>
-      <c r="F15" s="247"/>
-      <c r="G15" s="247"/>
-      <c r="H15" s="247"/>
-      <c r="I15" s="247"/>
-      <c r="J15" s="247"/>
-      <c r="K15" s="247"/>
-      <c r="L15" s="247"/>
-      <c r="M15" s="248"/>
+      <c r="B15" s="257"/>
+      <c r="C15" s="270"/>
+      <c r="D15" s="258"/>
+      <c r="E15" s="249"/>
+      <c r="F15" s="250"/>
+      <c r="G15" s="250"/>
+      <c r="H15" s="250"/>
+      <c r="I15" s="250"/>
+      <c r="J15" s="250"/>
+      <c r="K15" s="250"/>
+      <c r="L15" s="250"/>
+      <c r="M15" s="251"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="258"/>
-      <c r="C16" s="259"/>
-      <c r="D16" s="260"/>
-      <c r="E16" s="246"/>
-      <c r="F16" s="247"/>
-      <c r="G16" s="247"/>
-      <c r="H16" s="247"/>
-      <c r="I16" s="247"/>
-      <c r="J16" s="247"/>
-      <c r="K16" s="247"/>
-      <c r="L16" s="247"/>
-      <c r="M16" s="248"/>
+      <c r="B16" s="257"/>
+      <c r="C16" s="270"/>
+      <c r="D16" s="258"/>
+      <c r="E16" s="249"/>
+      <c r="F16" s="250"/>
+      <c r="G16" s="250"/>
+      <c r="H16" s="250"/>
+      <c r="I16" s="250"/>
+      <c r="J16" s="250"/>
+      <c r="K16" s="250"/>
+      <c r="L16" s="250"/>
+      <c r="M16" s="251"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="261"/>
-      <c r="C17" s="262"/>
-      <c r="D17" s="263"/>
-      <c r="E17" s="246"/>
-      <c r="F17" s="247"/>
-      <c r="G17" s="247"/>
-      <c r="H17" s="247"/>
-      <c r="I17" s="247"/>
-      <c r="J17" s="247"/>
-      <c r="K17" s="247"/>
-      <c r="L17" s="247"/>
-      <c r="M17" s="248"/>
+      <c r="B17" s="259"/>
+      <c r="C17" s="271"/>
+      <c r="D17" s="260"/>
+      <c r="E17" s="249"/>
+      <c r="F17" s="250"/>
+      <c r="G17" s="250"/>
+      <c r="H17" s="250"/>
+      <c r="I17" s="250"/>
+      <c r="J17" s="250"/>
+      <c r="K17" s="250"/>
+      <c r="L17" s="250"/>
+      <c r="M17" s="251"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="240" t="s">
+      <c r="B18" s="287" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="241"/>
+      <c r="C18" s="288"/>
       <c r="D18" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="249" t="s">
+      <c r="E18" s="268" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="247"/>
-      <c r="G18" s="247"/>
-      <c r="H18" s="247"/>
-      <c r="I18" s="247"/>
-      <c r="J18" s="247"/>
-      <c r="K18" s="247"/>
-      <c r="L18" s="247"/>
-      <c r="M18" s="248"/>
+      <c r="F18" s="250"/>
+      <c r="G18" s="250"/>
+      <c r="H18" s="250"/>
+      <c r="I18" s="250"/>
+      <c r="J18" s="250"/>
+      <c r="K18" s="250"/>
+      <c r="L18" s="250"/>
+      <c r="M18" s="251"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="242"/>
-      <c r="C19" s="243"/>
+      <c r="B19" s="289"/>
+      <c r="C19" s="263"/>
       <c r="D19" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="249"/>
-      <c r="F19" s="247"/>
-      <c r="G19" s="247"/>
-      <c r="H19" s="247"/>
-      <c r="I19" s="247"/>
-      <c r="J19" s="247"/>
-      <c r="K19" s="247"/>
-      <c r="L19" s="247"/>
-      <c r="M19" s="248"/>
+      <c r="E19" s="268"/>
+      <c r="F19" s="250"/>
+      <c r="G19" s="250"/>
+      <c r="H19" s="250"/>
+      <c r="I19" s="250"/>
+      <c r="J19" s="250"/>
+      <c r="K19" s="250"/>
+      <c r="L19" s="250"/>
+      <c r="M19" s="251"/>
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="244"/>
-      <c r="C20" s="245"/>
+      <c r="B20" s="290"/>
+      <c r="C20" s="291"/>
       <c r="D20" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="246"/>
-      <c r="F20" s="247"/>
-      <c r="G20" s="247"/>
-      <c r="H20" s="247"/>
-      <c r="I20" s="247"/>
-      <c r="J20" s="247"/>
-      <c r="K20" s="247"/>
-      <c r="L20" s="247"/>
-      <c r="M20" s="248"/>
+      <c r="E20" s="249"/>
+      <c r="F20" s="250"/>
+      <c r="G20" s="250"/>
+      <c r="H20" s="250"/>
+      <c r="I20" s="250"/>
+      <c r="J20" s="250"/>
+      <c r="K20" s="250"/>
+      <c r="L20" s="250"/>
+      <c r="M20" s="251"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
@@ -8185,126 +8200,126 @@
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="234" t="s">
+      <c r="B23" s="281" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="235"/>
-      <c r="D23" s="235"/>
-      <c r="E23" s="235"/>
-      <c r="F23" s="235"/>
-      <c r="G23" s="235"/>
-      <c r="H23" s="235"/>
-      <c r="I23" s="235"/>
-      <c r="J23" s="235"/>
-      <c r="K23" s="235"/>
-      <c r="L23" s="235"/>
-      <c r="M23" s="236"/>
+      <c r="C23" s="282"/>
+      <c r="D23" s="282"/>
+      <c r="E23" s="282"/>
+      <c r="F23" s="282"/>
+      <c r="G23" s="282"/>
+      <c r="H23" s="282"/>
+      <c r="I23" s="282"/>
+      <c r="J23" s="282"/>
+      <c r="K23" s="282"/>
+      <c r="L23" s="282"/>
+      <c r="M23" s="283"/>
     </row>
     <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="237" t="s">
+      <c r="C24" s="284" t="s">
         <v>155</v>
       </c>
-      <c r="D24" s="239"/>
-      <c r="E24" s="237" t="s">
+      <c r="D24" s="286"/>
+      <c r="E24" s="284" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="238"/>
-      <c r="G24" s="238"/>
-      <c r="H24" s="238"/>
-      <c r="I24" s="238"/>
-      <c r="J24" s="238"/>
-      <c r="K24" s="239"/>
-      <c r="L24" s="285" t="s">
+      <c r="F24" s="285"/>
+      <c r="G24" s="285"/>
+      <c r="H24" s="285"/>
+      <c r="I24" s="285"/>
+      <c r="J24" s="285"/>
+      <c r="K24" s="286"/>
+      <c r="L24" s="264" t="s">
         <v>157</v>
       </c>
-      <c r="M24" s="286"/>
+      <c r="M24" s="265"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="13"/>
-      <c r="C25" s="250"/>
-      <c r="D25" s="252"/>
-      <c r="E25" s="250"/>
-      <c r="F25" s="251"/>
-      <c r="G25" s="251"/>
-      <c r="H25" s="251"/>
-      <c r="I25" s="251"/>
-      <c r="J25" s="251"/>
-      <c r="K25" s="252"/>
-      <c r="L25" s="250"/>
-      <c r="M25" s="279"/>
+      <c r="C25" s="245"/>
+      <c r="D25" s="293"/>
+      <c r="E25" s="245"/>
+      <c r="F25" s="292"/>
+      <c r="G25" s="292"/>
+      <c r="H25" s="292"/>
+      <c r="I25" s="292"/>
+      <c r="J25" s="292"/>
+      <c r="K25" s="293"/>
+      <c r="L25" s="245"/>
+      <c r="M25" s="246"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="253"/>
-      <c r="D26" s="254"/>
-      <c r="E26" s="253"/>
-      <c r="F26" s="270"/>
-      <c r="G26" s="270"/>
-      <c r="H26" s="270"/>
-      <c r="I26" s="270"/>
-      <c r="J26" s="270"/>
-      <c r="K26" s="254"/>
-      <c r="L26" s="253"/>
-      <c r="M26" s="272"/>
+      <c r="C26" s="247"/>
+      <c r="D26" s="267"/>
+      <c r="E26" s="247"/>
+      <c r="F26" s="266"/>
+      <c r="G26" s="266"/>
+      <c r="H26" s="266"/>
+      <c r="I26" s="266"/>
+      <c r="J26" s="266"/>
+      <c r="K26" s="267"/>
+      <c r="L26" s="247"/>
+      <c r="M26" s="248"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
-      <c r="C27" s="253"/>
-      <c r="D27" s="254"/>
-      <c r="E27" s="253"/>
-      <c r="F27" s="270"/>
-      <c r="G27" s="270"/>
-      <c r="H27" s="270"/>
-      <c r="I27" s="270"/>
-      <c r="J27" s="270"/>
-      <c r="K27" s="254"/>
-      <c r="L27" s="253"/>
-      <c r="M27" s="272"/>
+      <c r="C27" s="247"/>
+      <c r="D27" s="267"/>
+      <c r="E27" s="247"/>
+      <c r="F27" s="266"/>
+      <c r="G27" s="266"/>
+      <c r="H27" s="266"/>
+      <c r="I27" s="266"/>
+      <c r="J27" s="266"/>
+      <c r="K27" s="267"/>
+      <c r="L27" s="247"/>
+      <c r="M27" s="248"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="13"/>
-      <c r="C28" s="253"/>
-      <c r="D28" s="254"/>
-      <c r="E28" s="253"/>
-      <c r="F28" s="270"/>
-      <c r="G28" s="270"/>
-      <c r="H28" s="270"/>
-      <c r="I28" s="270"/>
-      <c r="J28" s="270"/>
-      <c r="K28" s="254"/>
-      <c r="L28" s="253"/>
-      <c r="M28" s="272"/>
+      <c r="C28" s="247"/>
+      <c r="D28" s="267"/>
+      <c r="E28" s="247"/>
+      <c r="F28" s="266"/>
+      <c r="G28" s="266"/>
+      <c r="H28" s="266"/>
+      <c r="I28" s="266"/>
+      <c r="J28" s="266"/>
+      <c r="K28" s="267"/>
+      <c r="L28" s="247"/>
+      <c r="M28" s="248"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="13"/>
-      <c r="C29" s="253"/>
-      <c r="D29" s="254"/>
-      <c r="E29" s="253"/>
-      <c r="F29" s="270"/>
-      <c r="G29" s="270"/>
-      <c r="H29" s="270"/>
-      <c r="I29" s="270"/>
-      <c r="J29" s="270"/>
-      <c r="K29" s="254"/>
-      <c r="L29" s="253"/>
-      <c r="M29" s="272"/>
+      <c r="C29" s="247"/>
+      <c r="D29" s="267"/>
+      <c r="E29" s="247"/>
+      <c r="F29" s="266"/>
+      <c r="G29" s="266"/>
+      <c r="H29" s="266"/>
+      <c r="I29" s="266"/>
+      <c r="J29" s="266"/>
+      <c r="K29" s="267"/>
+      <c r="L29" s="247"/>
+      <c r="M29" s="248"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
-      <c r="C30" s="267"/>
-      <c r="D30" s="269"/>
-      <c r="E30" s="267"/>
-      <c r="F30" s="271"/>
-      <c r="G30" s="271"/>
-      <c r="H30" s="271"/>
-      <c r="I30" s="271"/>
-      <c r="J30" s="271"/>
-      <c r="K30" s="269"/>
-      <c r="L30" s="267"/>
-      <c r="M30" s="268"/>
+      <c r="C30" s="276"/>
+      <c r="D30" s="278"/>
+      <c r="E30" s="276"/>
+      <c r="F30" s="279"/>
+      <c r="G30" s="279"/>
+      <c r="H30" s="279"/>
+      <c r="I30" s="279"/>
+      <c r="J30" s="279"/>
+      <c r="K30" s="278"/>
+      <c r="L30" s="276"/>
+      <c r="M30" s="277"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
@@ -8321,20 +8336,20 @@
       <c r="M31" s="12"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="234" t="s">
+      <c r="B32" s="281" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="235"/>
-      <c r="D32" s="235"/>
-      <c r="E32" s="235"/>
-      <c r="F32" s="235"/>
-      <c r="G32" s="235"/>
-      <c r="H32" s="235"/>
-      <c r="I32" s="235"/>
-      <c r="J32" s="235"/>
-      <c r="K32" s="235"/>
-      <c r="L32" s="235"/>
-      <c r="M32" s="236"/>
+      <c r="C32" s="282"/>
+      <c r="D32" s="282"/>
+      <c r="E32" s="282"/>
+      <c r="F32" s="282"/>
+      <c r="G32" s="282"/>
+      <c r="H32" s="282"/>
+      <c r="I32" s="282"/>
+      <c r="J32" s="282"/>
+      <c r="K32" s="282"/>
+      <c r="L32" s="282"/>
+      <c r="M32" s="283"/>
     </row>
     <row r="33" spans="2:13" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="26" t="s">
@@ -8343,10 +8358,10 @@
       <c r="C33" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="D33" s="237" t="s">
+      <c r="D33" s="284" t="s">
         <v>161</v>
       </c>
-      <c r="E33" s="239"/>
+      <c r="E33" s="286"/>
       <c r="F33" s="27" t="s">
         <v>162</v>
       </c>
@@ -8377,8 +8392,8 @@
         <v>1</v>
       </c>
       <c r="C34" s="22"/>
-      <c r="D34" s="264"/>
-      <c r="E34" s="264"/>
+      <c r="D34" s="294"/>
+      <c r="E34" s="294"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
@@ -8393,8 +8408,8 @@
         <v>2</v>
       </c>
       <c r="C35" s="17"/>
-      <c r="D35" s="265"/>
-      <c r="E35" s="265"/>
+      <c r="D35" s="241"/>
+      <c r="E35" s="241"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -8409,8 +8424,8 @@
         <v>3</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="265"/>
-      <c r="E36" s="265"/>
+      <c r="D36" s="241"/>
+      <c r="E36" s="241"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
@@ -8425,8 +8440,8 @@
         <v>4</v>
       </c>
       <c r="C37" s="29"/>
-      <c r="D37" s="266"/>
-      <c r="E37" s="266"/>
+      <c r="D37" s="275"/>
+      <c r="E37" s="275"/>
       <c r="F37" s="30"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
@@ -8439,8 +8454,8 @@
     <row r="38" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="33"/>
       <c r="C38" s="34"/>
-      <c r="D38" s="233"/>
-      <c r="E38" s="233"/>
+      <c r="D38" s="280"/>
+      <c r="E38" s="280"/>
       <c r="F38" s="34"/>
       <c r="G38" s="34" t="s">
         <v>169</v>
@@ -8461,16 +8476,16 @@
       <c r="M38" s="36"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="291" t="s">
+      <c r="B41" s="237" t="s">
         <v>170</v>
       </c>
-      <c r="C41" s="291"/>
-      <c r="D41" s="291"/>
-      <c r="E41" s="291"/>
-      <c r="F41" s="291"/>
-      <c r="G41" s="291"/>
-      <c r="H41" s="291"/>
-      <c r="I41" s="291"/>
+      <c r="C41" s="237"/>
+      <c r="D41" s="237"/>
+      <c r="E41" s="237"/>
+      <c r="F41" s="237"/>
+      <c r="G41" s="237"/>
+      <c r="H41" s="237"/>
+      <c r="I41" s="237"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
@@ -8483,16 +8498,16 @@
       <c r="C42" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="290" t="s">
+      <c r="D42" s="236" t="s">
         <v>172</v>
       </c>
-      <c r="E42" s="290"/>
-      <c r="F42" s="290" t="s">
+      <c r="E42" s="236"/>
+      <c r="F42" s="236" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="290"/>
-      <c r="H42" s="290"/>
-      <c r="I42" s="290"/>
+      <c r="G42" s="236"/>
+      <c r="H42" s="236"/>
+      <c r="I42" s="236"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
@@ -8503,8 +8518,8 @@
         <v>1</v>
       </c>
       <c r="C43" s="17"/>
-      <c r="D43" s="265"/>
-      <c r="E43" s="265"/>
+      <c r="D43" s="241"/>
+      <c r="E43" s="241"/>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
@@ -8519,8 +8534,8 @@
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="265"/>
-      <c r="E44" s="265"/>
+      <c r="D44" s="241"/>
+      <c r="E44" s="241"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -8535,8 +8550,8 @@
         <v>3</v>
       </c>
       <c r="C45" s="17"/>
-      <c r="D45" s="265"/>
-      <c r="E45" s="265"/>
+      <c r="D45" s="241"/>
+      <c r="E45" s="241"/>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
@@ -8547,16 +8562,16 @@
       <c r="M45" s="12"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="291" t="s">
+      <c r="B47" s="237" t="s">
         <v>174</v>
       </c>
-      <c r="C47" s="291"/>
-      <c r="D47" s="291"/>
-      <c r="E47" s="291"/>
-      <c r="F47" s="291"/>
-      <c r="G47" s="291"/>
-      <c r="H47" s="291"/>
-      <c r="I47" s="291"/>
+      <c r="C47" s="237"/>
+      <c r="D47" s="237"/>
+      <c r="E47" s="237"/>
+      <c r="F47" s="237"/>
+      <c r="G47" s="237"/>
+      <c r="H47" s="237"/>
+      <c r="I47" s="237"/>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
@@ -8569,14 +8584,14 @@
       <c r="C48" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="D48" s="292" t="s">
+      <c r="D48" s="238" t="s">
         <v>176</v>
       </c>
-      <c r="E48" s="293"/>
-      <c r="F48" s="293"/>
-      <c r="G48" s="293"/>
-      <c r="H48" s="293"/>
-      <c r="I48" s="294"/>
+      <c r="E48" s="239"/>
+      <c r="F48" s="239"/>
+      <c r="G48" s="239"/>
+      <c r="H48" s="239"/>
+      <c r="I48" s="240"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
@@ -8589,12 +8604,12 @@
       <c r="C49" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D49" s="287"/>
-      <c r="E49" s="288"/>
-      <c r="F49" s="288"/>
-      <c r="G49" s="288"/>
-      <c r="H49" s="288"/>
-      <c r="I49" s="289"/>
+      <c r="D49" s="233"/>
+      <c r="E49" s="234"/>
+      <c r="F49" s="234"/>
+      <c r="G49" s="234"/>
+      <c r="H49" s="234"/>
+      <c r="I49" s="235"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="17">
@@ -8603,12 +8618,12 @@
       <c r="C50" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D50" s="287"/>
-      <c r="E50" s="288"/>
-      <c r="F50" s="288"/>
-      <c r="G50" s="288"/>
-      <c r="H50" s="288"/>
-      <c r="I50" s="289"/>
+      <c r="D50" s="233"/>
+      <c r="E50" s="234"/>
+      <c r="F50" s="234"/>
+      <c r="G50" s="234"/>
+      <c r="H50" s="234"/>
+      <c r="I50" s="235"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="17">
@@ -8617,77 +8632,128 @@
       <c r="C51" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D51" s="287"/>
-      <c r="E51" s="288"/>
-      <c r="F51" s="288"/>
-      <c r="G51" s="288"/>
-      <c r="H51" s="288"/>
-      <c r="I51" s="289"/>
+      <c r="D51" s="233"/>
+      <c r="E51" s="234"/>
+      <c r="F51" s="234"/>
+      <c r="G51" s="234"/>
+      <c r="H51" s="234"/>
+      <c r="I51" s="235"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="291" t="s">
+      <c r="B54" s="237" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="291"/>
-      <c r="D54" s="291"/>
-      <c r="E54" s="291"/>
-      <c r="F54" s="291"/>
-      <c r="G54" s="291"/>
-      <c r="H54" s="291"/>
-      <c r="I54" s="291"/>
+      <c r="C54" s="237"/>
+      <c r="D54" s="237"/>
+      <c r="E54" s="237"/>
+      <c r="F54" s="237"/>
+      <c r="G54" s="237"/>
+      <c r="H54" s="237"/>
+      <c r="I54" s="237"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="C55" s="292" t="s">
+      <c r="C55" s="238" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="293"/>
-      <c r="E55" s="293"/>
-      <c r="F55" s="293"/>
-      <c r="G55" s="293"/>
-      <c r="H55" s="293"/>
-      <c r="I55" s="294"/>
+      <c r="D55" s="239"/>
+      <c r="E55" s="239"/>
+      <c r="F55" s="239"/>
+      <c r="G55" s="239"/>
+      <c r="H55" s="239"/>
+      <c r="I55" s="240"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="17">
         <v>1</v>
       </c>
-      <c r="C56" s="287"/>
-      <c r="D56" s="288"/>
-      <c r="E56" s="288"/>
-      <c r="F56" s="288"/>
-      <c r="G56" s="288"/>
-      <c r="H56" s="288"/>
-      <c r="I56" s="289"/>
+      <c r="C56" s="233"/>
+      <c r="D56" s="234"/>
+      <c r="E56" s="234"/>
+      <c r="F56" s="234"/>
+      <c r="G56" s="234"/>
+      <c r="H56" s="234"/>
+      <c r="I56" s="235"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="17">
         <v>2</v>
       </c>
-      <c r="C57" s="287"/>
-      <c r="D57" s="288"/>
-      <c r="E57" s="288"/>
-      <c r="F57" s="288"/>
-      <c r="G57" s="288"/>
-      <c r="H57" s="288"/>
-      <c r="I57" s="289"/>
+      <c r="C57" s="233"/>
+      <c r="D57" s="234"/>
+      <c r="E57" s="234"/>
+      <c r="F57" s="234"/>
+      <c r="G57" s="234"/>
+      <c r="H57" s="234"/>
+      <c r="I57" s="235"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="17">
         <v>3</v>
       </c>
-      <c r="C58" s="287"/>
-      <c r="D58" s="288"/>
-      <c r="E58" s="288"/>
-      <c r="F58" s="288"/>
-      <c r="G58" s="288"/>
-      <c r="H58" s="288"/>
-      <c r="I58" s="289"/>
+      <c r="C58" s="233"/>
+      <c r="D58" s="234"/>
+      <c r="E58" s="234"/>
+      <c r="F58" s="234"/>
+      <c r="G58" s="234"/>
+      <c r="H58" s="234"/>
+      <c r="I58" s="235"/>
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="E24:K24"/>
+    <mergeCell ref="B18:C20"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E18:M18"/>
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B14:D17"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E27:K27"/>
+    <mergeCell ref="E28:K28"/>
+    <mergeCell ref="E29:K29"/>
+    <mergeCell ref="E30:K30"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="E15:M15"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="B10:D13"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="E7:M7"/>
+    <mergeCell ref="E8:M8"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="B6:C9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="E13:M13"/>
+    <mergeCell ref="E14:M14"/>
     <mergeCell ref="C57:I57"/>
     <mergeCell ref="C58:I58"/>
     <mergeCell ref="F42:I42"/>
@@ -8704,57 +8770,6 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="C56:I56"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E10:M10"/>
-    <mergeCell ref="B6:C9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="E11:M11"/>
-    <mergeCell ref="E12:M12"/>
-    <mergeCell ref="E13:M13"/>
-    <mergeCell ref="E14:M14"/>
-    <mergeCell ref="E15:M15"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="B10:D13"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="E7:M7"/>
-    <mergeCell ref="E8:M8"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E27:K27"/>
-    <mergeCell ref="E28:K28"/>
-    <mergeCell ref="E29:K29"/>
-    <mergeCell ref="E30:K30"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="E24:K24"/>
-    <mergeCell ref="B18:C20"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="E18:M18"/>
-    <mergeCell ref="E19:M19"/>
-    <mergeCell ref="E20:M20"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B14:D17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10546,34 +10561,34 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="328" t="s">
+      <c r="B2" s="317" t="s">
         <v>387</v>
       </c>
-      <c r="C2" s="329"/>
-      <c r="D2" s="329"/>
-      <c r="E2" s="329"/>
-      <c r="F2" s="329"/>
-      <c r="G2" s="329"/>
-      <c r="H2" s="329"/>
-      <c r="I2" s="329"/>
-      <c r="J2" s="329"/>
-      <c r="K2" s="330"/>
-      <c r="L2" s="331"/>
+      <c r="C2" s="318"/>
+      <c r="D2" s="318"/>
+      <c r="E2" s="318"/>
+      <c r="F2" s="318"/>
+      <c r="G2" s="318"/>
+      <c r="H2" s="318"/>
+      <c r="I2" s="318"/>
+      <c r="J2" s="318"/>
+      <c r="K2" s="319"/>
+      <c r="L2" s="320"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="332" t="s">
+      <c r="B3" s="321" t="s">
         <v>388</v>
       </c>
-      <c r="C3" s="333"/>
-      <c r="D3" s="333"/>
-      <c r="E3" s="333"/>
-      <c r="F3" s="333"/>
-      <c r="G3" s="333"/>
-      <c r="H3" s="333"/>
-      <c r="I3" s="333"/>
-      <c r="J3" s="333"/>
-      <c r="K3" s="334"/>
-      <c r="L3" s="335"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
+      <c r="I3" s="322"/>
+      <c r="J3" s="322"/>
+      <c r="K3" s="323"/>
+      <c r="L3" s="324"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="308" t="s">
@@ -10587,7 +10602,7 @@
       <c r="H4" s="309"/>
       <c r="I4" s="309"/>
       <c r="J4" s="309"/>
-      <c r="K4" s="336"/>
+      <c r="K4" s="325"/>
       <c r="L4" s="310"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -10602,53 +10617,53 @@
       <c r="H5" s="298"/>
       <c r="I5" s="298"/>
       <c r="J5" s="298"/>
-      <c r="K5" s="337"/>
+      <c r="K5" s="326"/>
       <c r="L5" s="299"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="338" t="s">
+      <c r="B6" s="327" t="s">
         <v>389</v>
       </c>
-      <c r="C6" s="339"/>
-      <c r="D6" s="339"/>
-      <c r="E6" s="339"/>
-      <c r="F6" s="339"/>
-      <c r="G6" s="339"/>
-      <c r="H6" s="339"/>
-      <c r="I6" s="339"/>
-      <c r="J6" s="339"/>
-      <c r="K6" s="339"/>
-      <c r="L6" s="340"/>
+      <c r="C6" s="328"/>
+      <c r="D6" s="328"/>
+      <c r="E6" s="328"/>
+      <c r="F6" s="328"/>
+      <c r="G6" s="328"/>
+      <c r="H6" s="328"/>
+      <c r="I6" s="328"/>
+      <c r="J6" s="328"/>
+      <c r="K6" s="328"/>
+      <c r="L6" s="329"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="325" t="s">
+      <c r="B7" s="314" t="s">
         <v>390</v>
       </c>
-      <c r="C7" s="326"/>
-      <c r="D7" s="326"/>
-      <c r="E7" s="326"/>
-      <c r="F7" s="326"/>
-      <c r="G7" s="326"/>
-      <c r="H7" s="326"/>
-      <c r="I7" s="326"/>
-      <c r="J7" s="326"/>
-      <c r="K7" s="326"/>
-      <c r="L7" s="327"/>
+      <c r="C7" s="315"/>
+      <c r="D7" s="315"/>
+      <c r="E7" s="315"/>
+      <c r="F7" s="315"/>
+      <c r="G7" s="315"/>
+      <c r="H7" s="315"/>
+      <c r="I7" s="315"/>
+      <c r="J7" s="315"/>
+      <c r="K7" s="315"/>
+      <c r="L7" s="316"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="318" t="s">
+      <c r="B8" s="334" t="s">
         <v>391</v>
       </c>
-      <c r="C8" s="319"/>
-      <c r="D8" s="319"/>
-      <c r="E8" s="319"/>
-      <c r="F8" s="319"/>
-      <c r="G8" s="319"/>
-      <c r="H8" s="319"/>
-      <c r="I8" s="319"/>
-      <c r="J8" s="319"/>
-      <c r="K8" s="319"/>
-      <c r="L8" s="320"/>
+      <c r="C8" s="335"/>
+      <c r="D8" s="335"/>
+      <c r="E8" s="335"/>
+      <c r="F8" s="335"/>
+      <c r="G8" s="335"/>
+      <c r="H8" s="335"/>
+      <c r="I8" s="335"/>
+      <c r="J8" s="335"/>
+      <c r="K8" s="335"/>
+      <c r="L8" s="336"/>
     </row>
     <row r="9" spans="2:12" ht="33" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
@@ -11984,19 +11999,19 @@
       <c r="L65" s="51"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B66" s="321" t="s">
+      <c r="B66" s="337" t="s">
         <v>382</v>
       </c>
-      <c r="C66" s="322"/>
-      <c r="D66" s="322"/>
-      <c r="E66" s="322"/>
-      <c r="F66" s="322"/>
-      <c r="G66" s="322"/>
-      <c r="H66" s="322"/>
-      <c r="I66" s="322"/>
-      <c r="J66" s="322"/>
-      <c r="K66" s="323"/>
-      <c r="L66" s="324"/>
+      <c r="C66" s="338"/>
+      <c r="D66" s="338"/>
+      <c r="E66" s="338"/>
+      <c r="F66" s="338"/>
+      <c r="G66" s="338"/>
+      <c r="H66" s="338"/>
+      <c r="I66" s="338"/>
+      <c r="J66" s="338"/>
+      <c r="K66" s="339"/>
+      <c r="L66" s="340"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="303" t="s">
@@ -12005,15 +12020,15 @@
       <c r="C67" s="304"/>
       <c r="D67" s="304"/>
       <c r="E67" s="52"/>
-      <c r="F67" s="314" t="s">
+      <c r="F67" s="330" t="s">
         <v>191</v>
       </c>
-      <c r="G67" s="314"/>
-      <c r="H67" s="314"/>
-      <c r="I67" s="314"/>
-      <c r="J67" s="314"/>
-      <c r="K67" s="314"/>
-      <c r="L67" s="315"/>
+      <c r="G67" s="330"/>
+      <c r="H67" s="330"/>
+      <c r="I67" s="330"/>
+      <c r="J67" s="330"/>
+      <c r="K67" s="330"/>
+      <c r="L67" s="331"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="303" t="s">
@@ -12022,13 +12037,13 @@
       <c r="C68" s="304"/>
       <c r="D68" s="304"/>
       <c r="E68" s="52"/>
-      <c r="F68" s="314"/>
-      <c r="G68" s="314"/>
-      <c r="H68" s="314"/>
-      <c r="I68" s="314"/>
-      <c r="J68" s="314"/>
-      <c r="K68" s="314"/>
-      <c r="L68" s="315"/>
+      <c r="F68" s="330"/>
+      <c r="G68" s="330"/>
+      <c r="H68" s="330"/>
+      <c r="I68" s="330"/>
+      <c r="J68" s="330"/>
+      <c r="K68" s="330"/>
+      <c r="L68" s="331"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="303" t="s">
@@ -12037,15 +12052,15 @@
       <c r="C69" s="304"/>
       <c r="D69" s="304"/>
       <c r="E69" s="52"/>
-      <c r="F69" s="314" t="s">
+      <c r="F69" s="330" t="s">
         <v>191</v>
       </c>
-      <c r="G69" s="314"/>
-      <c r="H69" s="314"/>
-      <c r="I69" s="314"/>
-      <c r="J69" s="314"/>
-      <c r="K69" s="314"/>
-      <c r="L69" s="315"/>
+      <c r="G69" s="330"/>
+      <c r="H69" s="330"/>
+      <c r="I69" s="330"/>
+      <c r="J69" s="330"/>
+      <c r="K69" s="330"/>
+      <c r="L69" s="331"/>
     </row>
     <row r="70" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B70" s="295" t="s">
@@ -12054,22 +12069,16 @@
       <c r="C70" s="296"/>
       <c r="D70" s="296"/>
       <c r="E70" s="53"/>
-      <c r="F70" s="316"/>
-      <c r="G70" s="316"/>
-      <c r="H70" s="316"/>
-      <c r="I70" s="316"/>
-      <c r="J70" s="316"/>
-      <c r="K70" s="316"/>
-      <c r="L70" s="317"/>
+      <c r="F70" s="332"/>
+      <c r="G70" s="332"/>
+      <c r="H70" s="332"/>
+      <c r="I70" s="332"/>
+      <c r="J70" s="332"/>
+      <c r="K70" s="332"/>
+      <c r="L70" s="333"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:L5"/>
-    <mergeCell ref="B6:L6"/>
     <mergeCell ref="B69:D69"/>
     <mergeCell ref="F69:L69"/>
     <mergeCell ref="B70:D70"/>
@@ -12080,6 +12089,12 @@
     <mergeCell ref="F67:L67"/>
     <mergeCell ref="B68:D68"/>
     <mergeCell ref="F68:L68"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="B6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12089,8 +12104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F031F4EE-3EC7-47DE-91AF-34380ED2D64A}">
   <dimension ref="B1:AO158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C90" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="G82" workbookViewId="0">
+      <selection activeCell="N95" sqref="N95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18143,8 +18158,8 @@
       <c r="E71" s="189" t="s">
         <v>780</v>
       </c>
-      <c r="F71" s="189" t="s">
-        <v>626</v>
+      <c r="F71" s="211" t="s">
+        <v>640</v>
       </c>
       <c r="G71" s="190" t="s">
         <v>631</v>
@@ -18193,8 +18208,8 @@
       <c r="E72" s="189" t="s">
         <v>781</v>
       </c>
-      <c r="F72" s="189" t="s">
-        <v>626</v>
+      <c r="F72" s="211" t="s">
+        <v>640</v>
       </c>
       <c r="G72" s="190" t="s">
         <v>631</v>
@@ -18243,8 +18258,8 @@
       <c r="E73" s="189" t="s">
         <v>782</v>
       </c>
-      <c r="F73" s="189" t="s">
-        <v>626</v>
+      <c r="F73" s="211" t="s">
+        <v>640</v>
       </c>
       <c r="G73" s="190" t="s">
         <v>631</v>
@@ -18293,8 +18308,8 @@
       <c r="E74" s="189" t="s">
         <v>783</v>
       </c>
-      <c r="F74" s="189" t="s">
-        <v>626</v>
+      <c r="F74" s="211" t="s">
+        <v>640</v>
       </c>
       <c r="G74" s="190" t="s">
         <v>631</v>
@@ -18530,7 +18545,7 @@
       <c r="V78" s="54"/>
       <c r="AF78" s="60"/>
     </row>
-    <row r="79" spans="2:41" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="192">
         <v>73</v>
       </c>
@@ -19251,7 +19266,9 @@
         <v>616</v>
       </c>
       <c r="M93" s="54"/>
-      <c r="N93" s="54"/>
+      <c r="N93" s="54" t="s">
+        <v>803</v>
+      </c>
       <c r="O93" s="54"/>
       <c r="P93" s="54"/>
       <c r="Q93" s="56"/>
@@ -19297,7 +19314,9 @@
         <v>616</v>
       </c>
       <c r="M94" s="54"/>
-      <c r="N94" s="54"/>
+      <c r="N94" s="54" t="s">
+        <v>803</v>
+      </c>
       <c r="O94" s="54"/>
       <c r="P94" s="54"/>
       <c r="Q94" s="56"/>
@@ -19588,7 +19607,9 @@
       <c r="N100" s="54" t="s">
         <v>835</v>
       </c>
-      <c r="O100" s="54"/>
+      <c r="O100" s="218">
+        <v>44757</v>
+      </c>
       <c r="P100" s="54"/>
       <c r="Q100" s="56"/>
       <c r="R100" s="54"/>
@@ -19897,18 +19918,32 @@
       <c r="B107" s="192">
         <v>101</v>
       </c>
-      <c r="C107" s="54"/>
-      <c r="D107" s="54"/>
-      <c r="E107" s="54"/>
-      <c r="F107" s="54"/>
-      <c r="G107" s="58"/>
-      <c r="H107" s="54"/>
+      <c r="C107" s="54" t="s">
+        <v>772</v>
+      </c>
+      <c r="D107" s="54" t="s">
+        <v>832</v>
+      </c>
+      <c r="E107" s="54" t="s">
+        <v>841</v>
+      </c>
+      <c r="F107" s="54" t="s">
+        <v>626</v>
+      </c>
+      <c r="G107" s="58" t="s">
+        <v>627</v>
+      </c>
+      <c r="H107" s="54" t="s">
+        <v>623</v>
+      </c>
       <c r="I107" s="54"/>
       <c r="J107" s="56"/>
       <c r="K107" s="57"/>
       <c r="L107" s="56"/>
       <c r="M107" s="54"/>
-      <c r="N107" s="54"/>
+      <c r="N107" s="54" t="s">
+        <v>805</v>
+      </c>
       <c r="O107" s="54"/>
       <c r="P107" s="54"/>
       <c r="Q107" s="56"/>
@@ -19922,18 +19957,32 @@
       <c r="B108" s="192">
         <v>102</v>
       </c>
-      <c r="C108" s="54"/>
-      <c r="D108" s="54"/>
-      <c r="E108" s="54"/>
-      <c r="F108" s="54"/>
-      <c r="G108" s="58"/>
-      <c r="H108" s="54"/>
+      <c r="C108" s="54" t="s">
+        <v>772</v>
+      </c>
+      <c r="D108" s="54" t="s">
+        <v>716</v>
+      </c>
+      <c r="E108" s="54" t="s">
+        <v>841</v>
+      </c>
+      <c r="F108" s="54" t="s">
+        <v>626</v>
+      </c>
+      <c r="G108" s="58" t="s">
+        <v>627</v>
+      </c>
+      <c r="H108" s="54" t="s">
+        <v>623</v>
+      </c>
       <c r="I108" s="54"/>
       <c r="J108" s="56"/>
       <c r="K108" s="57"/>
       <c r="L108" s="56"/>
       <c r="M108" s="54"/>
-      <c r="N108" s="54"/>
+      <c r="N108" s="54" t="s">
+        <v>805</v>
+      </c>
       <c r="O108" s="54"/>
       <c r="P108" s="54"/>
       <c r="Q108" s="56"/>
@@ -19947,18 +19996,32 @@
       <c r="B109" s="192">
         <v>103</v>
       </c>
-      <c r="C109" s="54"/>
-      <c r="D109" s="54"/>
-      <c r="E109" s="54"/>
-      <c r="F109" s="54"/>
-      <c r="G109" s="58"/>
-      <c r="H109" s="54"/>
+      <c r="C109" s="54" t="s">
+        <v>843</v>
+      </c>
+      <c r="D109" s="54" t="s">
+        <v>832</v>
+      </c>
+      <c r="E109" s="54" t="s">
+        <v>842</v>
+      </c>
+      <c r="F109" s="227" t="s">
+        <v>640</v>
+      </c>
+      <c r="G109" s="58" t="s">
+        <v>631</v>
+      </c>
+      <c r="H109" s="54" t="s">
+        <v>637</v>
+      </c>
       <c r="I109" s="54"/>
       <c r="J109" s="56"/>
       <c r="K109" s="57"/>
       <c r="L109" s="56"/>
       <c r="M109" s="54"/>
-      <c r="N109" s="54"/>
+      <c r="N109" s="54" t="s">
+        <v>844</v>
+      </c>
       <c r="O109" s="54"/>
       <c r="P109" s="54"/>
       <c r="Q109" s="56"/>
@@ -19974,7 +20037,7 @@
       </c>
       <c r="C110" s="54"/>
       <c r="D110" s="54"/>
-      <c r="E110" s="54"/>
+      <c r="E110" s="354"/>
       <c r="F110" s="54"/>
       <c r="G110" s="58"/>
       <c r="H110" s="54"/>
@@ -21110,7 +21173,7 @@
     <mergeCell ref="AJ44:AJ55"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVE983045:WVE983198 F6 F65541:F65694 IS65541:IS65694 SO65541:SO65694 ACK65541:ACK65694 AMG65541:AMG65694 AWC65541:AWC65694 BFY65541:BFY65694 BPU65541:BPU65694 BZQ65541:BZQ65694 CJM65541:CJM65694 CTI65541:CTI65694 DDE65541:DDE65694 DNA65541:DNA65694 DWW65541:DWW65694 EGS65541:EGS65694 EQO65541:EQO65694 FAK65541:FAK65694 FKG65541:FKG65694 FUC65541:FUC65694 GDY65541:GDY65694 GNU65541:GNU65694 GXQ65541:GXQ65694 HHM65541:HHM65694 HRI65541:HRI65694 IBE65541:IBE65694 ILA65541:ILA65694 IUW65541:IUW65694 JES65541:JES65694 JOO65541:JOO65694 JYK65541:JYK65694 KIG65541:KIG65694 KSC65541:KSC65694 LBY65541:LBY65694 LLU65541:LLU65694 LVQ65541:LVQ65694 MFM65541:MFM65694 MPI65541:MPI65694 MZE65541:MZE65694 NJA65541:NJA65694 NSW65541:NSW65694 OCS65541:OCS65694 OMO65541:OMO65694 OWK65541:OWK65694 PGG65541:PGG65694 PQC65541:PQC65694 PZY65541:PZY65694 QJU65541:QJU65694 QTQ65541:QTQ65694 RDM65541:RDM65694 RNI65541:RNI65694 RXE65541:RXE65694 SHA65541:SHA65694 SQW65541:SQW65694 TAS65541:TAS65694 TKO65541:TKO65694 TUK65541:TUK65694 UEG65541:UEG65694 UOC65541:UOC65694 UXY65541:UXY65694 VHU65541:VHU65694 VRQ65541:VRQ65694 WBM65541:WBM65694 WLI65541:WLI65694 WVE65541:WVE65694 F131077:F131230 IS131077:IS131230 SO131077:SO131230 ACK131077:ACK131230 AMG131077:AMG131230 AWC131077:AWC131230 BFY131077:BFY131230 BPU131077:BPU131230 BZQ131077:BZQ131230 CJM131077:CJM131230 CTI131077:CTI131230 DDE131077:DDE131230 DNA131077:DNA131230 DWW131077:DWW131230 EGS131077:EGS131230 EQO131077:EQO131230 FAK131077:FAK131230 FKG131077:FKG131230 FUC131077:FUC131230 GDY131077:GDY131230 GNU131077:GNU131230 GXQ131077:GXQ131230 HHM131077:HHM131230 HRI131077:HRI131230 IBE131077:IBE131230 ILA131077:ILA131230 IUW131077:IUW131230 JES131077:JES131230 JOO131077:JOO131230 JYK131077:JYK131230 KIG131077:KIG131230 KSC131077:KSC131230 LBY131077:LBY131230 LLU131077:LLU131230 LVQ131077:LVQ131230 MFM131077:MFM131230 MPI131077:MPI131230 MZE131077:MZE131230 NJA131077:NJA131230 NSW131077:NSW131230 OCS131077:OCS131230 OMO131077:OMO131230 OWK131077:OWK131230 PGG131077:PGG131230 PQC131077:PQC131230 PZY131077:PZY131230 QJU131077:QJU131230 QTQ131077:QTQ131230 RDM131077:RDM131230 RNI131077:RNI131230 RXE131077:RXE131230 SHA131077:SHA131230 SQW131077:SQW131230 TAS131077:TAS131230 TKO131077:TKO131230 TUK131077:TUK131230 UEG131077:UEG131230 UOC131077:UOC131230 UXY131077:UXY131230 VHU131077:VHU131230 VRQ131077:VRQ131230 WBM131077:WBM131230 WLI131077:WLI131230 WVE131077:WVE131230 F196613:F196766 IS196613:IS196766 SO196613:SO196766 ACK196613:ACK196766 AMG196613:AMG196766 AWC196613:AWC196766 BFY196613:BFY196766 BPU196613:BPU196766 BZQ196613:BZQ196766 CJM196613:CJM196766 CTI196613:CTI196766 DDE196613:DDE196766 DNA196613:DNA196766 DWW196613:DWW196766 EGS196613:EGS196766 EQO196613:EQO196766 FAK196613:FAK196766 FKG196613:FKG196766 FUC196613:FUC196766 GDY196613:GDY196766 GNU196613:GNU196766 GXQ196613:GXQ196766 HHM196613:HHM196766 HRI196613:HRI196766 IBE196613:IBE196766 ILA196613:ILA196766 IUW196613:IUW196766 JES196613:JES196766 JOO196613:JOO196766 JYK196613:JYK196766 KIG196613:KIG196766 KSC196613:KSC196766 LBY196613:LBY196766 LLU196613:LLU196766 LVQ196613:LVQ196766 MFM196613:MFM196766 MPI196613:MPI196766 MZE196613:MZE196766 NJA196613:NJA196766 NSW196613:NSW196766 OCS196613:OCS196766 OMO196613:OMO196766 OWK196613:OWK196766 PGG196613:PGG196766 PQC196613:PQC196766 PZY196613:PZY196766 QJU196613:QJU196766 QTQ196613:QTQ196766 RDM196613:RDM196766 RNI196613:RNI196766 RXE196613:RXE196766 SHA196613:SHA196766 SQW196613:SQW196766 TAS196613:TAS196766 TKO196613:TKO196766 TUK196613:TUK196766 UEG196613:UEG196766 UOC196613:UOC196766 UXY196613:UXY196766 VHU196613:VHU196766 VRQ196613:VRQ196766 WBM196613:WBM196766 WLI196613:WLI196766 WVE196613:WVE196766 F262149:F262302 IS262149:IS262302 SO262149:SO262302 ACK262149:ACK262302 AMG262149:AMG262302 AWC262149:AWC262302 BFY262149:BFY262302 BPU262149:BPU262302 BZQ262149:BZQ262302 CJM262149:CJM262302 CTI262149:CTI262302 DDE262149:DDE262302 DNA262149:DNA262302 DWW262149:DWW262302 EGS262149:EGS262302 EQO262149:EQO262302 FAK262149:FAK262302 FKG262149:FKG262302 FUC262149:FUC262302 GDY262149:GDY262302 GNU262149:GNU262302 GXQ262149:GXQ262302 HHM262149:HHM262302 HRI262149:HRI262302 IBE262149:IBE262302 ILA262149:ILA262302 IUW262149:IUW262302 JES262149:JES262302 JOO262149:JOO262302 JYK262149:JYK262302 KIG262149:KIG262302 KSC262149:KSC262302 LBY262149:LBY262302 LLU262149:LLU262302 LVQ262149:LVQ262302 MFM262149:MFM262302 MPI262149:MPI262302 MZE262149:MZE262302 NJA262149:NJA262302 NSW262149:NSW262302 OCS262149:OCS262302 OMO262149:OMO262302 OWK262149:OWK262302 PGG262149:PGG262302 PQC262149:PQC262302 PZY262149:PZY262302 QJU262149:QJU262302 QTQ262149:QTQ262302 RDM262149:RDM262302 RNI262149:RNI262302 RXE262149:RXE262302 SHA262149:SHA262302 SQW262149:SQW262302 TAS262149:TAS262302 TKO262149:TKO262302 TUK262149:TUK262302 UEG262149:UEG262302 UOC262149:UOC262302 UXY262149:UXY262302 VHU262149:VHU262302 VRQ262149:VRQ262302 WBM262149:WBM262302 WLI262149:WLI262302 WVE262149:WVE262302 F327685:F327838 IS327685:IS327838 SO327685:SO327838 ACK327685:ACK327838 AMG327685:AMG327838 AWC327685:AWC327838 BFY327685:BFY327838 BPU327685:BPU327838 BZQ327685:BZQ327838 CJM327685:CJM327838 CTI327685:CTI327838 DDE327685:DDE327838 DNA327685:DNA327838 DWW327685:DWW327838 EGS327685:EGS327838 EQO327685:EQO327838 FAK327685:FAK327838 FKG327685:FKG327838 FUC327685:FUC327838 GDY327685:GDY327838 GNU327685:GNU327838 GXQ327685:GXQ327838 HHM327685:HHM327838 HRI327685:HRI327838 IBE327685:IBE327838 ILA327685:ILA327838 IUW327685:IUW327838 JES327685:JES327838 JOO327685:JOO327838 JYK327685:JYK327838 KIG327685:KIG327838 KSC327685:KSC327838 LBY327685:LBY327838 LLU327685:LLU327838 LVQ327685:LVQ327838 MFM327685:MFM327838 MPI327685:MPI327838 MZE327685:MZE327838 NJA327685:NJA327838 NSW327685:NSW327838 OCS327685:OCS327838 OMO327685:OMO327838 OWK327685:OWK327838 PGG327685:PGG327838 PQC327685:PQC327838 PZY327685:PZY327838 QJU327685:QJU327838 QTQ327685:QTQ327838 RDM327685:RDM327838 RNI327685:RNI327838 RXE327685:RXE327838 SHA327685:SHA327838 SQW327685:SQW327838 TAS327685:TAS327838 TKO327685:TKO327838 TUK327685:TUK327838 UEG327685:UEG327838 UOC327685:UOC327838 UXY327685:UXY327838 VHU327685:VHU327838 VRQ327685:VRQ327838 WBM327685:WBM327838 WLI327685:WLI327838 WVE327685:WVE327838 F393221:F393374 IS393221:IS393374 SO393221:SO393374 ACK393221:ACK393374 AMG393221:AMG393374 AWC393221:AWC393374 BFY393221:BFY393374 BPU393221:BPU393374 BZQ393221:BZQ393374 CJM393221:CJM393374 CTI393221:CTI393374 DDE393221:DDE393374 DNA393221:DNA393374 DWW393221:DWW393374 EGS393221:EGS393374 EQO393221:EQO393374 FAK393221:FAK393374 FKG393221:FKG393374 FUC393221:FUC393374 GDY393221:GDY393374 GNU393221:GNU393374 GXQ393221:GXQ393374 HHM393221:HHM393374 HRI393221:HRI393374 IBE393221:IBE393374 ILA393221:ILA393374 IUW393221:IUW393374 JES393221:JES393374 JOO393221:JOO393374 JYK393221:JYK393374 KIG393221:KIG393374 KSC393221:KSC393374 LBY393221:LBY393374 LLU393221:LLU393374 LVQ393221:LVQ393374 MFM393221:MFM393374 MPI393221:MPI393374 MZE393221:MZE393374 NJA393221:NJA393374 NSW393221:NSW393374 OCS393221:OCS393374 OMO393221:OMO393374 OWK393221:OWK393374 PGG393221:PGG393374 PQC393221:PQC393374 PZY393221:PZY393374 QJU393221:QJU393374 QTQ393221:QTQ393374 RDM393221:RDM393374 RNI393221:RNI393374 RXE393221:RXE393374 SHA393221:SHA393374 SQW393221:SQW393374 TAS393221:TAS393374 TKO393221:TKO393374 TUK393221:TUK393374 UEG393221:UEG393374 UOC393221:UOC393374 UXY393221:UXY393374 VHU393221:VHU393374 VRQ393221:VRQ393374 WBM393221:WBM393374 WLI393221:WLI393374 WVE393221:WVE393374 F458757:F458910 IS458757:IS458910 SO458757:SO458910 ACK458757:ACK458910 AMG458757:AMG458910 AWC458757:AWC458910 BFY458757:BFY458910 BPU458757:BPU458910 BZQ458757:BZQ458910 CJM458757:CJM458910 CTI458757:CTI458910 DDE458757:DDE458910 DNA458757:DNA458910 DWW458757:DWW458910 EGS458757:EGS458910 EQO458757:EQO458910 FAK458757:FAK458910 FKG458757:FKG458910 FUC458757:FUC458910 GDY458757:GDY458910 GNU458757:GNU458910 GXQ458757:GXQ458910 HHM458757:HHM458910 HRI458757:HRI458910 IBE458757:IBE458910 ILA458757:ILA458910 IUW458757:IUW458910 JES458757:JES458910 JOO458757:JOO458910 JYK458757:JYK458910 KIG458757:KIG458910 KSC458757:KSC458910 LBY458757:LBY458910 LLU458757:LLU458910 LVQ458757:LVQ458910 MFM458757:MFM458910 MPI458757:MPI458910 MZE458757:MZE458910 NJA458757:NJA458910 NSW458757:NSW458910 OCS458757:OCS458910 OMO458757:OMO458910 OWK458757:OWK458910 PGG458757:PGG458910 PQC458757:PQC458910 PZY458757:PZY458910 QJU458757:QJU458910 QTQ458757:QTQ458910 RDM458757:RDM458910 RNI458757:RNI458910 RXE458757:RXE458910 SHA458757:SHA458910 SQW458757:SQW458910 TAS458757:TAS458910 TKO458757:TKO458910 TUK458757:TUK458910 UEG458757:UEG458910 UOC458757:UOC458910 UXY458757:UXY458910 VHU458757:VHU458910 VRQ458757:VRQ458910 WBM458757:WBM458910 WLI458757:WLI458910 WVE458757:WVE458910 F524293:F524446 IS524293:IS524446 SO524293:SO524446 ACK524293:ACK524446 AMG524293:AMG524446 AWC524293:AWC524446 BFY524293:BFY524446 BPU524293:BPU524446 BZQ524293:BZQ524446 CJM524293:CJM524446 CTI524293:CTI524446 DDE524293:DDE524446 DNA524293:DNA524446 DWW524293:DWW524446 EGS524293:EGS524446 EQO524293:EQO524446 FAK524293:FAK524446 FKG524293:FKG524446 FUC524293:FUC524446 GDY524293:GDY524446 GNU524293:GNU524446 GXQ524293:GXQ524446 HHM524293:HHM524446 HRI524293:HRI524446 IBE524293:IBE524446 ILA524293:ILA524446 IUW524293:IUW524446 JES524293:JES524446 JOO524293:JOO524446 JYK524293:JYK524446 KIG524293:KIG524446 KSC524293:KSC524446 LBY524293:LBY524446 LLU524293:LLU524446 LVQ524293:LVQ524446 MFM524293:MFM524446 MPI524293:MPI524446 MZE524293:MZE524446 NJA524293:NJA524446 NSW524293:NSW524446 OCS524293:OCS524446 OMO524293:OMO524446 OWK524293:OWK524446 PGG524293:PGG524446 PQC524293:PQC524446 PZY524293:PZY524446 QJU524293:QJU524446 QTQ524293:QTQ524446 RDM524293:RDM524446 RNI524293:RNI524446 RXE524293:RXE524446 SHA524293:SHA524446 SQW524293:SQW524446 TAS524293:TAS524446 TKO524293:TKO524446 TUK524293:TUK524446 UEG524293:UEG524446 UOC524293:UOC524446 UXY524293:UXY524446 VHU524293:VHU524446 VRQ524293:VRQ524446 WBM524293:WBM524446 WLI524293:WLI524446 WVE524293:WVE524446 F589829:F589982 IS589829:IS589982 SO589829:SO589982 ACK589829:ACK589982 AMG589829:AMG589982 AWC589829:AWC589982 BFY589829:BFY589982 BPU589829:BPU589982 BZQ589829:BZQ589982 CJM589829:CJM589982 CTI589829:CTI589982 DDE589829:DDE589982 DNA589829:DNA589982 DWW589829:DWW589982 EGS589829:EGS589982 EQO589829:EQO589982 FAK589829:FAK589982 FKG589829:FKG589982 FUC589829:FUC589982 GDY589829:GDY589982 GNU589829:GNU589982 GXQ589829:GXQ589982 HHM589829:HHM589982 HRI589829:HRI589982 IBE589829:IBE589982 ILA589829:ILA589982 IUW589829:IUW589982 JES589829:JES589982 JOO589829:JOO589982 JYK589829:JYK589982 KIG589829:KIG589982 KSC589829:KSC589982 LBY589829:LBY589982 LLU589829:LLU589982 LVQ589829:LVQ589982 MFM589829:MFM589982 MPI589829:MPI589982 MZE589829:MZE589982 NJA589829:NJA589982 NSW589829:NSW589982 OCS589829:OCS589982 OMO589829:OMO589982 OWK589829:OWK589982 PGG589829:PGG589982 PQC589829:PQC589982 PZY589829:PZY589982 QJU589829:QJU589982 QTQ589829:QTQ589982 RDM589829:RDM589982 RNI589829:RNI589982 RXE589829:RXE589982 SHA589829:SHA589982 SQW589829:SQW589982 TAS589829:TAS589982 TKO589829:TKO589982 TUK589829:TUK589982 UEG589829:UEG589982 UOC589829:UOC589982 UXY589829:UXY589982 VHU589829:VHU589982 VRQ589829:VRQ589982 WBM589829:WBM589982 WLI589829:WLI589982 WVE589829:WVE589982 F655365:F655518 IS655365:IS655518 SO655365:SO655518 ACK655365:ACK655518 AMG655365:AMG655518 AWC655365:AWC655518 BFY655365:BFY655518 BPU655365:BPU655518 BZQ655365:BZQ655518 CJM655365:CJM655518 CTI655365:CTI655518 DDE655365:DDE655518 DNA655365:DNA655518 DWW655365:DWW655518 EGS655365:EGS655518 EQO655365:EQO655518 FAK655365:FAK655518 FKG655365:FKG655518 FUC655365:FUC655518 GDY655365:GDY655518 GNU655365:GNU655518 GXQ655365:GXQ655518 HHM655365:HHM655518 HRI655365:HRI655518 IBE655365:IBE655518 ILA655365:ILA655518 IUW655365:IUW655518 JES655365:JES655518 JOO655365:JOO655518 JYK655365:JYK655518 KIG655365:KIG655518 KSC655365:KSC655518 LBY655365:LBY655518 LLU655365:LLU655518 LVQ655365:LVQ655518 MFM655365:MFM655518 MPI655365:MPI655518 MZE655365:MZE655518 NJA655365:NJA655518 NSW655365:NSW655518 OCS655365:OCS655518 OMO655365:OMO655518 OWK655365:OWK655518 PGG655365:PGG655518 PQC655365:PQC655518 PZY655365:PZY655518 QJU655365:QJU655518 QTQ655365:QTQ655518 RDM655365:RDM655518 RNI655365:RNI655518 RXE655365:RXE655518 SHA655365:SHA655518 SQW655365:SQW655518 TAS655365:TAS655518 TKO655365:TKO655518 TUK655365:TUK655518 UEG655365:UEG655518 UOC655365:UOC655518 UXY655365:UXY655518 VHU655365:VHU655518 VRQ655365:VRQ655518 WBM655365:WBM655518 WLI655365:WLI655518 WVE655365:WVE655518 F720901:F721054 IS720901:IS721054 SO720901:SO721054 ACK720901:ACK721054 AMG720901:AMG721054 AWC720901:AWC721054 BFY720901:BFY721054 BPU720901:BPU721054 BZQ720901:BZQ721054 CJM720901:CJM721054 CTI720901:CTI721054 DDE720901:DDE721054 DNA720901:DNA721054 DWW720901:DWW721054 EGS720901:EGS721054 EQO720901:EQO721054 FAK720901:FAK721054 FKG720901:FKG721054 FUC720901:FUC721054 GDY720901:GDY721054 GNU720901:GNU721054 GXQ720901:GXQ721054 HHM720901:HHM721054 HRI720901:HRI721054 IBE720901:IBE721054 ILA720901:ILA721054 IUW720901:IUW721054 JES720901:JES721054 JOO720901:JOO721054 JYK720901:JYK721054 KIG720901:KIG721054 KSC720901:KSC721054 LBY720901:LBY721054 LLU720901:LLU721054 LVQ720901:LVQ721054 MFM720901:MFM721054 MPI720901:MPI721054 MZE720901:MZE721054 NJA720901:NJA721054 NSW720901:NSW721054 OCS720901:OCS721054 OMO720901:OMO721054 OWK720901:OWK721054 PGG720901:PGG721054 PQC720901:PQC721054 PZY720901:PZY721054 QJU720901:QJU721054 QTQ720901:QTQ721054 RDM720901:RDM721054 RNI720901:RNI721054 RXE720901:RXE721054 SHA720901:SHA721054 SQW720901:SQW721054 TAS720901:TAS721054 TKO720901:TKO721054 TUK720901:TUK721054 UEG720901:UEG721054 UOC720901:UOC721054 UXY720901:UXY721054 VHU720901:VHU721054 VRQ720901:VRQ721054 WBM720901:WBM721054 WLI720901:WLI721054 WVE720901:WVE721054 F786437:F786590 IS786437:IS786590 SO786437:SO786590 ACK786437:ACK786590 AMG786437:AMG786590 AWC786437:AWC786590 BFY786437:BFY786590 BPU786437:BPU786590 BZQ786437:BZQ786590 CJM786437:CJM786590 CTI786437:CTI786590 DDE786437:DDE786590 DNA786437:DNA786590 DWW786437:DWW786590 EGS786437:EGS786590 EQO786437:EQO786590 FAK786437:FAK786590 FKG786437:FKG786590 FUC786437:FUC786590 GDY786437:GDY786590 GNU786437:GNU786590 GXQ786437:GXQ786590 HHM786437:HHM786590 HRI786437:HRI786590 IBE786437:IBE786590 ILA786437:ILA786590 IUW786437:IUW786590 JES786437:JES786590 JOO786437:JOO786590 JYK786437:JYK786590 KIG786437:KIG786590 KSC786437:KSC786590 LBY786437:LBY786590 LLU786437:LLU786590 LVQ786437:LVQ786590 MFM786437:MFM786590 MPI786437:MPI786590 MZE786437:MZE786590 NJA786437:NJA786590 NSW786437:NSW786590 OCS786437:OCS786590 OMO786437:OMO786590 OWK786437:OWK786590 PGG786437:PGG786590 PQC786437:PQC786590 PZY786437:PZY786590 QJU786437:QJU786590 QTQ786437:QTQ786590 RDM786437:RDM786590 RNI786437:RNI786590 RXE786437:RXE786590 SHA786437:SHA786590 SQW786437:SQW786590 TAS786437:TAS786590 TKO786437:TKO786590 TUK786437:TUK786590 UEG786437:UEG786590 UOC786437:UOC786590 UXY786437:UXY786590 VHU786437:VHU786590 VRQ786437:VRQ786590 WBM786437:WBM786590 WLI786437:WLI786590 WVE786437:WVE786590 F851973:F852126 IS851973:IS852126 SO851973:SO852126 ACK851973:ACK852126 AMG851973:AMG852126 AWC851973:AWC852126 BFY851973:BFY852126 BPU851973:BPU852126 BZQ851973:BZQ852126 CJM851973:CJM852126 CTI851973:CTI852126 DDE851973:DDE852126 DNA851973:DNA852126 DWW851973:DWW852126 EGS851973:EGS852126 EQO851973:EQO852126 FAK851973:FAK852126 FKG851973:FKG852126 FUC851973:FUC852126 GDY851973:GDY852126 GNU851973:GNU852126 GXQ851973:GXQ852126 HHM851973:HHM852126 HRI851973:HRI852126 IBE851973:IBE852126 ILA851973:ILA852126 IUW851973:IUW852126 JES851973:JES852126 JOO851973:JOO852126 JYK851973:JYK852126 KIG851973:KIG852126 KSC851973:KSC852126 LBY851973:LBY852126 LLU851973:LLU852126 LVQ851973:LVQ852126 MFM851973:MFM852126 MPI851973:MPI852126 MZE851973:MZE852126 NJA851973:NJA852126 NSW851973:NSW852126 OCS851973:OCS852126 OMO851973:OMO852126 OWK851973:OWK852126 PGG851973:PGG852126 PQC851973:PQC852126 PZY851973:PZY852126 QJU851973:QJU852126 QTQ851973:QTQ852126 RDM851973:RDM852126 RNI851973:RNI852126 RXE851973:RXE852126 SHA851973:SHA852126 SQW851973:SQW852126 TAS851973:TAS852126 TKO851973:TKO852126 TUK851973:TUK852126 UEG851973:UEG852126 UOC851973:UOC852126 UXY851973:UXY852126 VHU851973:VHU852126 VRQ851973:VRQ852126 WBM851973:WBM852126 WLI851973:WLI852126 WVE851973:WVE852126 F917509:F917662 IS917509:IS917662 SO917509:SO917662 ACK917509:ACK917662 AMG917509:AMG917662 AWC917509:AWC917662 BFY917509:BFY917662 BPU917509:BPU917662 BZQ917509:BZQ917662 CJM917509:CJM917662 CTI917509:CTI917662 DDE917509:DDE917662 DNA917509:DNA917662 DWW917509:DWW917662 EGS917509:EGS917662 EQO917509:EQO917662 FAK917509:FAK917662 FKG917509:FKG917662 FUC917509:FUC917662 GDY917509:GDY917662 GNU917509:GNU917662 GXQ917509:GXQ917662 HHM917509:HHM917662 HRI917509:HRI917662 IBE917509:IBE917662 ILA917509:ILA917662 IUW917509:IUW917662 JES917509:JES917662 JOO917509:JOO917662 JYK917509:JYK917662 KIG917509:KIG917662 KSC917509:KSC917662 LBY917509:LBY917662 LLU917509:LLU917662 LVQ917509:LVQ917662 MFM917509:MFM917662 MPI917509:MPI917662 MZE917509:MZE917662 NJA917509:NJA917662 NSW917509:NSW917662 OCS917509:OCS917662 OMO917509:OMO917662 OWK917509:OWK917662 PGG917509:PGG917662 PQC917509:PQC917662 PZY917509:PZY917662 QJU917509:QJU917662 QTQ917509:QTQ917662 RDM917509:RDM917662 RNI917509:RNI917662 RXE917509:RXE917662 SHA917509:SHA917662 SQW917509:SQW917662 TAS917509:TAS917662 TKO917509:TKO917662 TUK917509:TUK917662 UEG917509:UEG917662 UOC917509:UOC917662 UXY917509:UXY917662 VHU917509:VHU917662 VRQ917509:VRQ917662 WBM917509:WBM917662 WLI917509:WLI917662 WVE917509:WVE917662 F983045:F983198 IS983045:IS983198 SO983045:SO983198 ACK983045:ACK983198 AMG983045:AMG983198 AWC983045:AWC983198 BFY983045:BFY983198 BPU983045:BPU983198 BZQ983045:BZQ983198 CJM983045:CJM983198 CTI983045:CTI983198 DDE983045:DDE983198 DNA983045:DNA983198 DWW983045:DWW983198 EGS983045:EGS983198 EQO983045:EQO983198 FAK983045:FAK983198 FKG983045:FKG983198 FUC983045:FUC983198 GDY983045:GDY983198 GNU983045:GNU983198 GXQ983045:GXQ983198 HHM983045:HHM983198 HRI983045:HRI983198 IBE983045:IBE983198 ILA983045:ILA983198 IUW983045:IUW983198 JES983045:JES983198 JOO983045:JOO983198 JYK983045:JYK983198 KIG983045:KIG983198 KSC983045:KSC983198 LBY983045:LBY983198 LLU983045:LLU983198 LVQ983045:LVQ983198 MFM983045:MFM983198 MPI983045:MPI983198 MZE983045:MZE983198 NJA983045:NJA983198 NSW983045:NSW983198 OCS983045:OCS983198 OMO983045:OMO983198 OWK983045:OWK983198 PGG983045:PGG983198 PQC983045:PQC983198 PZY983045:PZY983198 QJU983045:QJU983198 QTQ983045:QTQ983198 RDM983045:RDM983198 RNI983045:RNI983198 RXE983045:RXE983198 SHA983045:SHA983198 SQW983045:SQW983198 TAS983045:TAS983198 TKO983045:TKO983198 TUK983045:TUK983198 UEG983045:UEG983198 UOC983045:UOC983198 UXY983045:UXY983198 VHU983045:VHU983198 VRQ983045:VRQ983198 WBM983045:WBM983198 WLI983045:WLI983198 F37:F158 WVE6:WVE158 WLI6:WLI158 WBM6:WBM158 VRQ6:VRQ158 VHU6:VHU158 UXY6:UXY158 UOC6:UOC158 UEG6:UEG158 TUK6:TUK158 TKO6:TKO158 TAS6:TAS158 SQW6:SQW158 SHA6:SHA158 RXE6:RXE158 RNI6:RNI158 RDM6:RDM158 QTQ6:QTQ158 QJU6:QJU158 PZY6:PZY158 PQC6:PQC158 PGG6:PGG158 OWK6:OWK158 OMO6:OMO158 OCS6:OCS158 NSW6:NSW158 NJA6:NJA158 MZE6:MZE158 MPI6:MPI158 MFM6:MFM158 LVQ6:LVQ158 LLU6:LLU158 LBY6:LBY158 KSC6:KSC158 KIG6:KIG158 JYK6:JYK158 JOO6:JOO158 JES6:JES158 IUW6:IUW158 ILA6:ILA158 IBE6:IBE158 HRI6:HRI158 HHM6:HHM158 GXQ6:GXQ158 GNU6:GNU158 GDY6:GDY158 FUC6:FUC158 FKG6:FKG158 FAK6:FAK158 EQO6:EQO158 EGS6:EGS158 DWW6:DWW158 DNA6:DNA158 DDE6:DDE158 CTI6:CTI158 CJM6:CJM158 BZQ6:BZQ158 BPU6:BPU158 BFY6:BFY158 AWC6:AWC158 AMG6:AMG158 ACK6:ACK158 SO6:SO158 IS6:IS158" xr:uid="{047E5A7D-3F66-4A74-9334-FE5570FDAD13}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVE983045:WVE983198 F6 F65541:F65694 IS65541:IS65694 SO65541:SO65694 ACK65541:ACK65694 AMG65541:AMG65694 AWC65541:AWC65694 BFY65541:BFY65694 BPU65541:BPU65694 BZQ65541:BZQ65694 CJM65541:CJM65694 CTI65541:CTI65694 DDE65541:DDE65694 DNA65541:DNA65694 DWW65541:DWW65694 EGS65541:EGS65694 EQO65541:EQO65694 FAK65541:FAK65694 FKG65541:FKG65694 FUC65541:FUC65694 GDY65541:GDY65694 GNU65541:GNU65694 GXQ65541:GXQ65694 HHM65541:HHM65694 HRI65541:HRI65694 IBE65541:IBE65694 ILA65541:ILA65694 IUW65541:IUW65694 JES65541:JES65694 JOO65541:JOO65694 JYK65541:JYK65694 KIG65541:KIG65694 KSC65541:KSC65694 LBY65541:LBY65694 LLU65541:LLU65694 LVQ65541:LVQ65694 MFM65541:MFM65694 MPI65541:MPI65694 MZE65541:MZE65694 NJA65541:NJA65694 NSW65541:NSW65694 OCS65541:OCS65694 OMO65541:OMO65694 OWK65541:OWK65694 PGG65541:PGG65694 PQC65541:PQC65694 PZY65541:PZY65694 QJU65541:QJU65694 QTQ65541:QTQ65694 RDM65541:RDM65694 RNI65541:RNI65694 RXE65541:RXE65694 SHA65541:SHA65694 SQW65541:SQW65694 TAS65541:TAS65694 TKO65541:TKO65694 TUK65541:TUK65694 UEG65541:UEG65694 UOC65541:UOC65694 UXY65541:UXY65694 VHU65541:VHU65694 VRQ65541:VRQ65694 WBM65541:WBM65694 WLI65541:WLI65694 WVE65541:WVE65694 F131077:F131230 IS131077:IS131230 SO131077:SO131230 ACK131077:ACK131230 AMG131077:AMG131230 AWC131077:AWC131230 BFY131077:BFY131230 BPU131077:BPU131230 BZQ131077:BZQ131230 CJM131077:CJM131230 CTI131077:CTI131230 DDE131077:DDE131230 DNA131077:DNA131230 DWW131077:DWW131230 EGS131077:EGS131230 EQO131077:EQO131230 FAK131077:FAK131230 FKG131077:FKG131230 FUC131077:FUC131230 GDY131077:GDY131230 GNU131077:GNU131230 GXQ131077:GXQ131230 HHM131077:HHM131230 HRI131077:HRI131230 IBE131077:IBE131230 ILA131077:ILA131230 IUW131077:IUW131230 JES131077:JES131230 JOO131077:JOO131230 JYK131077:JYK131230 KIG131077:KIG131230 KSC131077:KSC131230 LBY131077:LBY131230 LLU131077:LLU131230 LVQ131077:LVQ131230 MFM131077:MFM131230 MPI131077:MPI131230 MZE131077:MZE131230 NJA131077:NJA131230 NSW131077:NSW131230 OCS131077:OCS131230 OMO131077:OMO131230 OWK131077:OWK131230 PGG131077:PGG131230 PQC131077:PQC131230 PZY131077:PZY131230 QJU131077:QJU131230 QTQ131077:QTQ131230 RDM131077:RDM131230 RNI131077:RNI131230 RXE131077:RXE131230 SHA131077:SHA131230 SQW131077:SQW131230 TAS131077:TAS131230 TKO131077:TKO131230 TUK131077:TUK131230 UEG131077:UEG131230 UOC131077:UOC131230 UXY131077:UXY131230 VHU131077:VHU131230 VRQ131077:VRQ131230 WBM131077:WBM131230 WLI131077:WLI131230 WVE131077:WVE131230 F196613:F196766 IS196613:IS196766 SO196613:SO196766 ACK196613:ACK196766 AMG196613:AMG196766 AWC196613:AWC196766 BFY196613:BFY196766 BPU196613:BPU196766 BZQ196613:BZQ196766 CJM196613:CJM196766 CTI196613:CTI196766 DDE196613:DDE196766 DNA196613:DNA196766 DWW196613:DWW196766 EGS196613:EGS196766 EQO196613:EQO196766 FAK196613:FAK196766 FKG196613:FKG196766 FUC196613:FUC196766 GDY196613:GDY196766 GNU196613:GNU196766 GXQ196613:GXQ196766 HHM196613:HHM196766 HRI196613:HRI196766 IBE196613:IBE196766 ILA196613:ILA196766 IUW196613:IUW196766 JES196613:JES196766 JOO196613:JOO196766 JYK196613:JYK196766 KIG196613:KIG196766 KSC196613:KSC196766 LBY196613:LBY196766 LLU196613:LLU196766 LVQ196613:LVQ196766 MFM196613:MFM196766 MPI196613:MPI196766 MZE196613:MZE196766 NJA196613:NJA196766 NSW196613:NSW196766 OCS196613:OCS196766 OMO196613:OMO196766 OWK196613:OWK196766 PGG196613:PGG196766 PQC196613:PQC196766 PZY196613:PZY196766 QJU196613:QJU196766 QTQ196613:QTQ196766 RDM196613:RDM196766 RNI196613:RNI196766 RXE196613:RXE196766 SHA196613:SHA196766 SQW196613:SQW196766 TAS196613:TAS196766 TKO196613:TKO196766 TUK196613:TUK196766 UEG196613:UEG196766 UOC196613:UOC196766 UXY196613:UXY196766 VHU196613:VHU196766 VRQ196613:VRQ196766 WBM196613:WBM196766 WLI196613:WLI196766 WVE196613:WVE196766 F262149:F262302 IS262149:IS262302 SO262149:SO262302 ACK262149:ACK262302 AMG262149:AMG262302 AWC262149:AWC262302 BFY262149:BFY262302 BPU262149:BPU262302 BZQ262149:BZQ262302 CJM262149:CJM262302 CTI262149:CTI262302 DDE262149:DDE262302 DNA262149:DNA262302 DWW262149:DWW262302 EGS262149:EGS262302 EQO262149:EQO262302 FAK262149:FAK262302 FKG262149:FKG262302 FUC262149:FUC262302 GDY262149:GDY262302 GNU262149:GNU262302 GXQ262149:GXQ262302 HHM262149:HHM262302 HRI262149:HRI262302 IBE262149:IBE262302 ILA262149:ILA262302 IUW262149:IUW262302 JES262149:JES262302 JOO262149:JOO262302 JYK262149:JYK262302 KIG262149:KIG262302 KSC262149:KSC262302 LBY262149:LBY262302 LLU262149:LLU262302 LVQ262149:LVQ262302 MFM262149:MFM262302 MPI262149:MPI262302 MZE262149:MZE262302 NJA262149:NJA262302 NSW262149:NSW262302 OCS262149:OCS262302 OMO262149:OMO262302 OWK262149:OWK262302 PGG262149:PGG262302 PQC262149:PQC262302 PZY262149:PZY262302 QJU262149:QJU262302 QTQ262149:QTQ262302 RDM262149:RDM262302 RNI262149:RNI262302 RXE262149:RXE262302 SHA262149:SHA262302 SQW262149:SQW262302 TAS262149:TAS262302 TKO262149:TKO262302 TUK262149:TUK262302 UEG262149:UEG262302 UOC262149:UOC262302 UXY262149:UXY262302 VHU262149:VHU262302 VRQ262149:VRQ262302 WBM262149:WBM262302 WLI262149:WLI262302 WVE262149:WVE262302 F327685:F327838 IS327685:IS327838 SO327685:SO327838 ACK327685:ACK327838 AMG327685:AMG327838 AWC327685:AWC327838 BFY327685:BFY327838 BPU327685:BPU327838 BZQ327685:BZQ327838 CJM327685:CJM327838 CTI327685:CTI327838 DDE327685:DDE327838 DNA327685:DNA327838 DWW327685:DWW327838 EGS327685:EGS327838 EQO327685:EQO327838 FAK327685:FAK327838 FKG327685:FKG327838 FUC327685:FUC327838 GDY327685:GDY327838 GNU327685:GNU327838 GXQ327685:GXQ327838 HHM327685:HHM327838 HRI327685:HRI327838 IBE327685:IBE327838 ILA327685:ILA327838 IUW327685:IUW327838 JES327685:JES327838 JOO327685:JOO327838 JYK327685:JYK327838 KIG327685:KIG327838 KSC327685:KSC327838 LBY327685:LBY327838 LLU327685:LLU327838 LVQ327685:LVQ327838 MFM327685:MFM327838 MPI327685:MPI327838 MZE327685:MZE327838 NJA327685:NJA327838 NSW327685:NSW327838 OCS327685:OCS327838 OMO327685:OMO327838 OWK327685:OWK327838 PGG327685:PGG327838 PQC327685:PQC327838 PZY327685:PZY327838 QJU327685:QJU327838 QTQ327685:QTQ327838 RDM327685:RDM327838 RNI327685:RNI327838 RXE327685:RXE327838 SHA327685:SHA327838 SQW327685:SQW327838 TAS327685:TAS327838 TKO327685:TKO327838 TUK327685:TUK327838 UEG327685:UEG327838 UOC327685:UOC327838 UXY327685:UXY327838 VHU327685:VHU327838 VRQ327685:VRQ327838 WBM327685:WBM327838 WLI327685:WLI327838 WVE327685:WVE327838 F393221:F393374 IS393221:IS393374 SO393221:SO393374 ACK393221:ACK393374 AMG393221:AMG393374 AWC393221:AWC393374 BFY393221:BFY393374 BPU393221:BPU393374 BZQ393221:BZQ393374 CJM393221:CJM393374 CTI393221:CTI393374 DDE393221:DDE393374 DNA393221:DNA393374 DWW393221:DWW393374 EGS393221:EGS393374 EQO393221:EQO393374 FAK393221:FAK393374 FKG393221:FKG393374 FUC393221:FUC393374 GDY393221:GDY393374 GNU393221:GNU393374 GXQ393221:GXQ393374 HHM393221:HHM393374 HRI393221:HRI393374 IBE393221:IBE393374 ILA393221:ILA393374 IUW393221:IUW393374 JES393221:JES393374 JOO393221:JOO393374 JYK393221:JYK393374 KIG393221:KIG393374 KSC393221:KSC393374 LBY393221:LBY393374 LLU393221:LLU393374 LVQ393221:LVQ393374 MFM393221:MFM393374 MPI393221:MPI393374 MZE393221:MZE393374 NJA393221:NJA393374 NSW393221:NSW393374 OCS393221:OCS393374 OMO393221:OMO393374 OWK393221:OWK393374 PGG393221:PGG393374 PQC393221:PQC393374 PZY393221:PZY393374 QJU393221:QJU393374 QTQ393221:QTQ393374 RDM393221:RDM393374 RNI393221:RNI393374 RXE393221:RXE393374 SHA393221:SHA393374 SQW393221:SQW393374 TAS393221:TAS393374 TKO393221:TKO393374 TUK393221:TUK393374 UEG393221:UEG393374 UOC393221:UOC393374 UXY393221:UXY393374 VHU393221:VHU393374 VRQ393221:VRQ393374 WBM393221:WBM393374 WLI393221:WLI393374 WVE393221:WVE393374 F458757:F458910 IS458757:IS458910 SO458757:SO458910 ACK458757:ACK458910 AMG458757:AMG458910 AWC458757:AWC458910 BFY458757:BFY458910 BPU458757:BPU458910 BZQ458757:BZQ458910 CJM458757:CJM458910 CTI458757:CTI458910 DDE458757:DDE458910 DNA458757:DNA458910 DWW458757:DWW458910 EGS458757:EGS458910 EQO458757:EQO458910 FAK458757:FAK458910 FKG458757:FKG458910 FUC458757:FUC458910 GDY458757:GDY458910 GNU458757:GNU458910 GXQ458757:GXQ458910 HHM458757:HHM458910 HRI458757:HRI458910 IBE458757:IBE458910 ILA458757:ILA458910 IUW458757:IUW458910 JES458757:JES458910 JOO458757:JOO458910 JYK458757:JYK458910 KIG458757:KIG458910 KSC458757:KSC458910 LBY458757:LBY458910 LLU458757:LLU458910 LVQ458757:LVQ458910 MFM458757:MFM458910 MPI458757:MPI458910 MZE458757:MZE458910 NJA458757:NJA458910 NSW458757:NSW458910 OCS458757:OCS458910 OMO458757:OMO458910 OWK458757:OWK458910 PGG458757:PGG458910 PQC458757:PQC458910 PZY458757:PZY458910 QJU458757:QJU458910 QTQ458757:QTQ458910 RDM458757:RDM458910 RNI458757:RNI458910 RXE458757:RXE458910 SHA458757:SHA458910 SQW458757:SQW458910 TAS458757:TAS458910 TKO458757:TKO458910 TUK458757:TUK458910 UEG458757:UEG458910 UOC458757:UOC458910 UXY458757:UXY458910 VHU458757:VHU458910 VRQ458757:VRQ458910 WBM458757:WBM458910 WLI458757:WLI458910 WVE458757:WVE458910 F524293:F524446 IS524293:IS524446 SO524293:SO524446 ACK524293:ACK524446 AMG524293:AMG524446 AWC524293:AWC524446 BFY524293:BFY524446 BPU524293:BPU524446 BZQ524293:BZQ524446 CJM524293:CJM524446 CTI524293:CTI524446 DDE524293:DDE524446 DNA524293:DNA524446 DWW524293:DWW524446 EGS524293:EGS524446 EQO524293:EQO524446 FAK524293:FAK524446 FKG524293:FKG524446 FUC524293:FUC524446 GDY524293:GDY524446 GNU524293:GNU524446 GXQ524293:GXQ524446 HHM524293:HHM524446 HRI524293:HRI524446 IBE524293:IBE524446 ILA524293:ILA524446 IUW524293:IUW524446 JES524293:JES524446 JOO524293:JOO524446 JYK524293:JYK524446 KIG524293:KIG524446 KSC524293:KSC524446 LBY524293:LBY524446 LLU524293:LLU524446 LVQ524293:LVQ524446 MFM524293:MFM524446 MPI524293:MPI524446 MZE524293:MZE524446 NJA524293:NJA524446 NSW524293:NSW524446 OCS524293:OCS524446 OMO524293:OMO524446 OWK524293:OWK524446 PGG524293:PGG524446 PQC524293:PQC524446 PZY524293:PZY524446 QJU524293:QJU524446 QTQ524293:QTQ524446 RDM524293:RDM524446 RNI524293:RNI524446 RXE524293:RXE524446 SHA524293:SHA524446 SQW524293:SQW524446 TAS524293:TAS524446 TKO524293:TKO524446 TUK524293:TUK524446 UEG524293:UEG524446 UOC524293:UOC524446 UXY524293:UXY524446 VHU524293:VHU524446 VRQ524293:VRQ524446 WBM524293:WBM524446 WLI524293:WLI524446 WVE524293:WVE524446 F589829:F589982 IS589829:IS589982 SO589829:SO589982 ACK589829:ACK589982 AMG589829:AMG589982 AWC589829:AWC589982 BFY589829:BFY589982 BPU589829:BPU589982 BZQ589829:BZQ589982 CJM589829:CJM589982 CTI589829:CTI589982 DDE589829:DDE589982 DNA589829:DNA589982 DWW589829:DWW589982 EGS589829:EGS589982 EQO589829:EQO589982 FAK589829:FAK589982 FKG589829:FKG589982 FUC589829:FUC589982 GDY589829:GDY589982 GNU589829:GNU589982 GXQ589829:GXQ589982 HHM589829:HHM589982 HRI589829:HRI589982 IBE589829:IBE589982 ILA589829:ILA589982 IUW589829:IUW589982 JES589829:JES589982 JOO589829:JOO589982 JYK589829:JYK589982 KIG589829:KIG589982 KSC589829:KSC589982 LBY589829:LBY589982 LLU589829:LLU589982 LVQ589829:LVQ589982 MFM589829:MFM589982 MPI589829:MPI589982 MZE589829:MZE589982 NJA589829:NJA589982 NSW589829:NSW589982 OCS589829:OCS589982 OMO589829:OMO589982 OWK589829:OWK589982 PGG589829:PGG589982 PQC589829:PQC589982 PZY589829:PZY589982 QJU589829:QJU589982 QTQ589829:QTQ589982 RDM589829:RDM589982 RNI589829:RNI589982 RXE589829:RXE589982 SHA589829:SHA589982 SQW589829:SQW589982 TAS589829:TAS589982 TKO589829:TKO589982 TUK589829:TUK589982 UEG589829:UEG589982 UOC589829:UOC589982 UXY589829:UXY589982 VHU589829:VHU589982 VRQ589829:VRQ589982 WBM589829:WBM589982 WLI589829:WLI589982 WVE589829:WVE589982 F655365:F655518 IS655365:IS655518 SO655365:SO655518 ACK655365:ACK655518 AMG655365:AMG655518 AWC655365:AWC655518 BFY655365:BFY655518 BPU655365:BPU655518 BZQ655365:BZQ655518 CJM655365:CJM655518 CTI655365:CTI655518 DDE655365:DDE655518 DNA655365:DNA655518 DWW655365:DWW655518 EGS655365:EGS655518 EQO655365:EQO655518 FAK655365:FAK655518 FKG655365:FKG655518 FUC655365:FUC655518 GDY655365:GDY655518 GNU655365:GNU655518 GXQ655365:GXQ655518 HHM655365:HHM655518 HRI655365:HRI655518 IBE655365:IBE655518 ILA655365:ILA655518 IUW655365:IUW655518 JES655365:JES655518 JOO655365:JOO655518 JYK655365:JYK655518 KIG655365:KIG655518 KSC655365:KSC655518 LBY655365:LBY655518 LLU655365:LLU655518 LVQ655365:LVQ655518 MFM655365:MFM655518 MPI655365:MPI655518 MZE655365:MZE655518 NJA655365:NJA655518 NSW655365:NSW655518 OCS655365:OCS655518 OMO655365:OMO655518 OWK655365:OWK655518 PGG655365:PGG655518 PQC655365:PQC655518 PZY655365:PZY655518 QJU655365:QJU655518 QTQ655365:QTQ655518 RDM655365:RDM655518 RNI655365:RNI655518 RXE655365:RXE655518 SHA655365:SHA655518 SQW655365:SQW655518 TAS655365:TAS655518 TKO655365:TKO655518 TUK655365:TUK655518 UEG655365:UEG655518 UOC655365:UOC655518 UXY655365:UXY655518 VHU655365:VHU655518 VRQ655365:VRQ655518 WBM655365:WBM655518 WLI655365:WLI655518 WVE655365:WVE655518 F720901:F721054 IS720901:IS721054 SO720901:SO721054 ACK720901:ACK721054 AMG720901:AMG721054 AWC720901:AWC721054 BFY720901:BFY721054 BPU720901:BPU721054 BZQ720901:BZQ721054 CJM720901:CJM721054 CTI720901:CTI721054 DDE720901:DDE721054 DNA720901:DNA721054 DWW720901:DWW721054 EGS720901:EGS721054 EQO720901:EQO721054 FAK720901:FAK721054 FKG720901:FKG721054 FUC720901:FUC721054 GDY720901:GDY721054 GNU720901:GNU721054 GXQ720901:GXQ721054 HHM720901:HHM721054 HRI720901:HRI721054 IBE720901:IBE721054 ILA720901:ILA721054 IUW720901:IUW721054 JES720901:JES721054 JOO720901:JOO721054 JYK720901:JYK721054 KIG720901:KIG721054 KSC720901:KSC721054 LBY720901:LBY721054 LLU720901:LLU721054 LVQ720901:LVQ721054 MFM720901:MFM721054 MPI720901:MPI721054 MZE720901:MZE721054 NJA720901:NJA721054 NSW720901:NSW721054 OCS720901:OCS721054 OMO720901:OMO721054 OWK720901:OWK721054 PGG720901:PGG721054 PQC720901:PQC721054 PZY720901:PZY721054 QJU720901:QJU721054 QTQ720901:QTQ721054 RDM720901:RDM721054 RNI720901:RNI721054 RXE720901:RXE721054 SHA720901:SHA721054 SQW720901:SQW721054 TAS720901:TAS721054 TKO720901:TKO721054 TUK720901:TUK721054 UEG720901:UEG721054 UOC720901:UOC721054 UXY720901:UXY721054 VHU720901:VHU721054 VRQ720901:VRQ721054 WBM720901:WBM721054 WLI720901:WLI721054 WVE720901:WVE721054 F786437:F786590 IS786437:IS786590 SO786437:SO786590 ACK786437:ACK786590 AMG786437:AMG786590 AWC786437:AWC786590 BFY786437:BFY786590 BPU786437:BPU786590 BZQ786437:BZQ786590 CJM786437:CJM786590 CTI786437:CTI786590 DDE786437:DDE786590 DNA786437:DNA786590 DWW786437:DWW786590 EGS786437:EGS786590 EQO786437:EQO786590 FAK786437:FAK786590 FKG786437:FKG786590 FUC786437:FUC786590 GDY786437:GDY786590 GNU786437:GNU786590 GXQ786437:GXQ786590 HHM786437:HHM786590 HRI786437:HRI786590 IBE786437:IBE786590 ILA786437:ILA786590 IUW786437:IUW786590 JES786437:JES786590 JOO786437:JOO786590 JYK786437:JYK786590 KIG786437:KIG786590 KSC786437:KSC786590 LBY786437:LBY786590 LLU786437:LLU786590 LVQ786437:LVQ786590 MFM786437:MFM786590 MPI786437:MPI786590 MZE786437:MZE786590 NJA786437:NJA786590 NSW786437:NSW786590 OCS786437:OCS786590 OMO786437:OMO786590 OWK786437:OWK786590 PGG786437:PGG786590 PQC786437:PQC786590 PZY786437:PZY786590 QJU786437:QJU786590 QTQ786437:QTQ786590 RDM786437:RDM786590 RNI786437:RNI786590 RXE786437:RXE786590 SHA786437:SHA786590 SQW786437:SQW786590 TAS786437:TAS786590 TKO786437:TKO786590 TUK786437:TUK786590 UEG786437:UEG786590 UOC786437:UOC786590 UXY786437:UXY786590 VHU786437:VHU786590 VRQ786437:VRQ786590 WBM786437:WBM786590 WLI786437:WLI786590 WVE786437:WVE786590 F851973:F852126 IS851973:IS852126 SO851973:SO852126 ACK851973:ACK852126 AMG851973:AMG852126 AWC851973:AWC852126 BFY851973:BFY852126 BPU851973:BPU852126 BZQ851973:BZQ852126 CJM851973:CJM852126 CTI851973:CTI852126 DDE851973:DDE852126 DNA851973:DNA852126 DWW851973:DWW852126 EGS851973:EGS852126 EQO851973:EQO852126 FAK851973:FAK852126 FKG851973:FKG852126 FUC851973:FUC852126 GDY851973:GDY852126 GNU851973:GNU852126 GXQ851973:GXQ852126 HHM851973:HHM852126 HRI851973:HRI852126 IBE851973:IBE852126 ILA851973:ILA852126 IUW851973:IUW852126 JES851973:JES852126 JOO851973:JOO852126 JYK851973:JYK852126 KIG851973:KIG852126 KSC851973:KSC852126 LBY851973:LBY852126 LLU851973:LLU852126 LVQ851973:LVQ852126 MFM851973:MFM852126 MPI851973:MPI852126 MZE851973:MZE852126 NJA851973:NJA852126 NSW851973:NSW852126 OCS851973:OCS852126 OMO851973:OMO852126 OWK851973:OWK852126 PGG851973:PGG852126 PQC851973:PQC852126 PZY851973:PZY852126 QJU851973:QJU852126 QTQ851973:QTQ852126 RDM851973:RDM852126 RNI851973:RNI852126 RXE851973:RXE852126 SHA851973:SHA852126 SQW851973:SQW852126 TAS851973:TAS852126 TKO851973:TKO852126 TUK851973:TUK852126 UEG851973:UEG852126 UOC851973:UOC852126 UXY851973:UXY852126 VHU851973:VHU852126 VRQ851973:VRQ852126 WBM851973:WBM852126 WLI851973:WLI852126 WVE851973:WVE852126 F917509:F917662 IS917509:IS917662 SO917509:SO917662 ACK917509:ACK917662 AMG917509:AMG917662 AWC917509:AWC917662 BFY917509:BFY917662 BPU917509:BPU917662 BZQ917509:BZQ917662 CJM917509:CJM917662 CTI917509:CTI917662 DDE917509:DDE917662 DNA917509:DNA917662 DWW917509:DWW917662 EGS917509:EGS917662 EQO917509:EQO917662 FAK917509:FAK917662 FKG917509:FKG917662 FUC917509:FUC917662 GDY917509:GDY917662 GNU917509:GNU917662 GXQ917509:GXQ917662 HHM917509:HHM917662 HRI917509:HRI917662 IBE917509:IBE917662 ILA917509:ILA917662 IUW917509:IUW917662 JES917509:JES917662 JOO917509:JOO917662 JYK917509:JYK917662 KIG917509:KIG917662 KSC917509:KSC917662 LBY917509:LBY917662 LLU917509:LLU917662 LVQ917509:LVQ917662 MFM917509:MFM917662 MPI917509:MPI917662 MZE917509:MZE917662 NJA917509:NJA917662 NSW917509:NSW917662 OCS917509:OCS917662 OMO917509:OMO917662 OWK917509:OWK917662 PGG917509:PGG917662 PQC917509:PQC917662 PZY917509:PZY917662 QJU917509:QJU917662 QTQ917509:QTQ917662 RDM917509:RDM917662 RNI917509:RNI917662 RXE917509:RXE917662 SHA917509:SHA917662 SQW917509:SQW917662 TAS917509:TAS917662 TKO917509:TKO917662 TUK917509:TUK917662 UEG917509:UEG917662 UOC917509:UOC917662 UXY917509:UXY917662 VHU917509:VHU917662 VRQ917509:VRQ917662 WBM917509:WBM917662 WLI917509:WLI917662 WVE917509:WVE917662 F983045:F983198 IS983045:IS983198 SO983045:SO983198 ACK983045:ACK983198 AMG983045:AMG983198 AWC983045:AWC983198 BFY983045:BFY983198 BPU983045:BPU983198 BZQ983045:BZQ983198 CJM983045:CJM983198 CTI983045:CTI983198 DDE983045:DDE983198 DNA983045:DNA983198 DWW983045:DWW983198 EGS983045:EGS983198 EQO983045:EQO983198 FAK983045:FAK983198 FKG983045:FKG983198 FUC983045:FUC983198 GDY983045:GDY983198 GNU983045:GNU983198 GXQ983045:GXQ983198 HHM983045:HHM983198 HRI983045:HRI983198 IBE983045:IBE983198 ILA983045:ILA983198 IUW983045:IUW983198 JES983045:JES983198 JOO983045:JOO983198 JYK983045:JYK983198 KIG983045:KIG983198 KSC983045:KSC983198 LBY983045:LBY983198 LLU983045:LLU983198 LVQ983045:LVQ983198 MFM983045:MFM983198 MPI983045:MPI983198 MZE983045:MZE983198 NJA983045:NJA983198 NSW983045:NSW983198 OCS983045:OCS983198 OMO983045:OMO983198 OWK983045:OWK983198 PGG983045:PGG983198 PQC983045:PQC983198 PZY983045:PZY983198 QJU983045:QJU983198 QTQ983045:QTQ983198 RDM983045:RDM983198 RNI983045:RNI983198 RXE983045:RXE983198 SHA983045:SHA983198 SQW983045:SQW983198 TAS983045:TAS983198 TKO983045:TKO983198 TUK983045:TUK983198 UEG983045:UEG983198 UOC983045:UOC983198 UXY983045:UXY983198 VHU983045:VHU983198 VRQ983045:VRQ983198 WBM983045:WBM983198 WLI983045:WLI983198 IS6:IS158 WVE6:WVE158 WLI6:WLI158 WBM6:WBM158 VRQ6:VRQ158 VHU6:VHU158 UXY6:UXY158 UOC6:UOC158 UEG6:UEG158 TUK6:TUK158 TKO6:TKO158 TAS6:TAS158 SQW6:SQW158 SHA6:SHA158 RXE6:RXE158 RNI6:RNI158 RDM6:RDM158 QTQ6:QTQ158 QJU6:QJU158 PZY6:PZY158 PQC6:PQC158 PGG6:PGG158 OWK6:OWK158 OMO6:OMO158 OCS6:OCS158 NSW6:NSW158 NJA6:NJA158 MZE6:MZE158 MPI6:MPI158 MFM6:MFM158 LVQ6:LVQ158 LLU6:LLU158 LBY6:LBY158 KSC6:KSC158 KIG6:KIG158 JYK6:JYK158 JOO6:JOO158 JES6:JES158 IUW6:IUW158 ILA6:ILA158 IBE6:IBE158 HRI6:HRI158 HHM6:HHM158 GXQ6:GXQ158 GNU6:GNU158 GDY6:GDY158 FUC6:FUC158 FKG6:FKG158 FAK6:FAK158 EQO6:EQO158 EGS6:EGS158 DWW6:DWW158 DNA6:DNA158 DDE6:DDE158 CTI6:CTI158 CJM6:CJM158 BZQ6:BZQ158 BPU6:BPU158 BFY6:BFY158 AWC6:AWC158 AMG6:AMG158 ACK6:ACK158 SO6:SO158 F37:F158" xr:uid="{047E5A7D-3F66-4A74-9334-FE5570FDAD13}">
       <formula1>$AD$30:$AD$36</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVF983046:WVF983198 G65542:G65694 IT65542:IT65694 SP65542:SP65694 ACL65542:ACL65694 AMH65542:AMH65694 AWD65542:AWD65694 BFZ65542:BFZ65694 BPV65542:BPV65694 BZR65542:BZR65694 CJN65542:CJN65694 CTJ65542:CTJ65694 DDF65542:DDF65694 DNB65542:DNB65694 DWX65542:DWX65694 EGT65542:EGT65694 EQP65542:EQP65694 FAL65542:FAL65694 FKH65542:FKH65694 FUD65542:FUD65694 GDZ65542:GDZ65694 GNV65542:GNV65694 GXR65542:GXR65694 HHN65542:HHN65694 HRJ65542:HRJ65694 IBF65542:IBF65694 ILB65542:ILB65694 IUX65542:IUX65694 JET65542:JET65694 JOP65542:JOP65694 JYL65542:JYL65694 KIH65542:KIH65694 KSD65542:KSD65694 LBZ65542:LBZ65694 LLV65542:LLV65694 LVR65542:LVR65694 MFN65542:MFN65694 MPJ65542:MPJ65694 MZF65542:MZF65694 NJB65542:NJB65694 NSX65542:NSX65694 OCT65542:OCT65694 OMP65542:OMP65694 OWL65542:OWL65694 PGH65542:PGH65694 PQD65542:PQD65694 PZZ65542:PZZ65694 QJV65542:QJV65694 QTR65542:QTR65694 RDN65542:RDN65694 RNJ65542:RNJ65694 RXF65542:RXF65694 SHB65542:SHB65694 SQX65542:SQX65694 TAT65542:TAT65694 TKP65542:TKP65694 TUL65542:TUL65694 UEH65542:UEH65694 UOD65542:UOD65694 UXZ65542:UXZ65694 VHV65542:VHV65694 VRR65542:VRR65694 WBN65542:WBN65694 WLJ65542:WLJ65694 WVF65542:WVF65694 G131078:G131230 IT131078:IT131230 SP131078:SP131230 ACL131078:ACL131230 AMH131078:AMH131230 AWD131078:AWD131230 BFZ131078:BFZ131230 BPV131078:BPV131230 BZR131078:BZR131230 CJN131078:CJN131230 CTJ131078:CTJ131230 DDF131078:DDF131230 DNB131078:DNB131230 DWX131078:DWX131230 EGT131078:EGT131230 EQP131078:EQP131230 FAL131078:FAL131230 FKH131078:FKH131230 FUD131078:FUD131230 GDZ131078:GDZ131230 GNV131078:GNV131230 GXR131078:GXR131230 HHN131078:HHN131230 HRJ131078:HRJ131230 IBF131078:IBF131230 ILB131078:ILB131230 IUX131078:IUX131230 JET131078:JET131230 JOP131078:JOP131230 JYL131078:JYL131230 KIH131078:KIH131230 KSD131078:KSD131230 LBZ131078:LBZ131230 LLV131078:LLV131230 LVR131078:LVR131230 MFN131078:MFN131230 MPJ131078:MPJ131230 MZF131078:MZF131230 NJB131078:NJB131230 NSX131078:NSX131230 OCT131078:OCT131230 OMP131078:OMP131230 OWL131078:OWL131230 PGH131078:PGH131230 PQD131078:PQD131230 PZZ131078:PZZ131230 QJV131078:QJV131230 QTR131078:QTR131230 RDN131078:RDN131230 RNJ131078:RNJ131230 RXF131078:RXF131230 SHB131078:SHB131230 SQX131078:SQX131230 TAT131078:TAT131230 TKP131078:TKP131230 TUL131078:TUL131230 UEH131078:UEH131230 UOD131078:UOD131230 UXZ131078:UXZ131230 VHV131078:VHV131230 VRR131078:VRR131230 WBN131078:WBN131230 WLJ131078:WLJ131230 WVF131078:WVF131230 G196614:G196766 IT196614:IT196766 SP196614:SP196766 ACL196614:ACL196766 AMH196614:AMH196766 AWD196614:AWD196766 BFZ196614:BFZ196766 BPV196614:BPV196766 BZR196614:BZR196766 CJN196614:CJN196766 CTJ196614:CTJ196766 DDF196614:DDF196766 DNB196614:DNB196766 DWX196614:DWX196766 EGT196614:EGT196766 EQP196614:EQP196766 FAL196614:FAL196766 FKH196614:FKH196766 FUD196614:FUD196766 GDZ196614:GDZ196766 GNV196614:GNV196766 GXR196614:GXR196766 HHN196614:HHN196766 HRJ196614:HRJ196766 IBF196614:IBF196766 ILB196614:ILB196766 IUX196614:IUX196766 JET196614:JET196766 JOP196614:JOP196766 JYL196614:JYL196766 KIH196614:KIH196766 KSD196614:KSD196766 LBZ196614:LBZ196766 LLV196614:LLV196766 LVR196614:LVR196766 MFN196614:MFN196766 MPJ196614:MPJ196766 MZF196614:MZF196766 NJB196614:NJB196766 NSX196614:NSX196766 OCT196614:OCT196766 OMP196614:OMP196766 OWL196614:OWL196766 PGH196614:PGH196766 PQD196614:PQD196766 PZZ196614:PZZ196766 QJV196614:QJV196766 QTR196614:QTR196766 RDN196614:RDN196766 RNJ196614:RNJ196766 RXF196614:RXF196766 SHB196614:SHB196766 SQX196614:SQX196766 TAT196614:TAT196766 TKP196614:TKP196766 TUL196614:TUL196766 UEH196614:UEH196766 UOD196614:UOD196766 UXZ196614:UXZ196766 VHV196614:VHV196766 VRR196614:VRR196766 WBN196614:WBN196766 WLJ196614:WLJ196766 WVF196614:WVF196766 G262150:G262302 IT262150:IT262302 SP262150:SP262302 ACL262150:ACL262302 AMH262150:AMH262302 AWD262150:AWD262302 BFZ262150:BFZ262302 BPV262150:BPV262302 BZR262150:BZR262302 CJN262150:CJN262302 CTJ262150:CTJ262302 DDF262150:DDF262302 DNB262150:DNB262302 DWX262150:DWX262302 EGT262150:EGT262302 EQP262150:EQP262302 FAL262150:FAL262302 FKH262150:FKH262302 FUD262150:FUD262302 GDZ262150:GDZ262302 GNV262150:GNV262302 GXR262150:GXR262302 HHN262150:HHN262302 HRJ262150:HRJ262302 IBF262150:IBF262302 ILB262150:ILB262302 IUX262150:IUX262302 JET262150:JET262302 JOP262150:JOP262302 JYL262150:JYL262302 KIH262150:KIH262302 KSD262150:KSD262302 LBZ262150:LBZ262302 LLV262150:LLV262302 LVR262150:LVR262302 MFN262150:MFN262302 MPJ262150:MPJ262302 MZF262150:MZF262302 NJB262150:NJB262302 NSX262150:NSX262302 OCT262150:OCT262302 OMP262150:OMP262302 OWL262150:OWL262302 PGH262150:PGH262302 PQD262150:PQD262302 PZZ262150:PZZ262302 QJV262150:QJV262302 QTR262150:QTR262302 RDN262150:RDN262302 RNJ262150:RNJ262302 RXF262150:RXF262302 SHB262150:SHB262302 SQX262150:SQX262302 TAT262150:TAT262302 TKP262150:TKP262302 TUL262150:TUL262302 UEH262150:UEH262302 UOD262150:UOD262302 UXZ262150:UXZ262302 VHV262150:VHV262302 VRR262150:VRR262302 WBN262150:WBN262302 WLJ262150:WLJ262302 WVF262150:WVF262302 G327686:G327838 IT327686:IT327838 SP327686:SP327838 ACL327686:ACL327838 AMH327686:AMH327838 AWD327686:AWD327838 BFZ327686:BFZ327838 BPV327686:BPV327838 BZR327686:BZR327838 CJN327686:CJN327838 CTJ327686:CTJ327838 DDF327686:DDF327838 DNB327686:DNB327838 DWX327686:DWX327838 EGT327686:EGT327838 EQP327686:EQP327838 FAL327686:FAL327838 FKH327686:FKH327838 FUD327686:FUD327838 GDZ327686:GDZ327838 GNV327686:GNV327838 GXR327686:GXR327838 HHN327686:HHN327838 HRJ327686:HRJ327838 IBF327686:IBF327838 ILB327686:ILB327838 IUX327686:IUX327838 JET327686:JET327838 JOP327686:JOP327838 JYL327686:JYL327838 KIH327686:KIH327838 KSD327686:KSD327838 LBZ327686:LBZ327838 LLV327686:LLV327838 LVR327686:LVR327838 MFN327686:MFN327838 MPJ327686:MPJ327838 MZF327686:MZF327838 NJB327686:NJB327838 NSX327686:NSX327838 OCT327686:OCT327838 OMP327686:OMP327838 OWL327686:OWL327838 PGH327686:PGH327838 PQD327686:PQD327838 PZZ327686:PZZ327838 QJV327686:QJV327838 QTR327686:QTR327838 RDN327686:RDN327838 RNJ327686:RNJ327838 RXF327686:RXF327838 SHB327686:SHB327838 SQX327686:SQX327838 TAT327686:TAT327838 TKP327686:TKP327838 TUL327686:TUL327838 UEH327686:UEH327838 UOD327686:UOD327838 UXZ327686:UXZ327838 VHV327686:VHV327838 VRR327686:VRR327838 WBN327686:WBN327838 WLJ327686:WLJ327838 WVF327686:WVF327838 G393222:G393374 IT393222:IT393374 SP393222:SP393374 ACL393222:ACL393374 AMH393222:AMH393374 AWD393222:AWD393374 BFZ393222:BFZ393374 BPV393222:BPV393374 BZR393222:BZR393374 CJN393222:CJN393374 CTJ393222:CTJ393374 DDF393222:DDF393374 DNB393222:DNB393374 DWX393222:DWX393374 EGT393222:EGT393374 EQP393222:EQP393374 FAL393222:FAL393374 FKH393222:FKH393374 FUD393222:FUD393374 GDZ393222:GDZ393374 GNV393222:GNV393374 GXR393222:GXR393374 HHN393222:HHN393374 HRJ393222:HRJ393374 IBF393222:IBF393374 ILB393222:ILB393374 IUX393222:IUX393374 JET393222:JET393374 JOP393222:JOP393374 JYL393222:JYL393374 KIH393222:KIH393374 KSD393222:KSD393374 LBZ393222:LBZ393374 LLV393222:LLV393374 LVR393222:LVR393374 MFN393222:MFN393374 MPJ393222:MPJ393374 MZF393222:MZF393374 NJB393222:NJB393374 NSX393222:NSX393374 OCT393222:OCT393374 OMP393222:OMP393374 OWL393222:OWL393374 PGH393222:PGH393374 PQD393222:PQD393374 PZZ393222:PZZ393374 QJV393222:QJV393374 QTR393222:QTR393374 RDN393222:RDN393374 RNJ393222:RNJ393374 RXF393222:RXF393374 SHB393222:SHB393374 SQX393222:SQX393374 TAT393222:TAT393374 TKP393222:TKP393374 TUL393222:TUL393374 UEH393222:UEH393374 UOD393222:UOD393374 UXZ393222:UXZ393374 VHV393222:VHV393374 VRR393222:VRR393374 WBN393222:WBN393374 WLJ393222:WLJ393374 WVF393222:WVF393374 G458758:G458910 IT458758:IT458910 SP458758:SP458910 ACL458758:ACL458910 AMH458758:AMH458910 AWD458758:AWD458910 BFZ458758:BFZ458910 BPV458758:BPV458910 BZR458758:BZR458910 CJN458758:CJN458910 CTJ458758:CTJ458910 DDF458758:DDF458910 DNB458758:DNB458910 DWX458758:DWX458910 EGT458758:EGT458910 EQP458758:EQP458910 FAL458758:FAL458910 FKH458758:FKH458910 FUD458758:FUD458910 GDZ458758:GDZ458910 GNV458758:GNV458910 GXR458758:GXR458910 HHN458758:HHN458910 HRJ458758:HRJ458910 IBF458758:IBF458910 ILB458758:ILB458910 IUX458758:IUX458910 JET458758:JET458910 JOP458758:JOP458910 JYL458758:JYL458910 KIH458758:KIH458910 KSD458758:KSD458910 LBZ458758:LBZ458910 LLV458758:LLV458910 LVR458758:LVR458910 MFN458758:MFN458910 MPJ458758:MPJ458910 MZF458758:MZF458910 NJB458758:NJB458910 NSX458758:NSX458910 OCT458758:OCT458910 OMP458758:OMP458910 OWL458758:OWL458910 PGH458758:PGH458910 PQD458758:PQD458910 PZZ458758:PZZ458910 QJV458758:QJV458910 QTR458758:QTR458910 RDN458758:RDN458910 RNJ458758:RNJ458910 RXF458758:RXF458910 SHB458758:SHB458910 SQX458758:SQX458910 TAT458758:TAT458910 TKP458758:TKP458910 TUL458758:TUL458910 UEH458758:UEH458910 UOD458758:UOD458910 UXZ458758:UXZ458910 VHV458758:VHV458910 VRR458758:VRR458910 WBN458758:WBN458910 WLJ458758:WLJ458910 WVF458758:WVF458910 G524294:G524446 IT524294:IT524446 SP524294:SP524446 ACL524294:ACL524446 AMH524294:AMH524446 AWD524294:AWD524446 BFZ524294:BFZ524446 BPV524294:BPV524446 BZR524294:BZR524446 CJN524294:CJN524446 CTJ524294:CTJ524446 DDF524294:DDF524446 DNB524294:DNB524446 DWX524294:DWX524446 EGT524294:EGT524446 EQP524294:EQP524446 FAL524294:FAL524446 FKH524294:FKH524446 FUD524294:FUD524446 GDZ524294:GDZ524446 GNV524294:GNV524446 GXR524294:GXR524446 HHN524294:HHN524446 HRJ524294:HRJ524446 IBF524294:IBF524446 ILB524294:ILB524446 IUX524294:IUX524446 JET524294:JET524446 JOP524294:JOP524446 JYL524294:JYL524446 KIH524294:KIH524446 KSD524294:KSD524446 LBZ524294:LBZ524446 LLV524294:LLV524446 LVR524294:LVR524446 MFN524294:MFN524446 MPJ524294:MPJ524446 MZF524294:MZF524446 NJB524294:NJB524446 NSX524294:NSX524446 OCT524294:OCT524446 OMP524294:OMP524446 OWL524294:OWL524446 PGH524294:PGH524446 PQD524294:PQD524446 PZZ524294:PZZ524446 QJV524294:QJV524446 QTR524294:QTR524446 RDN524294:RDN524446 RNJ524294:RNJ524446 RXF524294:RXF524446 SHB524294:SHB524446 SQX524294:SQX524446 TAT524294:TAT524446 TKP524294:TKP524446 TUL524294:TUL524446 UEH524294:UEH524446 UOD524294:UOD524446 UXZ524294:UXZ524446 VHV524294:VHV524446 VRR524294:VRR524446 WBN524294:WBN524446 WLJ524294:WLJ524446 WVF524294:WVF524446 G589830:G589982 IT589830:IT589982 SP589830:SP589982 ACL589830:ACL589982 AMH589830:AMH589982 AWD589830:AWD589982 BFZ589830:BFZ589982 BPV589830:BPV589982 BZR589830:BZR589982 CJN589830:CJN589982 CTJ589830:CTJ589982 DDF589830:DDF589982 DNB589830:DNB589982 DWX589830:DWX589982 EGT589830:EGT589982 EQP589830:EQP589982 FAL589830:FAL589982 FKH589830:FKH589982 FUD589830:FUD589982 GDZ589830:GDZ589982 GNV589830:GNV589982 GXR589830:GXR589982 HHN589830:HHN589982 HRJ589830:HRJ589982 IBF589830:IBF589982 ILB589830:ILB589982 IUX589830:IUX589982 JET589830:JET589982 JOP589830:JOP589982 JYL589830:JYL589982 KIH589830:KIH589982 KSD589830:KSD589982 LBZ589830:LBZ589982 LLV589830:LLV589982 LVR589830:LVR589982 MFN589830:MFN589982 MPJ589830:MPJ589982 MZF589830:MZF589982 NJB589830:NJB589982 NSX589830:NSX589982 OCT589830:OCT589982 OMP589830:OMP589982 OWL589830:OWL589982 PGH589830:PGH589982 PQD589830:PQD589982 PZZ589830:PZZ589982 QJV589830:QJV589982 QTR589830:QTR589982 RDN589830:RDN589982 RNJ589830:RNJ589982 RXF589830:RXF589982 SHB589830:SHB589982 SQX589830:SQX589982 TAT589830:TAT589982 TKP589830:TKP589982 TUL589830:TUL589982 UEH589830:UEH589982 UOD589830:UOD589982 UXZ589830:UXZ589982 VHV589830:VHV589982 VRR589830:VRR589982 WBN589830:WBN589982 WLJ589830:WLJ589982 WVF589830:WVF589982 G655366:G655518 IT655366:IT655518 SP655366:SP655518 ACL655366:ACL655518 AMH655366:AMH655518 AWD655366:AWD655518 BFZ655366:BFZ655518 BPV655366:BPV655518 BZR655366:BZR655518 CJN655366:CJN655518 CTJ655366:CTJ655518 DDF655366:DDF655518 DNB655366:DNB655518 DWX655366:DWX655518 EGT655366:EGT655518 EQP655366:EQP655518 FAL655366:FAL655518 FKH655366:FKH655518 FUD655366:FUD655518 GDZ655366:GDZ655518 GNV655366:GNV655518 GXR655366:GXR655518 HHN655366:HHN655518 HRJ655366:HRJ655518 IBF655366:IBF655518 ILB655366:ILB655518 IUX655366:IUX655518 JET655366:JET655518 JOP655366:JOP655518 JYL655366:JYL655518 KIH655366:KIH655518 KSD655366:KSD655518 LBZ655366:LBZ655518 LLV655366:LLV655518 LVR655366:LVR655518 MFN655366:MFN655518 MPJ655366:MPJ655518 MZF655366:MZF655518 NJB655366:NJB655518 NSX655366:NSX655518 OCT655366:OCT655518 OMP655366:OMP655518 OWL655366:OWL655518 PGH655366:PGH655518 PQD655366:PQD655518 PZZ655366:PZZ655518 QJV655366:QJV655518 QTR655366:QTR655518 RDN655366:RDN655518 RNJ655366:RNJ655518 RXF655366:RXF655518 SHB655366:SHB655518 SQX655366:SQX655518 TAT655366:TAT655518 TKP655366:TKP655518 TUL655366:TUL655518 UEH655366:UEH655518 UOD655366:UOD655518 UXZ655366:UXZ655518 VHV655366:VHV655518 VRR655366:VRR655518 WBN655366:WBN655518 WLJ655366:WLJ655518 WVF655366:WVF655518 G720902:G721054 IT720902:IT721054 SP720902:SP721054 ACL720902:ACL721054 AMH720902:AMH721054 AWD720902:AWD721054 BFZ720902:BFZ721054 BPV720902:BPV721054 BZR720902:BZR721054 CJN720902:CJN721054 CTJ720902:CTJ721054 DDF720902:DDF721054 DNB720902:DNB721054 DWX720902:DWX721054 EGT720902:EGT721054 EQP720902:EQP721054 FAL720902:FAL721054 FKH720902:FKH721054 FUD720902:FUD721054 GDZ720902:GDZ721054 GNV720902:GNV721054 GXR720902:GXR721054 HHN720902:HHN721054 HRJ720902:HRJ721054 IBF720902:IBF721054 ILB720902:ILB721054 IUX720902:IUX721054 JET720902:JET721054 JOP720902:JOP721054 JYL720902:JYL721054 KIH720902:KIH721054 KSD720902:KSD721054 LBZ720902:LBZ721054 LLV720902:LLV721054 LVR720902:LVR721054 MFN720902:MFN721054 MPJ720902:MPJ721054 MZF720902:MZF721054 NJB720902:NJB721054 NSX720902:NSX721054 OCT720902:OCT721054 OMP720902:OMP721054 OWL720902:OWL721054 PGH720902:PGH721054 PQD720902:PQD721054 PZZ720902:PZZ721054 QJV720902:QJV721054 QTR720902:QTR721054 RDN720902:RDN721054 RNJ720902:RNJ721054 RXF720902:RXF721054 SHB720902:SHB721054 SQX720902:SQX721054 TAT720902:TAT721054 TKP720902:TKP721054 TUL720902:TUL721054 UEH720902:UEH721054 UOD720902:UOD721054 UXZ720902:UXZ721054 VHV720902:VHV721054 VRR720902:VRR721054 WBN720902:WBN721054 WLJ720902:WLJ721054 WVF720902:WVF721054 G786438:G786590 IT786438:IT786590 SP786438:SP786590 ACL786438:ACL786590 AMH786438:AMH786590 AWD786438:AWD786590 BFZ786438:BFZ786590 BPV786438:BPV786590 BZR786438:BZR786590 CJN786438:CJN786590 CTJ786438:CTJ786590 DDF786438:DDF786590 DNB786438:DNB786590 DWX786438:DWX786590 EGT786438:EGT786590 EQP786438:EQP786590 FAL786438:FAL786590 FKH786438:FKH786590 FUD786438:FUD786590 GDZ786438:GDZ786590 GNV786438:GNV786590 GXR786438:GXR786590 HHN786438:HHN786590 HRJ786438:HRJ786590 IBF786438:IBF786590 ILB786438:ILB786590 IUX786438:IUX786590 JET786438:JET786590 JOP786438:JOP786590 JYL786438:JYL786590 KIH786438:KIH786590 KSD786438:KSD786590 LBZ786438:LBZ786590 LLV786438:LLV786590 LVR786438:LVR786590 MFN786438:MFN786590 MPJ786438:MPJ786590 MZF786438:MZF786590 NJB786438:NJB786590 NSX786438:NSX786590 OCT786438:OCT786590 OMP786438:OMP786590 OWL786438:OWL786590 PGH786438:PGH786590 PQD786438:PQD786590 PZZ786438:PZZ786590 QJV786438:QJV786590 QTR786438:QTR786590 RDN786438:RDN786590 RNJ786438:RNJ786590 RXF786438:RXF786590 SHB786438:SHB786590 SQX786438:SQX786590 TAT786438:TAT786590 TKP786438:TKP786590 TUL786438:TUL786590 UEH786438:UEH786590 UOD786438:UOD786590 UXZ786438:UXZ786590 VHV786438:VHV786590 VRR786438:VRR786590 WBN786438:WBN786590 WLJ786438:WLJ786590 WVF786438:WVF786590 G851974:G852126 IT851974:IT852126 SP851974:SP852126 ACL851974:ACL852126 AMH851974:AMH852126 AWD851974:AWD852126 BFZ851974:BFZ852126 BPV851974:BPV852126 BZR851974:BZR852126 CJN851974:CJN852126 CTJ851974:CTJ852126 DDF851974:DDF852126 DNB851974:DNB852126 DWX851974:DWX852126 EGT851974:EGT852126 EQP851974:EQP852126 FAL851974:FAL852126 FKH851974:FKH852126 FUD851974:FUD852126 GDZ851974:GDZ852126 GNV851974:GNV852126 GXR851974:GXR852126 HHN851974:HHN852126 HRJ851974:HRJ852126 IBF851974:IBF852126 ILB851974:ILB852126 IUX851974:IUX852126 JET851974:JET852126 JOP851974:JOP852126 JYL851974:JYL852126 KIH851974:KIH852126 KSD851974:KSD852126 LBZ851974:LBZ852126 LLV851974:LLV852126 LVR851974:LVR852126 MFN851974:MFN852126 MPJ851974:MPJ852126 MZF851974:MZF852126 NJB851974:NJB852126 NSX851974:NSX852126 OCT851974:OCT852126 OMP851974:OMP852126 OWL851974:OWL852126 PGH851974:PGH852126 PQD851974:PQD852126 PZZ851974:PZZ852126 QJV851974:QJV852126 QTR851974:QTR852126 RDN851974:RDN852126 RNJ851974:RNJ852126 RXF851974:RXF852126 SHB851974:SHB852126 SQX851974:SQX852126 TAT851974:TAT852126 TKP851974:TKP852126 TUL851974:TUL852126 UEH851974:UEH852126 UOD851974:UOD852126 UXZ851974:UXZ852126 VHV851974:VHV852126 VRR851974:VRR852126 WBN851974:WBN852126 WLJ851974:WLJ852126 WVF851974:WVF852126 G917510:G917662 IT917510:IT917662 SP917510:SP917662 ACL917510:ACL917662 AMH917510:AMH917662 AWD917510:AWD917662 BFZ917510:BFZ917662 BPV917510:BPV917662 BZR917510:BZR917662 CJN917510:CJN917662 CTJ917510:CTJ917662 DDF917510:DDF917662 DNB917510:DNB917662 DWX917510:DWX917662 EGT917510:EGT917662 EQP917510:EQP917662 FAL917510:FAL917662 FKH917510:FKH917662 FUD917510:FUD917662 GDZ917510:GDZ917662 GNV917510:GNV917662 GXR917510:GXR917662 HHN917510:HHN917662 HRJ917510:HRJ917662 IBF917510:IBF917662 ILB917510:ILB917662 IUX917510:IUX917662 JET917510:JET917662 JOP917510:JOP917662 JYL917510:JYL917662 KIH917510:KIH917662 KSD917510:KSD917662 LBZ917510:LBZ917662 LLV917510:LLV917662 LVR917510:LVR917662 MFN917510:MFN917662 MPJ917510:MPJ917662 MZF917510:MZF917662 NJB917510:NJB917662 NSX917510:NSX917662 OCT917510:OCT917662 OMP917510:OMP917662 OWL917510:OWL917662 PGH917510:PGH917662 PQD917510:PQD917662 PZZ917510:PZZ917662 QJV917510:QJV917662 QTR917510:QTR917662 RDN917510:RDN917662 RNJ917510:RNJ917662 RXF917510:RXF917662 SHB917510:SHB917662 SQX917510:SQX917662 TAT917510:TAT917662 TKP917510:TKP917662 TUL917510:TUL917662 UEH917510:UEH917662 UOD917510:UOD917662 UXZ917510:UXZ917662 VHV917510:VHV917662 VRR917510:VRR917662 WBN917510:WBN917662 WLJ917510:WLJ917662 WVF917510:WVF917662 G983046:G983198 IT983046:IT983198 SP983046:SP983198 ACL983046:ACL983198 AMH983046:AMH983198 AWD983046:AWD983198 BFZ983046:BFZ983198 BPV983046:BPV983198 BZR983046:BZR983198 CJN983046:CJN983198 CTJ983046:CTJ983198 DDF983046:DDF983198 DNB983046:DNB983198 DWX983046:DWX983198 EGT983046:EGT983198 EQP983046:EQP983198 FAL983046:FAL983198 FKH983046:FKH983198 FUD983046:FUD983198 GDZ983046:GDZ983198 GNV983046:GNV983198 GXR983046:GXR983198 HHN983046:HHN983198 HRJ983046:HRJ983198 IBF983046:IBF983198 ILB983046:ILB983198 IUX983046:IUX983198 JET983046:JET983198 JOP983046:JOP983198 JYL983046:JYL983198 KIH983046:KIH983198 KSD983046:KSD983198 LBZ983046:LBZ983198 LLV983046:LLV983198 LVR983046:LVR983198 MFN983046:MFN983198 MPJ983046:MPJ983198 MZF983046:MZF983198 NJB983046:NJB983198 NSX983046:NSX983198 OCT983046:OCT983198 OMP983046:OMP983198 OWL983046:OWL983198 PGH983046:PGH983198 PQD983046:PQD983198 PZZ983046:PZZ983198 QJV983046:QJV983198 QTR983046:QTR983198 RDN983046:RDN983198 RNJ983046:RNJ983198 RXF983046:RXF983198 SHB983046:SHB983198 SQX983046:SQX983198 TAT983046:TAT983198 TKP983046:TKP983198 TUL983046:TUL983198 UEH983046:UEH983198 UOD983046:UOD983198 UXZ983046:UXZ983198 VHV983046:VHV983198 VRR983046:VRR983198 WBN983046:WBN983198 WLJ983046:WLJ983198 G7:G158 WVF7:WVF158 WLJ7:WLJ158 WBN7:WBN158 VRR7:VRR158 VHV7:VHV158 UXZ7:UXZ158 UOD7:UOD158 UEH7:UEH158 TUL7:TUL158 TKP7:TKP158 TAT7:TAT158 SQX7:SQX158 SHB7:SHB158 RXF7:RXF158 RNJ7:RNJ158 RDN7:RDN158 QTR7:QTR158 QJV7:QJV158 PZZ7:PZZ158 PQD7:PQD158 PGH7:PGH158 OWL7:OWL158 OMP7:OMP158 OCT7:OCT158 NSX7:NSX158 NJB7:NJB158 MZF7:MZF158 MPJ7:MPJ158 MFN7:MFN158 LVR7:LVR158 LLV7:LLV158 LBZ7:LBZ158 KSD7:KSD158 KIH7:KIH158 JYL7:JYL158 JOP7:JOP158 JET7:JET158 IUX7:IUX158 ILB7:ILB158 IBF7:IBF158 HRJ7:HRJ158 HHN7:HHN158 GXR7:GXR158 GNV7:GNV158 GDZ7:GDZ158 FUD7:FUD158 FKH7:FKH158 FAL7:FAL158 EQP7:EQP158 EGT7:EGT158 DWX7:DWX158 DNB7:DNB158 DDF7:DDF158 CTJ7:CTJ158 CJN7:CJN158 BZR7:BZR158 BPV7:BPV158 BFZ7:BFZ158 AWD7:AWD158 AMH7:AMH158 ACL7:ACL158 SP7:SP158 IT7:IT158" xr:uid="{EDC6663F-7307-453A-88F3-A3C62A439D69}">

</xml_diff>